<commit_message>
docs(gantt): hapus duplikat web build 4
</commit_message>
<xml_diff>
--- a/docs/Gantt Chart.xlsx
+++ b/docs/Gantt Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Materi Semester 7\PWL\warawiriweb\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{853D4172-6535-4B08-BDA4-68507EA8DA93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD6D988-B0F1-41B4-931F-7C6FE5BDC3F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -443,7 +443,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="187">
   <si>
     <t>WBS</t>
   </si>
@@ -2852,24 +2852,6 @@
     <xf numFmtId="1" fontId="50" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2877,9 +2859,27 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="45" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2931,7 +2931,7 @@
     <cellStyle name="Total" xfId="42" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="43" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="16">
     <dxf>
       <border>
         <left style="thin">
@@ -2943,46 +2943,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <border>
@@ -3876,11 +3836,11 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BN61"/>
+  <dimension ref="A1:BN54"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I24" sqref="I24"/>
+      <pane ySplit="7" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3907,29 +3867,29 @@
       <c r="E1" s="29"/>
       <c r="F1" s="29"/>
       <c r="I1" s="78"/>
-      <c r="K1" s="117" t="s">
+      <c r="K1" s="111" t="s">
         <v>71</v>
       </c>
-      <c r="L1" s="117"/>
-      <c r="M1" s="117"/>
-      <c r="N1" s="117"/>
-      <c r="O1" s="117"/>
-      <c r="P1" s="117"/>
-      <c r="Q1" s="117"/>
-      <c r="R1" s="117"/>
-      <c r="S1" s="117"/>
-      <c r="T1" s="117"/>
-      <c r="U1" s="117"/>
-      <c r="V1" s="117"/>
-      <c r="W1" s="117"/>
-      <c r="X1" s="117"/>
-      <c r="Y1" s="117"/>
-      <c r="Z1" s="117"/>
-      <c r="AA1" s="117"/>
-      <c r="AB1" s="117"/>
-      <c r="AC1" s="117"/>
-      <c r="AD1" s="117"/>
-      <c r="AE1" s="117"/>
+      <c r="L1" s="111"/>
+      <c r="M1" s="111"/>
+      <c r="N1" s="111"/>
+      <c r="O1" s="111"/>
+      <c r="P1" s="111"/>
+      <c r="Q1" s="111"/>
+      <c r="R1" s="111"/>
+      <c r="S1" s="111"/>
+      <c r="T1" s="111"/>
+      <c r="U1" s="111"/>
+      <c r="V1" s="111"/>
+      <c r="W1" s="111"/>
+      <c r="X1" s="111"/>
+      <c r="Y1" s="111"/>
+      <c r="Z1" s="111"/>
+      <c r="AA1" s="111"/>
+      <c r="AB1" s="111"/>
+      <c r="AC1" s="111"/>
+      <c r="AD1" s="111"/>
+      <c r="AE1" s="111"/>
     </row>
     <row r="2" spans="1:66" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
@@ -3969,11 +3929,11 @@
       <c r="B4" s="65" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="119">
+      <c r="C4" s="116">
         <v>45194</v>
       </c>
-      <c r="D4" s="119"/>
-      <c r="E4" s="119"/>
+      <c r="D4" s="116"/>
+      <c r="E4" s="116"/>
       <c r="F4" s="64"/>
       <c r="G4" s="65" t="s">
         <v>68</v>
@@ -3983,182 +3943,182 @@
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="30"/>
-      <c r="K4" s="111" t="str">
+      <c r="K4" s="113" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 3</v>
       </c>
-      <c r="L4" s="112"/>
-      <c r="M4" s="112"/>
-      <c r="N4" s="112"/>
-      <c r="O4" s="112"/>
-      <c r="P4" s="112"/>
-      <c r="Q4" s="113"/>
-      <c r="R4" s="111" t="str">
+      <c r="L4" s="114"/>
+      <c r="M4" s="114"/>
+      <c r="N4" s="114"/>
+      <c r="O4" s="114"/>
+      <c r="P4" s="114"/>
+      <c r="Q4" s="115"/>
+      <c r="R4" s="113" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="S4" s="112"/>
-      <c r="T4" s="112"/>
-      <c r="U4" s="112"/>
-      <c r="V4" s="112"/>
-      <c r="W4" s="112"/>
-      <c r="X4" s="113"/>
-      <c r="Y4" s="111" t="str">
+      <c r="S4" s="114"/>
+      <c r="T4" s="114"/>
+      <c r="U4" s="114"/>
+      <c r="V4" s="114"/>
+      <c r="W4" s="114"/>
+      <c r="X4" s="115"/>
+      <c r="Y4" s="113" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="Z4" s="112"/>
-      <c r="AA4" s="112"/>
-      <c r="AB4" s="112"/>
-      <c r="AC4" s="112"/>
-      <c r="AD4" s="112"/>
-      <c r="AE4" s="113"/>
-      <c r="AF4" s="111" t="str">
+      <c r="Z4" s="114"/>
+      <c r="AA4" s="114"/>
+      <c r="AB4" s="114"/>
+      <c r="AC4" s="114"/>
+      <c r="AD4" s="114"/>
+      <c r="AE4" s="115"/>
+      <c r="AF4" s="113" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="AG4" s="112"/>
-      <c r="AH4" s="112"/>
-      <c r="AI4" s="112"/>
-      <c r="AJ4" s="112"/>
-      <c r="AK4" s="112"/>
-      <c r="AL4" s="113"/>
-      <c r="AM4" s="111" t="str">
+      <c r="AG4" s="114"/>
+      <c r="AH4" s="114"/>
+      <c r="AI4" s="114"/>
+      <c r="AJ4" s="114"/>
+      <c r="AK4" s="114"/>
+      <c r="AL4" s="115"/>
+      <c r="AM4" s="113" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="AN4" s="112"/>
-      <c r="AO4" s="112"/>
-      <c r="AP4" s="112"/>
-      <c r="AQ4" s="112"/>
-      <c r="AR4" s="112"/>
-      <c r="AS4" s="113"/>
-      <c r="AT4" s="111" t="str">
+      <c r="AN4" s="114"/>
+      <c r="AO4" s="114"/>
+      <c r="AP4" s="114"/>
+      <c r="AQ4" s="114"/>
+      <c r="AR4" s="114"/>
+      <c r="AS4" s="115"/>
+      <c r="AT4" s="113" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="AU4" s="112"/>
-      <c r="AV4" s="112"/>
-      <c r="AW4" s="112"/>
-      <c r="AX4" s="112"/>
-      <c r="AY4" s="112"/>
-      <c r="AZ4" s="113"/>
-      <c r="BA4" s="111" t="str">
+      <c r="AU4" s="114"/>
+      <c r="AV4" s="114"/>
+      <c r="AW4" s="114"/>
+      <c r="AX4" s="114"/>
+      <c r="AY4" s="114"/>
+      <c r="AZ4" s="115"/>
+      <c r="BA4" s="113" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 9</v>
       </c>
-      <c r="BB4" s="112"/>
-      <c r="BC4" s="112"/>
-      <c r="BD4" s="112"/>
-      <c r="BE4" s="112"/>
-      <c r="BF4" s="112"/>
-      <c r="BG4" s="113"/>
-      <c r="BH4" s="111" t="str">
+      <c r="BB4" s="114"/>
+      <c r="BC4" s="114"/>
+      <c r="BD4" s="114"/>
+      <c r="BE4" s="114"/>
+      <c r="BF4" s="114"/>
+      <c r="BG4" s="115"/>
+      <c r="BH4" s="113" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 10</v>
       </c>
-      <c r="BI4" s="112"/>
-      <c r="BJ4" s="112"/>
-      <c r="BK4" s="112"/>
-      <c r="BL4" s="112"/>
-      <c r="BM4" s="112"/>
-      <c r="BN4" s="113"/>
+      <c r="BI4" s="114"/>
+      <c r="BJ4" s="114"/>
+      <c r="BK4" s="114"/>
+      <c r="BL4" s="114"/>
+      <c r="BM4" s="114"/>
+      <c r="BN4" s="115"/>
     </row>
     <row r="5" spans="1:66" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="64"/>
       <c r="B5" s="65" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="118" t="s">
+      <c r="C5" s="112" t="s">
         <v>132</v>
       </c>
-      <c r="D5" s="118"/>
-      <c r="E5" s="118"/>
+      <c r="D5" s="112"/>
+      <c r="E5" s="112"/>
       <c r="F5" s="64"/>
       <c r="G5" s="64"/>
       <c r="H5" s="64"/>
       <c r="I5" s="64"/>
       <c r="J5" s="30"/>
-      <c r="K5" s="114">
+      <c r="K5" s="117">
         <f>K6</f>
         <v>45208</v>
       </c>
-      <c r="L5" s="115"/>
-      <c r="M5" s="115"/>
-      <c r="N5" s="115"/>
-      <c r="O5" s="115"/>
-      <c r="P5" s="115"/>
-      <c r="Q5" s="116"/>
-      <c r="R5" s="114">
+      <c r="L5" s="118"/>
+      <c r="M5" s="118"/>
+      <c r="N5" s="118"/>
+      <c r="O5" s="118"/>
+      <c r="P5" s="118"/>
+      <c r="Q5" s="119"/>
+      <c r="R5" s="117">
         <f>R6</f>
         <v>45215</v>
       </c>
-      <c r="S5" s="115"/>
-      <c r="T5" s="115"/>
-      <c r="U5" s="115"/>
-      <c r="V5" s="115"/>
-      <c r="W5" s="115"/>
-      <c r="X5" s="116"/>
-      <c r="Y5" s="114">
+      <c r="S5" s="118"/>
+      <c r="T5" s="118"/>
+      <c r="U5" s="118"/>
+      <c r="V5" s="118"/>
+      <c r="W5" s="118"/>
+      <c r="X5" s="119"/>
+      <c r="Y5" s="117">
         <f>Y6</f>
         <v>45222</v>
       </c>
-      <c r="Z5" s="115"/>
-      <c r="AA5" s="115"/>
-      <c r="AB5" s="115"/>
-      <c r="AC5" s="115"/>
-      <c r="AD5" s="115"/>
-      <c r="AE5" s="116"/>
-      <c r="AF5" s="114">
+      <c r="Z5" s="118"/>
+      <c r="AA5" s="118"/>
+      <c r="AB5" s="118"/>
+      <c r="AC5" s="118"/>
+      <c r="AD5" s="118"/>
+      <c r="AE5" s="119"/>
+      <c r="AF5" s="117">
         <f>AF6</f>
         <v>45229</v>
       </c>
-      <c r="AG5" s="115"/>
-      <c r="AH5" s="115"/>
-      <c r="AI5" s="115"/>
-      <c r="AJ5" s="115"/>
-      <c r="AK5" s="115"/>
-      <c r="AL5" s="116"/>
-      <c r="AM5" s="114">
+      <c r="AG5" s="118"/>
+      <c r="AH5" s="118"/>
+      <c r="AI5" s="118"/>
+      <c r="AJ5" s="118"/>
+      <c r="AK5" s="118"/>
+      <c r="AL5" s="119"/>
+      <c r="AM5" s="117">
         <f>AM6</f>
         <v>45236</v>
       </c>
-      <c r="AN5" s="115"/>
-      <c r="AO5" s="115"/>
-      <c r="AP5" s="115"/>
-      <c r="AQ5" s="115"/>
-      <c r="AR5" s="115"/>
-      <c r="AS5" s="116"/>
-      <c r="AT5" s="114">
+      <c r="AN5" s="118"/>
+      <c r="AO5" s="118"/>
+      <c r="AP5" s="118"/>
+      <c r="AQ5" s="118"/>
+      <c r="AR5" s="118"/>
+      <c r="AS5" s="119"/>
+      <c r="AT5" s="117">
         <f>AT6</f>
         <v>45243</v>
       </c>
-      <c r="AU5" s="115"/>
-      <c r="AV5" s="115"/>
-      <c r="AW5" s="115"/>
-      <c r="AX5" s="115"/>
-      <c r="AY5" s="115"/>
-      <c r="AZ5" s="116"/>
-      <c r="BA5" s="114">
+      <c r="AU5" s="118"/>
+      <c r="AV5" s="118"/>
+      <c r="AW5" s="118"/>
+      <c r="AX5" s="118"/>
+      <c r="AY5" s="118"/>
+      <c r="AZ5" s="119"/>
+      <c r="BA5" s="117">
         <f>BA6</f>
         <v>45250</v>
       </c>
-      <c r="BB5" s="115"/>
-      <c r="BC5" s="115"/>
-      <c r="BD5" s="115"/>
-      <c r="BE5" s="115"/>
-      <c r="BF5" s="115"/>
-      <c r="BG5" s="116"/>
-      <c r="BH5" s="114">
+      <c r="BB5" s="118"/>
+      <c r="BC5" s="118"/>
+      <c r="BD5" s="118"/>
+      <c r="BE5" s="118"/>
+      <c r="BF5" s="118"/>
+      <c r="BG5" s="119"/>
+      <c r="BH5" s="117">
         <f>BH6</f>
         <v>45257</v>
       </c>
-      <c r="BI5" s="115"/>
-      <c r="BJ5" s="115"/>
-      <c r="BK5" s="115"/>
-      <c r="BL5" s="115"/>
-      <c r="BM5" s="115"/>
-      <c r="BN5" s="116"/>
+      <c r="BI5" s="118"/>
+      <c r="BJ5" s="118"/>
+      <c r="BK5" s="118"/>
+      <c r="BL5" s="118"/>
+      <c r="BM5" s="118"/>
+      <c r="BN5" s="119"/>
     </row>
     <row r="6" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A6" s="30"/>
@@ -7799,7 +7759,7 @@
         <v>45233</v>
       </c>
       <c r="F44" s="59">
-        <f t="shared" ref="F44:F50" si="20">IF(ISBLANK(E44)," - ",IF(G44=0,E44,E44+G44-1))</f>
+        <f t="shared" ref="F44" si="20">IF(ISBLANK(E44)," - ",IF(G44=0,E44,E44+G44-1))</f>
         <v>45233</v>
       </c>
       <c r="G44" s="41">
@@ -7809,7 +7769,7 @@
         <v>0</v>
       </c>
       <c r="I44" s="43">
-        <f t="shared" ref="I44:I50" si="21">IF(OR(F44=0,E44=0)," - ",NETWORKDAYS(E44,F44))</f>
+        <f t="shared" ref="I44" si="21">IF(OR(F44=0,E44=0)," - ",NETWORKDAYS(E44,F44))</f>
         <v>1</v>
       </c>
       <c r="J44" s="56"/>
@@ -7876,15 +7836,15 @@
         <v>7</v>
       </c>
       <c r="B45" s="33" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D45" s="35"/>
       <c r="E45" s="60">
-        <f>F44+3</f>
+        <f>F38+3</f>
         <v>45236</v>
       </c>
       <c r="F45" s="60">
-        <f t="shared" si="20"/>
+        <f t="shared" ref="F45" si="22">IF(ISBLANK(E45)," - ",IF(G45=0,E45,E45+G45-1))</f>
         <v>45240</v>
       </c>
       <c r="G45" s="36">
@@ -7892,7 +7852,7 @@
       </c>
       <c r="H45" s="37"/>
       <c r="I45" s="38">
-        <f t="shared" si="21"/>
+        <f t="shared" ref="I45" si="23">IF(OR(F45=0,E45=0)," - ",NETWORKDAYS(E45,F45))</f>
         <v>5</v>
       </c>
       <c r="J45" s="57"/>
@@ -7955,11 +7915,11 @@
     </row>
     <row r="46" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" s="39" t="str">
-        <f t="shared" ref="A46:A51" si="22">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>7.1</v>
       </c>
       <c r="B46" s="75" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C46" s="40" t="s">
         <v>144</v>
@@ -7971,17 +7931,17 @@
       </c>
       <c r="F46" s="59">
         <f>IF(ISBLANK(E46)," - ",IF(G46=0,E46,E46+G46-1))</f>
-        <v>45236</v>
+        <v>45238</v>
       </c>
       <c r="G46" s="41">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H46" s="42">
         <v>0</v>
       </c>
       <c r="I46" s="43">
         <f>IF(OR(F46=0,E46=0)," - ",NETWORKDAYS(E46,F46))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J46" s="56"/>
       <c r="K46" s="39"/>
@@ -8043,33 +8003,33 @@
     </row>
     <row r="47" spans="1:66" s="40" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A47" s="39" t="str">
-        <f t="shared" si="22"/>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>7.2</v>
       </c>
       <c r="B47" s="75" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="C47" s="40" t="s">
-        <v>150</v>
+        <v>179</v>
       </c>
       <c r="D47" s="76"/>
       <c r="E47" s="58">
-        <f>E45</f>
-        <v>45236</v>
+        <f>E46+1</f>
+        <v>45237</v>
       </c>
       <c r="F47" s="59">
-        <f t="shared" si="20"/>
-        <v>45237</v>
+        <f t="shared" ref="F47" si="24">IF(ISBLANK(E47)," - ",IF(G47=0,E47,E47+G47-1))</f>
+        <v>45240</v>
       </c>
       <c r="G47" s="41">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H47" s="42">
         <v>0</v>
       </c>
       <c r="I47" s="43">
-        <f t="shared" si="21"/>
-        <v>2</v>
+        <f t="shared" ref="I47" si="25">IF(OR(F47=0,E47=0)," - ",NETWORKDAYS(E47,F47))</f>
+        <v>4</v>
       </c>
       <c r="J47" s="56"/>
       <c r="K47" s="39"/>
@@ -8131,11 +8091,11 @@
     </row>
     <row r="48" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A48" s="39" t="str">
-        <f t="shared" si="22"/>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>7.3</v>
       </c>
       <c r="B48" s="75" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="C48" s="40" t="s">
         <v>155</v>
@@ -8219,23 +8179,23 @@
     </row>
     <row r="49" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A49" s="39" t="str">
-        <f t="shared" si="22"/>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>7.4</v>
       </c>
       <c r="B49" s="75" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="C49" s="40" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="D49" s="76"/>
       <c r="E49" s="58">
-        <f>F46+1</f>
-        <v>45237</v>
+        <f>F48+1</f>
+        <v>45239</v>
       </c>
       <c r="F49" s="59">
         <f>IF(ISBLANK(E49)," - ",IF(G49=0,E49,E49+G49-1))</f>
-        <v>45238</v>
+        <v>45240</v>
       </c>
       <c r="G49" s="41">
         <v>2</v>
@@ -8305,123 +8265,118 @@
       <c r="BM49" s="39"/>
       <c r="BN49" s="39"/>
     </row>
-    <row r="50" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A50" s="39" t="str">
-        <f t="shared" si="22"/>
-        <v>7.5</v>
-      </c>
-      <c r="B50" s="75" t="s">
-        <v>171</v>
-      </c>
-      <c r="C50" s="40" t="s">
-        <v>134</v>
-      </c>
-      <c r="D50" s="76"/>
-      <c r="E50" s="58">
-        <f>F47+1</f>
-        <v>45238</v>
-      </c>
-      <c r="F50" s="59">
-        <f t="shared" si="20"/>
-        <v>45240</v>
-      </c>
-      <c r="G50" s="41">
-        <v>3</v>
-      </c>
-      <c r="H50" s="42">
-        <v>0</v>
-      </c>
-      <c r="I50" s="43">
-        <f t="shared" si="21"/>
-        <v>3</v>
-      </c>
-      <c r="J50" s="56"/>
-      <c r="K50" s="39"/>
-      <c r="L50" s="39"/>
-      <c r="M50" s="39"/>
-      <c r="N50" s="39"/>
-      <c r="O50" s="39"/>
-      <c r="P50" s="39"/>
-      <c r="Q50" s="39"/>
-      <c r="R50" s="39"/>
-      <c r="S50" s="39"/>
-      <c r="T50" s="39"/>
-      <c r="U50" s="39"/>
-      <c r="V50" s="39"/>
-      <c r="W50" s="39"/>
-      <c r="X50" s="39"/>
-      <c r="Y50" s="39"/>
-      <c r="Z50" s="39"/>
-      <c r="AA50" s="39"/>
-      <c r="AB50" s="39"/>
-      <c r="AC50" s="39"/>
-      <c r="AD50" s="39"/>
-      <c r="AE50" s="39"/>
-      <c r="AF50" s="39"/>
-      <c r="AG50" s="39"/>
-      <c r="AH50" s="39"/>
-      <c r="AI50" s="39"/>
-      <c r="AJ50" s="39"/>
-      <c r="AK50" s="39"/>
-      <c r="AL50" s="39"/>
-      <c r="AM50" s="39"/>
-      <c r="AN50" s="39"/>
-      <c r="AO50" s="39"/>
-      <c r="AP50" s="39"/>
-      <c r="AQ50" s="39"/>
-      <c r="AR50" s="39"/>
-      <c r="AS50" s="39"/>
-      <c r="AT50" s="39"/>
-      <c r="AU50" s="39"/>
-      <c r="AV50" s="39"/>
-      <c r="AW50" s="39"/>
-      <c r="AX50" s="39"/>
-      <c r="AY50" s="39"/>
-      <c r="AZ50" s="39"/>
-      <c r="BA50" s="39"/>
-      <c r="BB50" s="39"/>
-      <c r="BC50" s="39"/>
-      <c r="BD50" s="39"/>
-      <c r="BE50" s="39"/>
-      <c r="BF50" s="39"/>
-      <c r="BG50" s="39"/>
-      <c r="BH50" s="39"/>
-      <c r="BI50" s="39"/>
-      <c r="BJ50" s="39"/>
-      <c r="BK50" s="39"/>
-      <c r="BL50" s="39"/>
-      <c r="BM50" s="39"/>
-      <c r="BN50" s="39"/>
-    </row>
-    <row r="51" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:66" s="34" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A50" s="32" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>8</v>
+      </c>
+      <c r="B50" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="D50" s="35"/>
+      <c r="E50" s="60">
+        <f>F49+3</f>
+        <v>45243</v>
+      </c>
+      <c r="F50" s="60">
+        <f t="shared" ref="F50" si="26">IF(ISBLANK(E50)," - ",IF(G50=0,E50,E50+G50-1))</f>
+        <v>45247</v>
+      </c>
+      <c r="G50" s="36">
+        <v>5</v>
+      </c>
+      <c r="H50" s="37"/>
+      <c r="I50" s="38">
+        <f t="shared" ref="I50" si="27">IF(OR(F50=0,E50=0)," - ",NETWORKDAYS(E50,F50))</f>
+        <v>5</v>
+      </c>
+      <c r="J50" s="57"/>
+      <c r="K50" s="63"/>
+      <c r="L50" s="63"/>
+      <c r="M50" s="63"/>
+      <c r="N50" s="63"/>
+      <c r="O50" s="63"/>
+      <c r="P50" s="63"/>
+      <c r="Q50" s="63"/>
+      <c r="R50" s="63"/>
+      <c r="S50" s="63"/>
+      <c r="T50" s="63"/>
+      <c r="U50" s="63"/>
+      <c r="V50" s="63"/>
+      <c r="W50" s="63"/>
+      <c r="X50" s="63"/>
+      <c r="Y50" s="63"/>
+      <c r="Z50" s="63"/>
+      <c r="AA50" s="63"/>
+      <c r="AB50" s="63"/>
+      <c r="AC50" s="63"/>
+      <c r="AD50" s="63"/>
+      <c r="AE50" s="63"/>
+      <c r="AF50" s="63"/>
+      <c r="AG50" s="63"/>
+      <c r="AH50" s="63"/>
+      <c r="AI50" s="63"/>
+      <c r="AJ50" s="63"/>
+      <c r="AK50" s="63"/>
+      <c r="AL50" s="63"/>
+      <c r="AM50" s="63"/>
+      <c r="AN50" s="63"/>
+      <c r="AO50" s="63"/>
+      <c r="AP50" s="63"/>
+      <c r="AQ50" s="63"/>
+      <c r="AR50" s="63"/>
+      <c r="AS50" s="63"/>
+      <c r="AT50" s="63"/>
+      <c r="AU50" s="63"/>
+      <c r="AV50" s="63"/>
+      <c r="AW50" s="63"/>
+      <c r="AX50" s="63"/>
+      <c r="AY50" s="63"/>
+      <c r="AZ50" s="63"/>
+      <c r="BA50" s="63"/>
+      <c r="BB50" s="63"/>
+      <c r="BC50" s="63"/>
+      <c r="BD50" s="63"/>
+      <c r="BE50" s="63"/>
+      <c r="BF50" s="63"/>
+      <c r="BG50" s="63"/>
+      <c r="BH50" s="63"/>
+      <c r="BI50" s="63"/>
+      <c r="BJ50" s="63"/>
+      <c r="BK50" s="63"/>
+      <c r="BL50" s="63"/>
+      <c r="BM50" s="63"/>
+      <c r="BN50" s="63"/>
+    </row>
+    <row r="51" spans="1:66" s="40" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A51" s="39" t="str">
-        <f t="shared" si="22"/>
-        <v>7.6</v>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>8.1</v>
       </c>
       <c r="B51" s="75" t="s">
-        <v>163</v>
+        <v>182</v>
       </c>
       <c r="C51" s="40" t="s">
-        <v>134</v>
+        <v>155</v>
       </c>
       <c r="D51" s="76"/>
       <c r="E51" s="58">
-        <f>F45</f>
-        <v>45240</v>
+        <f>E50</f>
+        <v>45243</v>
       </c>
       <c r="F51" s="59">
-        <f t="shared" ref="F51:F52" si="23">IF(ISBLANK(E51)," - ",IF(G51=0,E51,E51+G51-1))</f>
-        <v>45240</v>
+        <f>IF(ISBLANK(E51)," - ",IF(G51=0,E51,E51+G51-1))</f>
+        <v>45245</v>
       </c>
       <c r="G51" s="41">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H51" s="42">
         <v>0</v>
       </c>
       <c r="I51" s="43">
-        <f t="shared" ref="I51:I52" si="24">IF(OR(F51=0,E51=0)," - ",NETWORKDAYS(E51,F51))</f>
-        <v>1</v>
+        <f>IF(OR(F51=0,E51=0)," - ",NETWORKDAYS(E51,F51))</f>
+        <v>3</v>
       </c>
       <c r="J51" s="56"/>
       <c r="K51" s="39"/>
@@ -8481,118 +8436,123 @@
       <c r="BM51" s="39"/>
       <c r="BN51" s="39"/>
     </row>
-    <row r="52" spans="1:66" s="34" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A52" s="32" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>8</v>
-      </c>
-      <c r="B52" s="33" t="s">
-        <v>176</v>
-      </c>
-      <c r="D52" s="35"/>
-      <c r="E52" s="60">
-        <f>F51+3</f>
+    <row r="52" spans="1:66" s="40" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A52" s="39" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>8.2</v>
+      </c>
+      <c r="B52" s="75" t="s">
+        <v>183</v>
+      </c>
+      <c r="C52" s="40" t="s">
+        <v>134</v>
+      </c>
+      <c r="D52" s="76"/>
+      <c r="E52" s="58">
+        <f>E50</f>
         <v>45243</v>
       </c>
-      <c r="F52" s="60">
-        <f t="shared" si="23"/>
-        <v>45247</v>
-      </c>
-      <c r="G52" s="36">
-        <v>5</v>
-      </c>
-      <c r="H52" s="37"/>
-      <c r="I52" s="38">
-        <f t="shared" si="24"/>
-        <v>5</v>
-      </c>
-      <c r="J52" s="57"/>
-      <c r="K52" s="63"/>
-      <c r="L52" s="63"/>
-      <c r="M52" s="63"/>
-      <c r="N52" s="63"/>
-      <c r="O52" s="63"/>
-      <c r="P52" s="63"/>
-      <c r="Q52" s="63"/>
-      <c r="R52" s="63"/>
-      <c r="S52" s="63"/>
-      <c r="T52" s="63"/>
-      <c r="U52" s="63"/>
-      <c r="V52" s="63"/>
-      <c r="W52" s="63"/>
-      <c r="X52" s="63"/>
-      <c r="Y52" s="63"/>
-      <c r="Z52" s="63"/>
-      <c r="AA52" s="63"/>
-      <c r="AB52" s="63"/>
-      <c r="AC52" s="63"/>
-      <c r="AD52" s="63"/>
-      <c r="AE52" s="63"/>
-      <c r="AF52" s="63"/>
-      <c r="AG52" s="63"/>
-      <c r="AH52" s="63"/>
-      <c r="AI52" s="63"/>
-      <c r="AJ52" s="63"/>
-      <c r="AK52" s="63"/>
-      <c r="AL52" s="63"/>
-      <c r="AM52" s="63"/>
-      <c r="AN52" s="63"/>
-      <c r="AO52" s="63"/>
-      <c r="AP52" s="63"/>
-      <c r="AQ52" s="63"/>
-      <c r="AR52" s="63"/>
-      <c r="AS52" s="63"/>
-      <c r="AT52" s="63"/>
-      <c r="AU52" s="63"/>
-      <c r="AV52" s="63"/>
-      <c r="AW52" s="63"/>
-      <c r="AX52" s="63"/>
-      <c r="AY52" s="63"/>
-      <c r="AZ52" s="63"/>
-      <c r="BA52" s="63"/>
-      <c r="BB52" s="63"/>
-      <c r="BC52" s="63"/>
-      <c r="BD52" s="63"/>
-      <c r="BE52" s="63"/>
-      <c r="BF52" s="63"/>
-      <c r="BG52" s="63"/>
-      <c r="BH52" s="63"/>
-      <c r="BI52" s="63"/>
-      <c r="BJ52" s="63"/>
-      <c r="BK52" s="63"/>
-      <c r="BL52" s="63"/>
-      <c r="BM52" s="63"/>
-      <c r="BN52" s="63"/>
+      <c r="F52" s="59">
+        <f t="shared" ref="F52" si="28">IF(ISBLANK(E52)," - ",IF(G52=0,E52,E52+G52-1))</f>
+        <v>45245</v>
+      </c>
+      <c r="G52" s="41">
+        <v>3</v>
+      </c>
+      <c r="H52" s="42">
+        <v>0</v>
+      </c>
+      <c r="I52" s="43">
+        <f t="shared" ref="I52" si="29">IF(OR(F52=0,E52=0)," - ",NETWORKDAYS(E52,F52))</f>
+        <v>3</v>
+      </c>
+      <c r="J52" s="56"/>
+      <c r="K52" s="39"/>
+      <c r="L52" s="39"/>
+      <c r="M52" s="39"/>
+      <c r="N52" s="39"/>
+      <c r="O52" s="39"/>
+      <c r="P52" s="39"/>
+      <c r="Q52" s="39"/>
+      <c r="R52" s="39"/>
+      <c r="S52" s="39"/>
+      <c r="T52" s="39"/>
+      <c r="U52" s="39"/>
+      <c r="V52" s="39"/>
+      <c r="W52" s="39"/>
+      <c r="X52" s="39"/>
+      <c r="Y52" s="39"/>
+      <c r="Z52" s="39"/>
+      <c r="AA52" s="39"/>
+      <c r="AB52" s="39"/>
+      <c r="AC52" s="39"/>
+      <c r="AD52" s="39"/>
+      <c r="AE52" s="39"/>
+      <c r="AF52" s="39"/>
+      <c r="AG52" s="39"/>
+      <c r="AH52" s="39"/>
+      <c r="AI52" s="39"/>
+      <c r="AJ52" s="39"/>
+      <c r="AK52" s="39"/>
+      <c r="AL52" s="39"/>
+      <c r="AM52" s="39"/>
+      <c r="AN52" s="39"/>
+      <c r="AO52" s="39"/>
+      <c r="AP52" s="39"/>
+      <c r="AQ52" s="39"/>
+      <c r="AR52" s="39"/>
+      <c r="AS52" s="39"/>
+      <c r="AT52" s="39"/>
+      <c r="AU52" s="39"/>
+      <c r="AV52" s="39"/>
+      <c r="AW52" s="39"/>
+      <c r="AX52" s="39"/>
+      <c r="AY52" s="39"/>
+      <c r="AZ52" s="39"/>
+      <c r="BA52" s="39"/>
+      <c r="BB52" s="39"/>
+      <c r="BC52" s="39"/>
+      <c r="BD52" s="39"/>
+      <c r="BE52" s="39"/>
+      <c r="BF52" s="39"/>
+      <c r="BG52" s="39"/>
+      <c r="BH52" s="39"/>
+      <c r="BI52" s="39"/>
+      <c r="BJ52" s="39"/>
+      <c r="BK52" s="39"/>
+      <c r="BL52" s="39"/>
+      <c r="BM52" s="39"/>
+      <c r="BN52" s="39"/>
     </row>
     <row r="53" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A53" s="39" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>8.1</v>
+        <v>8.3</v>
       </c>
       <c r="B53" s="75" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="C53" s="40" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="D53" s="76"/>
       <c r="E53" s="58">
-        <f>E52</f>
-        <v>45243</v>
+        <f>F52+1</f>
+        <v>45246</v>
       </c>
       <c r="F53" s="59">
         <f>IF(ISBLANK(E53)," - ",IF(G53=0,E53,E53+G53-1))</f>
-        <v>45245</v>
+        <v>45246</v>
       </c>
       <c r="G53" s="41">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H53" s="42">
         <v>0</v>
       </c>
       <c r="I53" s="43">
         <f>IF(OR(F53=0,E53=0)," - ",NETWORKDAYS(E53,F53))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J53" s="56"/>
       <c r="K53" s="39"/>
@@ -8652,35 +8612,35 @@
       <c r="BM53" s="39"/>
       <c r="BN53" s="39"/>
     </row>
-    <row r="54" spans="1:66" s="40" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A54" s="39" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>8.2</v>
+        <v>8.4</v>
       </c>
       <c r="B54" s="75" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="C54" s="40" t="s">
-        <v>179</v>
+        <v>134</v>
       </c>
       <c r="D54" s="76"/>
       <c r="E54" s="58">
-        <f>E53+1</f>
-        <v>45244</v>
+        <f>F53+1</f>
+        <v>45247</v>
       </c>
       <c r="F54" s="59">
-        <f t="shared" ref="F54" si="25">IF(ISBLANK(E54)," - ",IF(G54=0,E54,E54+G54-1))</f>
+        <f>IF(ISBLANK(E54)," - ",IF(G54=0,E54,E54+G54-1))</f>
         <v>45247</v>
       </c>
       <c r="G54" s="41">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H54" s="42">
         <v>0</v>
       </c>
       <c r="I54" s="43">
-        <f t="shared" ref="I54" si="26">IF(OR(F54=0,E54=0)," - ",NETWORKDAYS(E54,F54))</f>
-        <v>4</v>
+        <f>IF(OR(F54=0,E54=0)," - ",NETWORKDAYS(E54,F54))</f>
+        <v>1</v>
       </c>
       <c r="J54" s="56"/>
       <c r="K54" s="39"/>
@@ -8740,629 +8700,9 @@
       <c r="BM54" s="39"/>
       <c r="BN54" s="39"/>
     </row>
-    <row r="55" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A55" s="39" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>8.3</v>
-      </c>
-      <c r="B55" s="75" t="s">
-        <v>180</v>
-      </c>
-      <c r="C55" s="40" t="s">
-        <v>155</v>
-      </c>
-      <c r="D55" s="76"/>
-      <c r="E55" s="58">
-        <f>E52</f>
-        <v>45243</v>
-      </c>
-      <c r="F55" s="59">
-        <f>IF(ISBLANK(E55)," - ",IF(G55=0,E55,E55+G55-1))</f>
-        <v>45245</v>
-      </c>
-      <c r="G55" s="41">
-        <v>3</v>
-      </c>
-      <c r="H55" s="42">
-        <v>0</v>
-      </c>
-      <c r="I55" s="43">
-        <f>IF(OR(F55=0,E55=0)," - ",NETWORKDAYS(E55,F55))</f>
-        <v>3</v>
-      </c>
-      <c r="J55" s="56"/>
-      <c r="K55" s="39"/>
-      <c r="L55" s="39"/>
-      <c r="M55" s="39"/>
-      <c r="N55" s="39"/>
-      <c r="O55" s="39"/>
-      <c r="P55" s="39"/>
-      <c r="Q55" s="39"/>
-      <c r="R55" s="39"/>
-      <c r="S55" s="39"/>
-      <c r="T55" s="39"/>
-      <c r="U55" s="39"/>
-      <c r="V55" s="39"/>
-      <c r="W55" s="39"/>
-      <c r="X55" s="39"/>
-      <c r="Y55" s="39"/>
-      <c r="Z55" s="39"/>
-      <c r="AA55" s="39"/>
-      <c r="AB55" s="39"/>
-      <c r="AC55" s="39"/>
-      <c r="AD55" s="39"/>
-      <c r="AE55" s="39"/>
-      <c r="AF55" s="39"/>
-      <c r="AG55" s="39"/>
-      <c r="AH55" s="39"/>
-      <c r="AI55" s="39"/>
-      <c r="AJ55" s="39"/>
-      <c r="AK55" s="39"/>
-      <c r="AL55" s="39"/>
-      <c r="AM55" s="39"/>
-      <c r="AN55" s="39"/>
-      <c r="AO55" s="39"/>
-      <c r="AP55" s="39"/>
-      <c r="AQ55" s="39"/>
-      <c r="AR55" s="39"/>
-      <c r="AS55" s="39"/>
-      <c r="AT55" s="39"/>
-      <c r="AU55" s="39"/>
-      <c r="AV55" s="39"/>
-      <c r="AW55" s="39"/>
-      <c r="AX55" s="39"/>
-      <c r="AY55" s="39"/>
-      <c r="AZ55" s="39"/>
-      <c r="BA55" s="39"/>
-      <c r="BB55" s="39"/>
-      <c r="BC55" s="39"/>
-      <c r="BD55" s="39"/>
-      <c r="BE55" s="39"/>
-      <c r="BF55" s="39"/>
-      <c r="BG55" s="39"/>
-      <c r="BH55" s="39"/>
-      <c r="BI55" s="39"/>
-      <c r="BJ55" s="39"/>
-      <c r="BK55" s="39"/>
-      <c r="BL55" s="39"/>
-      <c r="BM55" s="39"/>
-      <c r="BN55" s="39"/>
-    </row>
-    <row r="56" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A56" s="39" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>8.4</v>
-      </c>
-      <c r="B56" s="75" t="s">
-        <v>181</v>
-      </c>
-      <c r="C56" s="40" t="s">
-        <v>155</v>
-      </c>
-      <c r="D56" s="76"/>
-      <c r="E56" s="58">
-        <f>F55+1</f>
-        <v>45246</v>
-      </c>
-      <c r="F56" s="59">
-        <f>IF(ISBLANK(E56)," - ",IF(G56=0,E56,E56+G56-1))</f>
-        <v>45247</v>
-      </c>
-      <c r="G56" s="41">
-        <v>2</v>
-      </c>
-      <c r="H56" s="42">
-        <v>0</v>
-      </c>
-      <c r="I56" s="43">
-        <f>IF(OR(F56=0,E56=0)," - ",NETWORKDAYS(E56,F56))</f>
-        <v>2</v>
-      </c>
-      <c r="J56" s="56"/>
-      <c r="K56" s="39"/>
-      <c r="L56" s="39"/>
-      <c r="M56" s="39"/>
-      <c r="N56" s="39"/>
-      <c r="O56" s="39"/>
-      <c r="P56" s="39"/>
-      <c r="Q56" s="39"/>
-      <c r="R56" s="39"/>
-      <c r="S56" s="39"/>
-      <c r="T56" s="39"/>
-      <c r="U56" s="39"/>
-      <c r="V56" s="39"/>
-      <c r="W56" s="39"/>
-      <c r="X56" s="39"/>
-      <c r="Y56" s="39"/>
-      <c r="Z56" s="39"/>
-      <c r="AA56" s="39"/>
-      <c r="AB56" s="39"/>
-      <c r="AC56" s="39"/>
-      <c r="AD56" s="39"/>
-      <c r="AE56" s="39"/>
-      <c r="AF56" s="39"/>
-      <c r="AG56" s="39"/>
-      <c r="AH56" s="39"/>
-      <c r="AI56" s="39"/>
-      <c r="AJ56" s="39"/>
-      <c r="AK56" s="39"/>
-      <c r="AL56" s="39"/>
-      <c r="AM56" s="39"/>
-      <c r="AN56" s="39"/>
-      <c r="AO56" s="39"/>
-      <c r="AP56" s="39"/>
-      <c r="AQ56" s="39"/>
-      <c r="AR56" s="39"/>
-      <c r="AS56" s="39"/>
-      <c r="AT56" s="39"/>
-      <c r="AU56" s="39"/>
-      <c r="AV56" s="39"/>
-      <c r="AW56" s="39"/>
-      <c r="AX56" s="39"/>
-      <c r="AY56" s="39"/>
-      <c r="AZ56" s="39"/>
-      <c r="BA56" s="39"/>
-      <c r="BB56" s="39"/>
-      <c r="BC56" s="39"/>
-      <c r="BD56" s="39"/>
-      <c r="BE56" s="39"/>
-      <c r="BF56" s="39"/>
-      <c r="BG56" s="39"/>
-      <c r="BH56" s="39"/>
-      <c r="BI56" s="39"/>
-      <c r="BJ56" s="39"/>
-      <c r="BK56" s="39"/>
-      <c r="BL56" s="39"/>
-      <c r="BM56" s="39"/>
-      <c r="BN56" s="39"/>
-    </row>
-    <row r="57" spans="1:66" s="34" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A57" s="32" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>9</v>
-      </c>
-      <c r="B57" s="33" t="s">
-        <v>184</v>
-      </c>
-      <c r="D57" s="35"/>
-      <c r="E57" s="60">
-        <f>F56+3</f>
-        <v>45250</v>
-      </c>
-      <c r="F57" s="60">
-        <f t="shared" ref="F57" si="27">IF(ISBLANK(E57)," - ",IF(G57=0,E57,E57+G57-1))</f>
-        <v>45254</v>
-      </c>
-      <c r="G57" s="36">
-        <v>5</v>
-      </c>
-      <c r="H57" s="37"/>
-      <c r="I57" s="38">
-        <f t="shared" ref="I57" si="28">IF(OR(F57=0,E57=0)," - ",NETWORKDAYS(E57,F57))</f>
-        <v>5</v>
-      </c>
-      <c r="J57" s="57"/>
-      <c r="K57" s="63"/>
-      <c r="L57" s="63"/>
-      <c r="M57" s="63"/>
-      <c r="N57" s="63"/>
-      <c r="O57" s="63"/>
-      <c r="P57" s="63"/>
-      <c r="Q57" s="63"/>
-      <c r="R57" s="63"/>
-      <c r="S57" s="63"/>
-      <c r="T57" s="63"/>
-      <c r="U57" s="63"/>
-      <c r="V57" s="63"/>
-      <c r="W57" s="63"/>
-      <c r="X57" s="63"/>
-      <c r="Y57" s="63"/>
-      <c r="Z57" s="63"/>
-      <c r="AA57" s="63"/>
-      <c r="AB57" s="63"/>
-      <c r="AC57" s="63"/>
-      <c r="AD57" s="63"/>
-      <c r="AE57" s="63"/>
-      <c r="AF57" s="63"/>
-      <c r="AG57" s="63"/>
-      <c r="AH57" s="63"/>
-      <c r="AI57" s="63"/>
-      <c r="AJ57" s="63"/>
-      <c r="AK57" s="63"/>
-      <c r="AL57" s="63"/>
-      <c r="AM57" s="63"/>
-      <c r="AN57" s="63"/>
-      <c r="AO57" s="63"/>
-      <c r="AP57" s="63"/>
-      <c r="AQ57" s="63"/>
-      <c r="AR57" s="63"/>
-      <c r="AS57" s="63"/>
-      <c r="AT57" s="63"/>
-      <c r="AU57" s="63"/>
-      <c r="AV57" s="63"/>
-      <c r="AW57" s="63"/>
-      <c r="AX57" s="63"/>
-      <c r="AY57" s="63"/>
-      <c r="AZ57" s="63"/>
-      <c r="BA57" s="63"/>
-      <c r="BB57" s="63"/>
-      <c r="BC57" s="63"/>
-      <c r="BD57" s="63"/>
-      <c r="BE57" s="63"/>
-      <c r="BF57" s="63"/>
-      <c r="BG57" s="63"/>
-      <c r="BH57" s="63"/>
-      <c r="BI57" s="63"/>
-      <c r="BJ57" s="63"/>
-      <c r="BK57" s="63"/>
-      <c r="BL57" s="63"/>
-      <c r="BM57" s="63"/>
-      <c r="BN57" s="63"/>
-    </row>
-    <row r="58" spans="1:66" s="40" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A58" s="39" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>9.1</v>
-      </c>
-      <c r="B58" s="75" t="s">
-        <v>182</v>
-      </c>
-      <c r="C58" s="40" t="s">
-        <v>155</v>
-      </c>
-      <c r="D58" s="76"/>
-      <c r="E58" s="58">
-        <f>E57</f>
-        <v>45250</v>
-      </c>
-      <c r="F58" s="59">
-        <f>IF(ISBLANK(E58)," - ",IF(G58=0,E58,E58+G58-1))</f>
-        <v>45252</v>
-      </c>
-      <c r="G58" s="41">
-        <v>3</v>
-      </c>
-      <c r="H58" s="42">
-        <v>0</v>
-      </c>
-      <c r="I58" s="43">
-        <f>IF(OR(F58=0,E58=0)," - ",NETWORKDAYS(E58,F58))</f>
-        <v>3</v>
-      </c>
-      <c r="J58" s="56"/>
-      <c r="K58" s="39"/>
-      <c r="L58" s="39"/>
-      <c r="M58" s="39"/>
-      <c r="N58" s="39"/>
-      <c r="O58" s="39"/>
-      <c r="P58" s="39"/>
-      <c r="Q58" s="39"/>
-      <c r="R58" s="39"/>
-      <c r="S58" s="39"/>
-      <c r="T58" s="39"/>
-      <c r="U58" s="39"/>
-      <c r="V58" s="39"/>
-      <c r="W58" s="39"/>
-      <c r="X58" s="39"/>
-      <c r="Y58" s="39"/>
-      <c r="Z58" s="39"/>
-      <c r="AA58" s="39"/>
-      <c r="AB58" s="39"/>
-      <c r="AC58" s="39"/>
-      <c r="AD58" s="39"/>
-      <c r="AE58" s="39"/>
-      <c r="AF58" s="39"/>
-      <c r="AG58" s="39"/>
-      <c r="AH58" s="39"/>
-      <c r="AI58" s="39"/>
-      <c r="AJ58" s="39"/>
-      <c r="AK58" s="39"/>
-      <c r="AL58" s="39"/>
-      <c r="AM58" s="39"/>
-      <c r="AN58" s="39"/>
-      <c r="AO58" s="39"/>
-      <c r="AP58" s="39"/>
-      <c r="AQ58" s="39"/>
-      <c r="AR58" s="39"/>
-      <c r="AS58" s="39"/>
-      <c r="AT58" s="39"/>
-      <c r="AU58" s="39"/>
-      <c r="AV58" s="39"/>
-      <c r="AW58" s="39"/>
-      <c r="AX58" s="39"/>
-      <c r="AY58" s="39"/>
-      <c r="AZ58" s="39"/>
-      <c r="BA58" s="39"/>
-      <c r="BB58" s="39"/>
-      <c r="BC58" s="39"/>
-      <c r="BD58" s="39"/>
-      <c r="BE58" s="39"/>
-      <c r="BF58" s="39"/>
-      <c r="BG58" s="39"/>
-      <c r="BH58" s="39"/>
-      <c r="BI58" s="39"/>
-      <c r="BJ58" s="39"/>
-      <c r="BK58" s="39"/>
-      <c r="BL58" s="39"/>
-      <c r="BM58" s="39"/>
-      <c r="BN58" s="39"/>
-    </row>
-    <row r="59" spans="1:66" s="40" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A59" s="39" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>9.2</v>
-      </c>
-      <c r="B59" s="75" t="s">
-        <v>183</v>
-      </c>
-      <c r="C59" s="40" t="s">
-        <v>134</v>
-      </c>
-      <c r="D59" s="76"/>
-      <c r="E59" s="58">
-        <f>E57</f>
-        <v>45250</v>
-      </c>
-      <c r="F59" s="59">
-        <f t="shared" ref="F59" si="29">IF(ISBLANK(E59)," - ",IF(G59=0,E59,E59+G59-1))</f>
-        <v>45252</v>
-      </c>
-      <c r="G59" s="41">
-        <v>3</v>
-      </c>
-      <c r="H59" s="42">
-        <v>0</v>
-      </c>
-      <c r="I59" s="43">
-        <f t="shared" ref="I59" si="30">IF(OR(F59=0,E59=0)," - ",NETWORKDAYS(E59,F59))</f>
-        <v>3</v>
-      </c>
-      <c r="J59" s="56"/>
-      <c r="K59" s="39"/>
-      <c r="L59" s="39"/>
-      <c r="M59" s="39"/>
-      <c r="N59" s="39"/>
-      <c r="O59" s="39"/>
-      <c r="P59" s="39"/>
-      <c r="Q59" s="39"/>
-      <c r="R59" s="39"/>
-      <c r="S59" s="39"/>
-      <c r="T59" s="39"/>
-      <c r="U59" s="39"/>
-      <c r="V59" s="39"/>
-      <c r="W59" s="39"/>
-      <c r="X59" s="39"/>
-      <c r="Y59" s="39"/>
-      <c r="Z59" s="39"/>
-      <c r="AA59" s="39"/>
-      <c r="AB59" s="39"/>
-      <c r="AC59" s="39"/>
-      <c r="AD59" s="39"/>
-      <c r="AE59" s="39"/>
-      <c r="AF59" s="39"/>
-      <c r="AG59" s="39"/>
-      <c r="AH59" s="39"/>
-      <c r="AI59" s="39"/>
-      <c r="AJ59" s="39"/>
-      <c r="AK59" s="39"/>
-      <c r="AL59" s="39"/>
-      <c r="AM59" s="39"/>
-      <c r="AN59" s="39"/>
-      <c r="AO59" s="39"/>
-      <c r="AP59" s="39"/>
-      <c r="AQ59" s="39"/>
-      <c r="AR59" s="39"/>
-      <c r="AS59" s="39"/>
-      <c r="AT59" s="39"/>
-      <c r="AU59" s="39"/>
-      <c r="AV59" s="39"/>
-      <c r="AW59" s="39"/>
-      <c r="AX59" s="39"/>
-      <c r="AY59" s="39"/>
-      <c r="AZ59" s="39"/>
-      <c r="BA59" s="39"/>
-      <c r="BB59" s="39"/>
-      <c r="BC59" s="39"/>
-      <c r="BD59" s="39"/>
-      <c r="BE59" s="39"/>
-      <c r="BF59" s="39"/>
-      <c r="BG59" s="39"/>
-      <c r="BH59" s="39"/>
-      <c r="BI59" s="39"/>
-      <c r="BJ59" s="39"/>
-      <c r="BK59" s="39"/>
-      <c r="BL59" s="39"/>
-      <c r="BM59" s="39"/>
-      <c r="BN59" s="39"/>
-    </row>
-    <row r="60" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A60" s="39" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>9.3</v>
-      </c>
-      <c r="B60" s="75" t="s">
-        <v>185</v>
-      </c>
-      <c r="C60" s="40" t="s">
-        <v>134</v>
-      </c>
-      <c r="D60" s="76"/>
-      <c r="E60" s="58">
-        <f>F59+1</f>
-        <v>45253</v>
-      </c>
-      <c r="F60" s="59">
-        <f>IF(ISBLANK(E60)," - ",IF(G60=0,E60,E60+G60-1))</f>
-        <v>45253</v>
-      </c>
-      <c r="G60" s="41">
-        <v>1</v>
-      </c>
-      <c r="H60" s="42">
-        <v>0</v>
-      </c>
-      <c r="I60" s="43">
-        <f>IF(OR(F60=0,E60=0)," - ",NETWORKDAYS(E60,F60))</f>
-        <v>1</v>
-      </c>
-      <c r="J60" s="56"/>
-      <c r="K60" s="39"/>
-      <c r="L60" s="39"/>
-      <c r="M60" s="39"/>
-      <c r="N60" s="39"/>
-      <c r="O60" s="39"/>
-      <c r="P60" s="39"/>
-      <c r="Q60" s="39"/>
-      <c r="R60" s="39"/>
-      <c r="S60" s="39"/>
-      <c r="T60" s="39"/>
-      <c r="U60" s="39"/>
-      <c r="V60" s="39"/>
-      <c r="W60" s="39"/>
-      <c r="X60" s="39"/>
-      <c r="Y60" s="39"/>
-      <c r="Z60" s="39"/>
-      <c r="AA60" s="39"/>
-      <c r="AB60" s="39"/>
-      <c r="AC60" s="39"/>
-      <c r="AD60" s="39"/>
-      <c r="AE60" s="39"/>
-      <c r="AF60" s="39"/>
-      <c r="AG60" s="39"/>
-      <c r="AH60" s="39"/>
-      <c r="AI60" s="39"/>
-      <c r="AJ60" s="39"/>
-      <c r="AK60" s="39"/>
-      <c r="AL60" s="39"/>
-      <c r="AM60" s="39"/>
-      <c r="AN60" s="39"/>
-      <c r="AO60" s="39"/>
-      <c r="AP60" s="39"/>
-      <c r="AQ60" s="39"/>
-      <c r="AR60" s="39"/>
-      <c r="AS60" s="39"/>
-      <c r="AT60" s="39"/>
-      <c r="AU60" s="39"/>
-      <c r="AV60" s="39"/>
-      <c r="AW60" s="39"/>
-      <c r="AX60" s="39"/>
-      <c r="AY60" s="39"/>
-      <c r="AZ60" s="39"/>
-      <c r="BA60" s="39"/>
-      <c r="BB60" s="39"/>
-      <c r="BC60" s="39"/>
-      <c r="BD60" s="39"/>
-      <c r="BE60" s="39"/>
-      <c r="BF60" s="39"/>
-      <c r="BG60" s="39"/>
-      <c r="BH60" s="39"/>
-      <c r="BI60" s="39"/>
-      <c r="BJ60" s="39"/>
-      <c r="BK60" s="39"/>
-      <c r="BL60" s="39"/>
-      <c r="BM60" s="39"/>
-      <c r="BN60" s="39"/>
-    </row>
-    <row r="61" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A61" s="39" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>9.4</v>
-      </c>
-      <c r="B61" s="75" t="s">
-        <v>186</v>
-      </c>
-      <c r="C61" s="40" t="s">
-        <v>134</v>
-      </c>
-      <c r="D61" s="76"/>
-      <c r="E61" s="58">
-        <f>F60+1</f>
-        <v>45254</v>
-      </c>
-      <c r="F61" s="59">
-        <f>IF(ISBLANK(E61)," - ",IF(G61=0,E61,E61+G61-1))</f>
-        <v>45254</v>
-      </c>
-      <c r="G61" s="41">
-        <v>1</v>
-      </c>
-      <c r="H61" s="42">
-        <v>0</v>
-      </c>
-      <c r="I61" s="43">
-        <f>IF(OR(F61=0,E61=0)," - ",NETWORKDAYS(E61,F61))</f>
-        <v>1</v>
-      </c>
-      <c r="J61" s="56"/>
-      <c r="K61" s="39"/>
-      <c r="L61" s="39"/>
-      <c r="M61" s="39"/>
-      <c r="N61" s="39"/>
-      <c r="O61" s="39"/>
-      <c r="P61" s="39"/>
-      <c r="Q61" s="39"/>
-      <c r="R61" s="39"/>
-      <c r="S61" s="39"/>
-      <c r="T61" s="39"/>
-      <c r="U61" s="39"/>
-      <c r="V61" s="39"/>
-      <c r="W61" s="39"/>
-      <c r="X61" s="39"/>
-      <c r="Y61" s="39"/>
-      <c r="Z61" s="39"/>
-      <c r="AA61" s="39"/>
-      <c r="AB61" s="39"/>
-      <c r="AC61" s="39"/>
-      <c r="AD61" s="39"/>
-      <c r="AE61" s="39"/>
-      <c r="AF61" s="39"/>
-      <c r="AG61" s="39"/>
-      <c r="AH61" s="39"/>
-      <c r="AI61" s="39"/>
-      <c r="AJ61" s="39"/>
-      <c r="AK61" s="39"/>
-      <c r="AL61" s="39"/>
-      <c r="AM61" s="39"/>
-      <c r="AN61" s="39"/>
-      <c r="AO61" s="39"/>
-      <c r="AP61" s="39"/>
-      <c r="AQ61" s="39"/>
-      <c r="AR61" s="39"/>
-      <c r="AS61" s="39"/>
-      <c r="AT61" s="39"/>
-      <c r="AU61" s="39"/>
-      <c r="AV61" s="39"/>
-      <c r="AW61" s="39"/>
-      <c r="AX61" s="39"/>
-      <c r="AY61" s="39"/>
-      <c r="AZ61" s="39"/>
-      <c r="BA61" s="39"/>
-      <c r="BB61" s="39"/>
-      <c r="BC61" s="39"/>
-      <c r="BD61" s="39"/>
-      <c r="BE61" s="39"/>
-      <c r="BF61" s="39"/>
-      <c r="BG61" s="39"/>
-      <c r="BH61" s="39"/>
-      <c r="BI61" s="39"/>
-      <c r="BJ61" s="39"/>
-      <c r="BK61" s="39"/>
-      <c r="BL61" s="39"/>
-      <c r="BM61" s="39"/>
-      <c r="BN61" s="39"/>
-    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -9373,9 +8713,18 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="H8:H13 H15:H22 H24:H29 H38:H43 H45:H50">
+  <conditionalFormatting sqref="H8:H13 H15:H22 H24:H29 H38:H43">
     <cfRule type="dataBar" priority="66">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9390,20 +8739,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:BN7">
-    <cfRule type="expression" dxfId="20" priority="109">
+    <cfRule type="expression" dxfId="15" priority="109">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K8:BN13 K15:BN22 K24:BN51">
-    <cfRule type="expression" dxfId="19" priority="112">
+  <conditionalFormatting sqref="K8:BN13 K15:BN22 K24:BN54">
+    <cfRule type="expression" dxfId="14" priority="112">
       <formula>AND($E8&lt;=K$6,ROUNDDOWN(($F8-$E8+1)*$H8,0)+$E8-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="113">
+    <cfRule type="expression" dxfId="13" priority="113">
       <formula>AND(NOT(ISBLANK($E8)),$E8&lt;=K$6,$F8&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K6:BN13 K15:BN22 K24:BN29 K38:BN43 K45:BN50">
-    <cfRule type="expression" dxfId="17" priority="72">
+  <conditionalFormatting sqref="K6:BN13 K15:BN22 K24:BN29 K38:BN43">
+    <cfRule type="expression" dxfId="12" priority="72">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9422,15 +8771,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14:BN14">
-    <cfRule type="expression" dxfId="16" priority="63">
+    <cfRule type="expression" dxfId="11" priority="63">
       <formula>AND($E14&lt;=K$6,ROUNDDOWN(($F14-$E14+1)*$H14,0)+$E14-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="64">
+    <cfRule type="expression" dxfId="10" priority="64">
       <formula>AND(NOT(ISBLANK($E14)),$E14&lt;=K$6,$F14&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14:BN14">
-    <cfRule type="expression" dxfId="14" priority="62">
+    <cfRule type="expression" dxfId="9" priority="62">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9449,7 +8798,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30:BN30">
-    <cfRule type="expression" dxfId="13" priority="54">
+    <cfRule type="expression" dxfId="8" priority="54">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9468,15 +8817,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K23:BN23">
-    <cfRule type="expression" dxfId="12" priority="51">
+    <cfRule type="expression" dxfId="7" priority="51">
       <formula>AND($E23&lt;=K$6,ROUNDDOWN(($F23-$E23+1)*$H23,0)+$E23-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="52">
+    <cfRule type="expression" dxfId="6" priority="52">
       <formula>AND(NOT(ISBLANK($E23)),$E23&lt;=K$6,$F23&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K23:BN23">
-    <cfRule type="expression" dxfId="10" priority="50">
+    <cfRule type="expression" dxfId="5" priority="50">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9495,22 +8844,8 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31:BN31">
-    <cfRule type="expression" dxfId="9" priority="46">
+    <cfRule type="expression" dxfId="4" priority="46">
       <formula>K$6=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H51">
-    <cfRule type="dataBar" priority="17">
-      <dataBar>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{899A89DD-74A0-466B-A372-72AFD40C14A4}</x14:id>
-        </ext>
-      </extLst>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32:H37">
@@ -9528,12 +8863,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32:BN37">
-    <cfRule type="expression" dxfId="8" priority="42">
-      <formula>K$6=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K51:BN51">
-    <cfRule type="expression" dxfId="7" priority="18">
+    <cfRule type="expression" dxfId="3" priority="42">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9552,11 +8882,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K44:BN44">
-    <cfRule type="expression" dxfId="6" priority="26">
+    <cfRule type="expression" dxfId="2" priority="26">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H52:H56">
+  <conditionalFormatting sqref="H45:H49">
     <cfRule type="dataBar" priority="13">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9570,20 +8900,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K52:BN56">
-    <cfRule type="expression" dxfId="5" priority="15">
-      <formula>AND($E52&lt;=K$6,ROUNDDOWN(($F52-$E52+1)*$H52,0)+$E52-1&gt;=K$6)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="16">
-      <formula>AND(NOT(ISBLANK($E52)),$E52&lt;=K$6,$F52&gt;=K$6)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K52:BN56">
-    <cfRule type="expression" dxfId="3" priority="14">
+  <conditionalFormatting sqref="K45:BN49">
+    <cfRule type="expression" dxfId="1" priority="14">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H57:H61">
+  <conditionalFormatting sqref="H50:H54">
     <cfRule type="dataBar" priority="7">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -9597,15 +8919,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K57:BN61">
-    <cfRule type="expression" dxfId="2" priority="9">
-      <formula>AND($E57&lt;=K$6,ROUNDDOWN(($F57-$E57+1)*$H57,0)+$E57-1&gt;=K$6)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="10">
-      <formula>AND(NOT(ISBLANK($E57)),$E57&lt;=K$6,$F57&gt;=K$6)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K57:BN61">
+  <conditionalFormatting sqref="K50:BN54">
     <cfRule type="expression" dxfId="0" priority="8">
       <formula>K$6=TODAY()</formula>
     </cfRule>
@@ -9669,7 +8983,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H8:H13 H15:H22 H24:H29 H38:H43 H45:H50</xm:sqref>
+          <xm:sqref>H8:H13 H15:H22 H24:H29 H38:H43</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{8B894183-9857-4A8A-A710-A8E0A3639C63}">
@@ -9732,21 +9046,6 @@
           <xm:sqref>H31</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{899A89DD-74A0-466B-A372-72AFD40C14A4}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>H51</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{FBE85918-163F-478B-A582-154FD7C53A35}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
@@ -9789,7 +9088,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H52:H56</xm:sqref>
+          <xm:sqref>H45:H49</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{120CCD98-F855-4770-BAE7-6F6EA0A92E96}">
@@ -9804,7 +9103,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H57:H61</xm:sqref>
+          <xm:sqref>H50:H54</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
docs(gantt): sesuai client meet
</commit_message>
<xml_diff>
--- a/docs/Gantt Chart.xlsx
+++ b/docs/Gantt Chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Materi Semester 7\PWL\warawiriweb\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\punch\Documents\GitHub\warawiriweb\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD6D988-B0F1-41B4-931F-7C6FE5BDC3F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ABBEF32-3082-4DEF-8C64-C5527D35A1D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChart" sheetId="9" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="prevWBS" localSheetId="0">GanttChart!$A1048576</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">GanttChart!$A$1:$BN$33</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">GanttChart!$A$1:$BN$32</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">GanttChartPro!$A$1:$C$47</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">GanttChart!$4:$7</definedName>
     <definedName name="valuevx">42.314159</definedName>
@@ -28,7 +28,18 @@
     <definedName name="vertex42_id" hidden="1">"gantt-chart_L.xlsx"</definedName>
     <definedName name="vertex42_title" hidden="1">"Gantt Chart Template"</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -443,7 +454,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="186">
   <si>
     <t>WBS</t>
   </si>
@@ -1538,18 +1549,12 @@
     <t>Dandy</t>
   </si>
   <si>
-    <t>Initiation 2</t>
-  </si>
-  <si>
     <t>Design &amp; Typography (rev)</t>
   </si>
   <si>
     <t>Navbar Mockup</t>
   </si>
   <si>
-    <t>Initiation &amp; Web Build 1</t>
-  </si>
-  <si>
     <t>Navbar &amp; Home Frontend</t>
   </si>
   <si>
@@ -1662,6 +1667,9 @@
   </si>
   <si>
     <t>Deploy</t>
+  </si>
+  <si>
+    <t>Web Build 1</t>
   </si>
 </sst>
 </file>
@@ -2852,6 +2860,24 @@
     <xf numFmtId="1" fontId="50" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2859,27 +2885,9 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="45" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2931,7 +2939,7 @@
     <cellStyle name="Total" xfId="42" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="43" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="14">
     <dxf>
       <border>
         <left style="thin">
@@ -3003,20 +3011,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <border>
@@ -3180,7 +3174,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$H$4" horiz="1" max="100" min="1" page="0" val="3"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$H$4" horiz="1" max="100" min="1" page="0"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3836,11 +3830,11 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BN54"/>
+  <dimension ref="A1:BN53"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B55" sqref="B55"/>
+      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3867,29 +3861,29 @@
       <c r="E1" s="29"/>
       <c r="F1" s="29"/>
       <c r="I1" s="78"/>
-      <c r="K1" s="111" t="s">
+      <c r="K1" s="117" t="s">
         <v>71</v>
       </c>
-      <c r="L1" s="111"/>
-      <c r="M1" s="111"/>
-      <c r="N1" s="111"/>
-      <c r="O1" s="111"/>
-      <c r="P1" s="111"/>
-      <c r="Q1" s="111"/>
-      <c r="R1" s="111"/>
-      <c r="S1" s="111"/>
-      <c r="T1" s="111"/>
-      <c r="U1" s="111"/>
-      <c r="V1" s="111"/>
-      <c r="W1" s="111"/>
-      <c r="X1" s="111"/>
-      <c r="Y1" s="111"/>
-      <c r="Z1" s="111"/>
-      <c r="AA1" s="111"/>
-      <c r="AB1" s="111"/>
-      <c r="AC1" s="111"/>
-      <c r="AD1" s="111"/>
-      <c r="AE1" s="111"/>
+      <c r="L1" s="117"/>
+      <c r="M1" s="117"/>
+      <c r="N1" s="117"/>
+      <c r="O1" s="117"/>
+      <c r="P1" s="117"/>
+      <c r="Q1" s="117"/>
+      <c r="R1" s="117"/>
+      <c r="S1" s="117"/>
+      <c r="T1" s="117"/>
+      <c r="U1" s="117"/>
+      <c r="V1" s="117"/>
+      <c r="W1" s="117"/>
+      <c r="X1" s="117"/>
+      <c r="Y1" s="117"/>
+      <c r="Z1" s="117"/>
+      <c r="AA1" s="117"/>
+      <c r="AB1" s="117"/>
+      <c r="AC1" s="117"/>
+      <c r="AD1" s="117"/>
+      <c r="AE1" s="117"/>
     </row>
     <row r="2" spans="1:66" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
@@ -3929,196 +3923,196 @@
       <c r="B4" s="65" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="116">
+      <c r="C4" s="119">
         <v>45194</v>
       </c>
-      <c r="D4" s="116"/>
-      <c r="E4" s="116"/>
+      <c r="D4" s="119"/>
+      <c r="E4" s="119"/>
       <c r="F4" s="64"/>
       <c r="G4" s="65" t="s">
         <v>68</v>
       </c>
       <c r="H4" s="77">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="30"/>
-      <c r="K4" s="113" t="str">
+      <c r="K4" s="111" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+        <v>Week 1</v>
+      </c>
+      <c r="L4" s="112"/>
+      <c r="M4" s="112"/>
+      <c r="N4" s="112"/>
+      <c r="O4" s="112"/>
+      <c r="P4" s="112"/>
+      <c r="Q4" s="113"/>
+      <c r="R4" s="111" t="str">
+        <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+        <v>Week 2</v>
+      </c>
+      <c r="S4" s="112"/>
+      <c r="T4" s="112"/>
+      <c r="U4" s="112"/>
+      <c r="V4" s="112"/>
+      <c r="W4" s="112"/>
+      <c r="X4" s="113"/>
+      <c r="Y4" s="111" t="str">
+        <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 3</v>
       </c>
-      <c r="L4" s="114"/>
-      <c r="M4" s="114"/>
-      <c r="N4" s="114"/>
-      <c r="O4" s="114"/>
-      <c r="P4" s="114"/>
-      <c r="Q4" s="115"/>
-      <c r="R4" s="113" t="str">
-        <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="Z4" s="112"/>
+      <c r="AA4" s="112"/>
+      <c r="AB4" s="112"/>
+      <c r="AC4" s="112"/>
+      <c r="AD4" s="112"/>
+      <c r="AE4" s="113"/>
+      <c r="AF4" s="111" t="str">
+        <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="S4" s="114"/>
-      <c r="T4" s="114"/>
-      <c r="U4" s="114"/>
-      <c r="V4" s="114"/>
-      <c r="W4" s="114"/>
-      <c r="X4" s="115"/>
-      <c r="Y4" s="113" t="str">
-        <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="AG4" s="112"/>
+      <c r="AH4" s="112"/>
+      <c r="AI4" s="112"/>
+      <c r="AJ4" s="112"/>
+      <c r="AK4" s="112"/>
+      <c r="AL4" s="113"/>
+      <c r="AM4" s="111" t="str">
+        <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="Z4" s="114"/>
-      <c r="AA4" s="114"/>
-      <c r="AB4" s="114"/>
-      <c r="AC4" s="114"/>
-      <c r="AD4" s="114"/>
-      <c r="AE4" s="115"/>
-      <c r="AF4" s="113" t="str">
-        <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="AN4" s="112"/>
+      <c r="AO4" s="112"/>
+      <c r="AP4" s="112"/>
+      <c r="AQ4" s="112"/>
+      <c r="AR4" s="112"/>
+      <c r="AS4" s="113"/>
+      <c r="AT4" s="111" t="str">
+        <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="AG4" s="114"/>
-      <c r="AH4" s="114"/>
-      <c r="AI4" s="114"/>
-      <c r="AJ4" s="114"/>
-      <c r="AK4" s="114"/>
-      <c r="AL4" s="115"/>
-      <c r="AM4" s="113" t="str">
-        <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="AU4" s="112"/>
+      <c r="AV4" s="112"/>
+      <c r="AW4" s="112"/>
+      <c r="AX4" s="112"/>
+      <c r="AY4" s="112"/>
+      <c r="AZ4" s="113"/>
+      <c r="BA4" s="111" t="str">
+        <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="AN4" s="114"/>
-      <c r="AO4" s="114"/>
-      <c r="AP4" s="114"/>
-      <c r="AQ4" s="114"/>
-      <c r="AR4" s="114"/>
-      <c r="AS4" s="115"/>
-      <c r="AT4" s="113" t="str">
-        <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="BB4" s="112"/>
+      <c r="BC4" s="112"/>
+      <c r="BD4" s="112"/>
+      <c r="BE4" s="112"/>
+      <c r="BF4" s="112"/>
+      <c r="BG4" s="113"/>
+      <c r="BH4" s="111" t="str">
+        <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="AU4" s="114"/>
-      <c r="AV4" s="114"/>
-      <c r="AW4" s="114"/>
-      <c r="AX4" s="114"/>
-      <c r="AY4" s="114"/>
-      <c r="AZ4" s="115"/>
-      <c r="BA4" s="113" t="str">
-        <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 9</v>
-      </c>
-      <c r="BB4" s="114"/>
-      <c r="BC4" s="114"/>
-      <c r="BD4" s="114"/>
-      <c r="BE4" s="114"/>
-      <c r="BF4" s="114"/>
-      <c r="BG4" s="115"/>
-      <c r="BH4" s="113" t="str">
-        <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 10</v>
-      </c>
-      <c r="BI4" s="114"/>
-      <c r="BJ4" s="114"/>
-      <c r="BK4" s="114"/>
-      <c r="BL4" s="114"/>
-      <c r="BM4" s="114"/>
-      <c r="BN4" s="115"/>
+      <c r="BI4" s="112"/>
+      <c r="BJ4" s="112"/>
+      <c r="BK4" s="112"/>
+      <c r="BL4" s="112"/>
+      <c r="BM4" s="112"/>
+      <c r="BN4" s="113"/>
     </row>
     <row r="5" spans="1:66" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="64"/>
       <c r="B5" s="65" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="112" t="s">
+      <c r="C5" s="118" t="s">
         <v>132</v>
       </c>
-      <c r="D5" s="112"/>
-      <c r="E5" s="112"/>
+      <c r="D5" s="118"/>
+      <c r="E5" s="118"/>
       <c r="F5" s="64"/>
       <c r="G5" s="64"/>
       <c r="H5" s="64"/>
       <c r="I5" s="64"/>
       <c r="J5" s="30"/>
-      <c r="K5" s="117">
+      <c r="K5" s="114">
         <f>K6</f>
+        <v>45194</v>
+      </c>
+      <c r="L5" s="115"/>
+      <c r="M5" s="115"/>
+      <c r="N5" s="115"/>
+      <c r="O5" s="115"/>
+      <c r="P5" s="115"/>
+      <c r="Q5" s="116"/>
+      <c r="R5" s="114">
+        <f>R6</f>
+        <v>45201</v>
+      </c>
+      <c r="S5" s="115"/>
+      <c r="T5" s="115"/>
+      <c r="U5" s="115"/>
+      <c r="V5" s="115"/>
+      <c r="W5" s="115"/>
+      <c r="X5" s="116"/>
+      <c r="Y5" s="114">
+        <f>Y6</f>
         <v>45208</v>
       </c>
-      <c r="L5" s="118"/>
-      <c r="M5" s="118"/>
-      <c r="N5" s="118"/>
-      <c r="O5" s="118"/>
-      <c r="P5" s="118"/>
-      <c r="Q5" s="119"/>
-      <c r="R5" s="117">
-        <f>R6</f>
+      <c r="Z5" s="115"/>
+      <c r="AA5" s="115"/>
+      <c r="AB5" s="115"/>
+      <c r="AC5" s="115"/>
+      <c r="AD5" s="115"/>
+      <c r="AE5" s="116"/>
+      <c r="AF5" s="114">
+        <f>AF6</f>
         <v>45215</v>
       </c>
-      <c r="S5" s="118"/>
-      <c r="T5" s="118"/>
-      <c r="U5" s="118"/>
-      <c r="V5" s="118"/>
-      <c r="W5" s="118"/>
-      <c r="X5" s="119"/>
-      <c r="Y5" s="117">
-        <f>Y6</f>
+      <c r="AG5" s="115"/>
+      <c r="AH5" s="115"/>
+      <c r="AI5" s="115"/>
+      <c r="AJ5" s="115"/>
+      <c r="AK5" s="115"/>
+      <c r="AL5" s="116"/>
+      <c r="AM5" s="114">
+        <f>AM6</f>
         <v>45222</v>
       </c>
-      <c r="Z5" s="118"/>
-      <c r="AA5" s="118"/>
-      <c r="AB5" s="118"/>
-      <c r="AC5" s="118"/>
-      <c r="AD5" s="118"/>
-      <c r="AE5" s="119"/>
-      <c r="AF5" s="117">
-        <f>AF6</f>
+      <c r="AN5" s="115"/>
+      <c r="AO5" s="115"/>
+      <c r="AP5" s="115"/>
+      <c r="AQ5" s="115"/>
+      <c r="AR5" s="115"/>
+      <c r="AS5" s="116"/>
+      <c r="AT5" s="114">
+        <f>AT6</f>
         <v>45229</v>
       </c>
-      <c r="AG5" s="118"/>
-      <c r="AH5" s="118"/>
-      <c r="AI5" s="118"/>
-      <c r="AJ5" s="118"/>
-      <c r="AK5" s="118"/>
-      <c r="AL5" s="119"/>
-      <c r="AM5" s="117">
-        <f>AM6</f>
+      <c r="AU5" s="115"/>
+      <c r="AV5" s="115"/>
+      <c r="AW5" s="115"/>
+      <c r="AX5" s="115"/>
+      <c r="AY5" s="115"/>
+      <c r="AZ5" s="116"/>
+      <c r="BA5" s="114">
+        <f>BA6</f>
         <v>45236</v>
       </c>
-      <c r="AN5" s="118"/>
-      <c r="AO5" s="118"/>
-      <c r="AP5" s="118"/>
-      <c r="AQ5" s="118"/>
-      <c r="AR5" s="118"/>
-      <c r="AS5" s="119"/>
-      <c r="AT5" s="117">
-        <f>AT6</f>
+      <c r="BB5" s="115"/>
+      <c r="BC5" s="115"/>
+      <c r="BD5" s="115"/>
+      <c r="BE5" s="115"/>
+      <c r="BF5" s="115"/>
+      <c r="BG5" s="116"/>
+      <c r="BH5" s="114">
+        <f>BH6</f>
         <v>45243</v>
       </c>
-      <c r="AU5" s="118"/>
-      <c r="AV5" s="118"/>
-      <c r="AW5" s="118"/>
-      <c r="AX5" s="118"/>
-      <c r="AY5" s="118"/>
-      <c r="AZ5" s="119"/>
-      <c r="BA5" s="117">
-        <f>BA6</f>
-        <v>45250</v>
-      </c>
-      <c r="BB5" s="118"/>
-      <c r="BC5" s="118"/>
-      <c r="BD5" s="118"/>
-      <c r="BE5" s="118"/>
-      <c r="BF5" s="118"/>
-      <c r="BG5" s="119"/>
-      <c r="BH5" s="117">
-        <f>BH6</f>
-        <v>45257</v>
-      </c>
-      <c r="BI5" s="118"/>
-      <c r="BJ5" s="118"/>
-      <c r="BK5" s="118"/>
-      <c r="BL5" s="118"/>
-      <c r="BM5" s="118"/>
-      <c r="BN5" s="119"/>
+      <c r="BI5" s="115"/>
+      <c r="BJ5" s="115"/>
+      <c r="BK5" s="115"/>
+      <c r="BL5" s="115"/>
+      <c r="BM5" s="115"/>
+      <c r="BN5" s="116"/>
     </row>
     <row r="6" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A6" s="30"/>
@@ -4133,227 +4127,227 @@
       <c r="J6" s="30"/>
       <c r="K6" s="53">
         <f>C4-WEEKDAY(C4,1)+2+7*(H4-1)</f>
-        <v>45208</v>
+        <v>45194</v>
       </c>
       <c r="L6" s="44">
         <f t="shared" ref="L6:AQ6" si="0">K6+1</f>
-        <v>45209</v>
+        <v>45195</v>
       </c>
       <c r="M6" s="44">
         <f t="shared" si="0"/>
-        <v>45210</v>
+        <v>45196</v>
       </c>
       <c r="N6" s="44">
         <f t="shared" si="0"/>
-        <v>45211</v>
+        <v>45197</v>
       </c>
       <c r="O6" s="44">
         <f t="shared" si="0"/>
-        <v>45212</v>
+        <v>45198</v>
       </c>
       <c r="P6" s="44">
         <f t="shared" si="0"/>
-        <v>45213</v>
+        <v>45199</v>
       </c>
       <c r="Q6" s="54">
         <f t="shared" si="0"/>
-        <v>45214</v>
+        <v>45200</v>
       </c>
       <c r="R6" s="53">
         <f t="shared" si="0"/>
-        <v>45215</v>
+        <v>45201</v>
       </c>
       <c r="S6" s="44">
         <f t="shared" si="0"/>
-        <v>45216</v>
+        <v>45202</v>
       </c>
       <c r="T6" s="44">
         <f t="shared" si="0"/>
-        <v>45217</v>
+        <v>45203</v>
       </c>
       <c r="U6" s="44">
         <f t="shared" si="0"/>
-        <v>45218</v>
+        <v>45204</v>
       </c>
       <c r="V6" s="44">
         <f t="shared" si="0"/>
-        <v>45219</v>
+        <v>45205</v>
       </c>
       <c r="W6" s="44">
         <f t="shared" si="0"/>
-        <v>45220</v>
+        <v>45206</v>
       </c>
       <c r="X6" s="54">
         <f t="shared" si="0"/>
-        <v>45221</v>
+        <v>45207</v>
       </c>
       <c r="Y6" s="53">
         <f t="shared" si="0"/>
-        <v>45222</v>
+        <v>45208</v>
       </c>
       <c r="Z6" s="44">
         <f t="shared" si="0"/>
-        <v>45223</v>
+        <v>45209</v>
       </c>
       <c r="AA6" s="44">
         <f t="shared" si="0"/>
-        <v>45224</v>
+        <v>45210</v>
       </c>
       <c r="AB6" s="44">
         <f t="shared" si="0"/>
-        <v>45225</v>
+        <v>45211</v>
       </c>
       <c r="AC6" s="44">
         <f t="shared" si="0"/>
-        <v>45226</v>
+        <v>45212</v>
       </c>
       <c r="AD6" s="44">
         <f t="shared" si="0"/>
-        <v>45227</v>
+        <v>45213</v>
       </c>
       <c r="AE6" s="54">
         <f t="shared" si="0"/>
-        <v>45228</v>
+        <v>45214</v>
       </c>
       <c r="AF6" s="53">
         <f t="shared" si="0"/>
-        <v>45229</v>
+        <v>45215</v>
       </c>
       <c r="AG6" s="44">
         <f t="shared" si="0"/>
-        <v>45230</v>
+        <v>45216</v>
       </c>
       <c r="AH6" s="44">
         <f t="shared" si="0"/>
-        <v>45231</v>
+        <v>45217</v>
       </c>
       <c r="AI6" s="44">
         <f t="shared" si="0"/>
-        <v>45232</v>
+        <v>45218</v>
       </c>
       <c r="AJ6" s="44">
         <f t="shared" si="0"/>
-        <v>45233</v>
+        <v>45219</v>
       </c>
       <c r="AK6" s="44">
         <f t="shared" si="0"/>
-        <v>45234</v>
+        <v>45220</v>
       </c>
       <c r="AL6" s="54">
         <f t="shared" si="0"/>
-        <v>45235</v>
+        <v>45221</v>
       </c>
       <c r="AM6" s="53">
         <f t="shared" si="0"/>
-        <v>45236</v>
+        <v>45222</v>
       </c>
       <c r="AN6" s="44">
         <f t="shared" si="0"/>
-        <v>45237</v>
+        <v>45223</v>
       </c>
       <c r="AO6" s="44">
         <f t="shared" si="0"/>
-        <v>45238</v>
+        <v>45224</v>
       </c>
       <c r="AP6" s="44">
         <f t="shared" si="0"/>
-        <v>45239</v>
+        <v>45225</v>
       </c>
       <c r="AQ6" s="44">
         <f t="shared" si="0"/>
-        <v>45240</v>
+        <v>45226</v>
       </c>
       <c r="AR6" s="44">
         <f t="shared" ref="AR6:BN6" si="1">AQ6+1</f>
-        <v>45241</v>
+        <v>45227</v>
       </c>
       <c r="AS6" s="54">
         <f t="shared" si="1"/>
-        <v>45242</v>
+        <v>45228</v>
       </c>
       <c r="AT6" s="53">
         <f t="shared" si="1"/>
-        <v>45243</v>
+        <v>45229</v>
       </c>
       <c r="AU6" s="44">
         <f t="shared" si="1"/>
-        <v>45244</v>
+        <v>45230</v>
       </c>
       <c r="AV6" s="44">
         <f t="shared" si="1"/>
-        <v>45245</v>
+        <v>45231</v>
       </c>
       <c r="AW6" s="44">
         <f t="shared" si="1"/>
-        <v>45246</v>
+        <v>45232</v>
       </c>
       <c r="AX6" s="44">
         <f t="shared" si="1"/>
-        <v>45247</v>
+        <v>45233</v>
       </c>
       <c r="AY6" s="44">
         <f t="shared" si="1"/>
-        <v>45248</v>
+        <v>45234</v>
       </c>
       <c r="AZ6" s="54">
         <f t="shared" si="1"/>
-        <v>45249</v>
+        <v>45235</v>
       </c>
       <c r="BA6" s="53">
         <f t="shared" si="1"/>
-        <v>45250</v>
+        <v>45236</v>
       </c>
       <c r="BB6" s="44">
         <f t="shared" si="1"/>
-        <v>45251</v>
+        <v>45237</v>
       </c>
       <c r="BC6" s="44">
         <f t="shared" si="1"/>
-        <v>45252</v>
+        <v>45238</v>
       </c>
       <c r="BD6" s="44">
         <f t="shared" si="1"/>
-        <v>45253</v>
+        <v>45239</v>
       </c>
       <c r="BE6" s="44">
         <f t="shared" si="1"/>
-        <v>45254</v>
+        <v>45240</v>
       </c>
       <c r="BF6" s="44">
         <f t="shared" si="1"/>
-        <v>45255</v>
+        <v>45241</v>
       </c>
       <c r="BG6" s="54">
         <f t="shared" si="1"/>
-        <v>45256</v>
+        <v>45242</v>
       </c>
       <c r="BH6" s="53">
         <f t="shared" si="1"/>
-        <v>45257</v>
+        <v>45243</v>
       </c>
       <c r="BI6" s="44">
         <f t="shared" si="1"/>
-        <v>45258</v>
+        <v>45244</v>
       </c>
       <c r="BJ6" s="44">
         <f t="shared" si="1"/>
-        <v>45259</v>
+        <v>45245</v>
       </c>
       <c r="BK6" s="44">
         <f t="shared" si="1"/>
-        <v>45260</v>
+        <v>45246</v>
       </c>
       <c r="BL6" s="44">
         <f t="shared" si="1"/>
-        <v>45261</v>
+        <v>45247</v>
       </c>
       <c r="BM6" s="44">
         <f t="shared" si="1"/>
-        <v>45262</v>
+        <v>45248</v>
       </c>
       <c r="BN6" s="54">
         <f t="shared" si="1"/>
-        <v>45263</v>
+        <v>45249</v>
       </c>
     </row>
     <row r="7" spans="1:66" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -4632,7 +4626,7 @@
       </c>
       <c r="H8" s="51"/>
       <c r="I8" s="52">
-        <f t="shared" ref="I8:I29" si="4">IF(OR(F8=0,E8=0)," - ",NETWORKDAYS(E8,F8))</f>
+        <f t="shared" ref="I8:I28" si="4">IF(OR(F8=0,E8=0)," - ",NETWORKDAYS(E8,F8))</f>
         <v>5</v>
       </c>
       <c r="J8" s="55"/>
@@ -4796,7 +4790,7 @@
         <v>45195</v>
       </c>
       <c r="F10" s="59">
-        <f t="shared" ref="F10:F29" si="6">IF(ISBLANK(E10)," - ",IF(G10=0,E10,E10+G10-1))</f>
+        <f t="shared" ref="F10:F28" si="6">IF(ISBLANK(E10)," - ",IF(G10=0,E10,E10+G10-1))</f>
         <v>45197</v>
       </c>
       <c r="G10" s="41">
@@ -4960,7 +4954,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>145</v>
+        <v>185</v>
       </c>
       <c r="D12" s="35"/>
       <c r="E12" s="60">
@@ -4968,15 +4962,15 @@
       </c>
       <c r="F12" s="60">
         <f>IF(ISBLANK(E12)," - ",IF(G12=0,E12,E12+G12-1))</f>
-        <v>45205</v>
+        <v>45212</v>
       </c>
       <c r="G12" s="36">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="H12" s="37"/>
       <c r="I12" s="38">
         <f>IF(OR(F12=0,E12=0)," - ",NETWORKDAYS(E12,F12))</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J12" s="57"/>
       <c r="K12" s="63"/>
@@ -5300,117 +5294,123 @@
       <c r="BM15" s="39"/>
       <c r="BN15" s="39"/>
     </row>
-    <row r="16" spans="1:66" s="34" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A16" s="32" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>3</v>
-      </c>
-      <c r="B16" s="33" t="s">
-        <v>148</v>
-      </c>
-      <c r="D16" s="35"/>
-      <c r="E16" s="60">
+    <row r="16" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A16" s="39" t="str">
+        <f t="shared" ref="A16:A22" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>2.4</v>
+      </c>
+      <c r="B16" s="75" t="s">
+        <v>142</v>
+      </c>
+      <c r="C16" s="40" t="s">
+        <v>137</v>
+      </c>
+      <c r="D16" s="76"/>
+      <c r="E16" s="58">
+        <f>F15+3</f>
         <v>45208</v>
       </c>
-      <c r="F16" s="60">
+      <c r="F16" s="59">
         <f t="shared" si="6"/>
-        <v>45212</v>
-      </c>
-      <c r="G16" s="36">
-        <v>5</v>
-      </c>
-      <c r="H16" s="37"/>
-      <c r="I16" s="38">
+        <v>45211</v>
+      </c>
+      <c r="G16" s="41">
+        <v>4</v>
+      </c>
+      <c r="H16" s="42">
+        <v>1</v>
+      </c>
+      <c r="I16" s="43">
         <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="J16" s="57"/>
-      <c r="K16" s="63"/>
-      <c r="L16" s="63"/>
-      <c r="M16" s="63"/>
-      <c r="N16" s="63"/>
-      <c r="O16" s="63"/>
-      <c r="P16" s="63"/>
-      <c r="Q16" s="63"/>
-      <c r="R16" s="63"/>
-      <c r="S16" s="63"/>
-      <c r="T16" s="63"/>
-      <c r="U16" s="63"/>
-      <c r="V16" s="63"/>
-      <c r="W16" s="63"/>
-      <c r="X16" s="63"/>
-      <c r="Y16" s="63"/>
-      <c r="Z16" s="63"/>
-      <c r="AA16" s="63"/>
-      <c r="AB16" s="63"/>
-      <c r="AC16" s="63"/>
-      <c r="AD16" s="63"/>
-      <c r="AE16" s="63"/>
-      <c r="AF16" s="63"/>
-      <c r="AG16" s="63"/>
-      <c r="AH16" s="63"/>
-      <c r="AI16" s="63"/>
-      <c r="AJ16" s="63"/>
-      <c r="AK16" s="63"/>
-      <c r="AL16" s="63"/>
-      <c r="AM16" s="63"/>
-      <c r="AN16" s="63"/>
-      <c r="AO16" s="63"/>
-      <c r="AP16" s="63"/>
-      <c r="AQ16" s="63"/>
-      <c r="AR16" s="63"/>
-      <c r="AS16" s="63"/>
-      <c r="AT16" s="63"/>
-      <c r="AU16" s="63"/>
-      <c r="AV16" s="63"/>
-      <c r="AW16" s="63"/>
-      <c r="AX16" s="63"/>
-      <c r="AY16" s="63"/>
-      <c r="AZ16" s="63"/>
-      <c r="BA16" s="63"/>
-      <c r="BB16" s="63"/>
-      <c r="BC16" s="63"/>
-      <c r="BD16" s="63"/>
-      <c r="BE16" s="63"/>
-      <c r="BF16" s="63"/>
-      <c r="BG16" s="63"/>
-      <c r="BH16" s="63"/>
-      <c r="BI16" s="63"/>
-      <c r="BJ16" s="63"/>
-      <c r="BK16" s="63"/>
-      <c r="BL16" s="63"/>
-      <c r="BM16" s="63"/>
-      <c r="BN16" s="63"/>
-    </row>
-    <row r="17" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="J16" s="56"/>
+      <c r="K16" s="39"/>
+      <c r="L16" s="39"/>
+      <c r="M16" s="39"/>
+      <c r="N16" s="39"/>
+      <c r="O16" s="39"/>
+      <c r="P16" s="39"/>
+      <c r="Q16" s="39"/>
+      <c r="R16" s="39"/>
+      <c r="S16" s="39"/>
+      <c r="T16" s="39"/>
+      <c r="U16" s="39"/>
+      <c r="V16" s="39"/>
+      <c r="W16" s="39"/>
+      <c r="X16" s="39"/>
+      <c r="Y16" s="39"/>
+      <c r="Z16" s="39"/>
+      <c r="AA16" s="39"/>
+      <c r="AB16" s="39"/>
+      <c r="AC16" s="39"/>
+      <c r="AD16" s="39"/>
+      <c r="AE16" s="39"/>
+      <c r="AF16" s="39"/>
+      <c r="AG16" s="39"/>
+      <c r="AH16" s="39"/>
+      <c r="AI16" s="39"/>
+      <c r="AJ16" s="39"/>
+      <c r="AK16" s="39"/>
+      <c r="AL16" s="39"/>
+      <c r="AM16" s="39"/>
+      <c r="AN16" s="39"/>
+      <c r="AO16" s="39"/>
+      <c r="AP16" s="39"/>
+      <c r="AQ16" s="39"/>
+      <c r="AR16" s="39"/>
+      <c r="AS16" s="39"/>
+      <c r="AT16" s="39"/>
+      <c r="AU16" s="39"/>
+      <c r="AV16" s="39"/>
+      <c r="AW16" s="39"/>
+      <c r="AX16" s="39"/>
+      <c r="AY16" s="39"/>
+      <c r="AZ16" s="39"/>
+      <c r="BA16" s="39"/>
+      <c r="BB16" s="39"/>
+      <c r="BC16" s="39"/>
+      <c r="BD16" s="39"/>
+      <c r="BE16" s="39"/>
+      <c r="BF16" s="39"/>
+      <c r="BG16" s="39"/>
+      <c r="BH16" s="39"/>
+      <c r="BI16" s="39"/>
+      <c r="BJ16" s="39"/>
+      <c r="BK16" s="39"/>
+      <c r="BL16" s="39"/>
+      <c r="BM16" s="39"/>
+      <c r="BN16" s="39"/>
+    </row>
+    <row r="17" spans="1:66" s="40" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A17" s="39" t="str">
-        <f t="shared" ref="A17:A23" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>3.1</v>
+        <f t="shared" si="9"/>
+        <v>2.5</v>
       </c>
       <c r="B17" s="75" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C17" s="40" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="D17" s="76"/>
       <c r="E17" s="58">
-        <f>E16</f>
+        <f>F15+3</f>
         <v>45208</v>
       </c>
       <c r="F17" s="59">
         <f t="shared" si="6"/>
-        <v>45211</v>
+        <v>45210</v>
       </c>
       <c r="G17" s="41">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H17" s="42">
         <v>1</v>
       </c>
       <c r="I17" s="43">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J17" s="56"/>
       <c r="K17" s="39"/>
@@ -5470,35 +5470,35 @@
       <c r="BM17" s="39"/>
       <c r="BN17" s="39"/>
     </row>
-    <row r="18" spans="1:66" s="40" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="39" t="str">
         <f t="shared" si="9"/>
-        <v>3.2</v>
+        <v>2.6</v>
       </c>
       <c r="B18" s="75" t="s">
         <v>146</v>
       </c>
       <c r="C18" s="40" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="D18" s="76"/>
       <c r="E18" s="58">
-        <f>E16</f>
+        <f>E17</f>
         <v>45208</v>
       </c>
       <c r="F18" s="59">
         <f t="shared" si="6"/>
-        <v>45210</v>
+        <v>45208</v>
       </c>
       <c r="G18" s="41">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H18" s="42">
         <v>1</v>
       </c>
       <c r="I18" s="43">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J18" s="56"/>
       <c r="K18" s="39"/>
@@ -5558,25 +5558,25 @@
       <c r="BM18" s="39"/>
       <c r="BN18" s="39"/>
     </row>
-    <row r="19" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:66" s="40" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A19" s="39" t="str">
         <f t="shared" si="9"/>
-        <v>3.3</v>
+        <v>2.7</v>
       </c>
       <c r="B19" s="75" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C19" s="40" t="s">
         <v>134</v>
       </c>
       <c r="D19" s="76"/>
       <c r="E19" s="58">
-        <f>E16</f>
-        <v>45208</v>
+        <f>F18+1</f>
+        <v>45209</v>
       </c>
       <c r="F19" s="59">
         <f t="shared" si="6"/>
-        <v>45208</v>
+        <v>45209</v>
       </c>
       <c r="G19" s="41">
         <v>1</v>
@@ -5649,32 +5649,32 @@
     <row r="20" spans="1:66" s="40" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A20" s="39" t="str">
         <f t="shared" si="9"/>
-        <v>3.4</v>
+        <v>2.8</v>
       </c>
       <c r="B20" s="75" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C20" s="40" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="D20" s="76"/>
       <c r="E20" s="58">
-        <f>E16+1</f>
-        <v>45209</v>
+        <f>F19+1</f>
+        <v>45210</v>
       </c>
       <c r="F20" s="59">
         <f t="shared" si="6"/>
-        <v>45209</v>
+        <v>45211</v>
       </c>
       <c r="G20" s="41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H20" s="42">
         <v>1</v>
       </c>
       <c r="I20" s="43">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J20" s="56"/>
       <c r="K20" s="39"/>
@@ -5734,10 +5734,10 @@
       <c r="BM20" s="39"/>
       <c r="BN20" s="39"/>
     </row>
-    <row r="21" spans="1:66" s="40" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" s="39" t="str">
         <f t="shared" si="9"/>
-        <v>3.5</v>
+        <v>2.9</v>
       </c>
       <c r="B21" s="75" t="s">
         <v>149</v>
@@ -5745,26 +5745,26 @@
       <c r="C21" s="40" t="s">
         <v>150</v>
       </c>
-      <c r="D21" s="76"/>
-      <c r="E21" s="58">
-        <f>F20+1</f>
+      <c r="D21" s="104"/>
+      <c r="E21" s="105">
+        <f>F19+1</f>
         <v>45210</v>
       </c>
-      <c r="F21" s="59">
+      <c r="F21" s="106">
         <f t="shared" si="6"/>
         <v>45211</v>
       </c>
-      <c r="G21" s="41">
+      <c r="G21" s="107">
         <v>2</v>
       </c>
-      <c r="H21" s="42">
-        <v>1</v>
-      </c>
-      <c r="I21" s="43">
+      <c r="H21" s="108">
+        <v>0.5</v>
+      </c>
+      <c r="I21" s="109">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="J21" s="56"/>
+      <c r="J21" s="110"/>
       <c r="K21" s="39"/>
       <c r="L21" s="39"/>
       <c r="M21" s="39"/>
@@ -5825,32 +5825,32 @@
     <row r="22" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" s="39" t="str">
         <f t="shared" si="9"/>
-        <v>3.6</v>
+        <v>2.10</v>
       </c>
       <c r="B22" s="75" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="C22" s="40" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="D22" s="104"/>
       <c r="E22" s="105">
         <f>F20+1</f>
-        <v>45210</v>
+        <v>45212</v>
       </c>
       <c r="F22" s="106">
-        <f t="shared" si="6"/>
-        <v>45211</v>
+        <f t="shared" ref="F22" si="10">IF(ISBLANK(E22)," - ",IF(G22=0,E22,E22+G22-1))</f>
+        <v>45212</v>
       </c>
       <c r="G22" s="107">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H22" s="108">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="I22" s="109">
-        <f t="shared" si="4"/>
-        <v>2</v>
+        <f t="shared" ref="I22" si="11">IF(OR(F22=0,E22=0)," - ",NETWORKDAYS(E22,F22))</f>
+        <v>1</v>
       </c>
       <c r="J22" s="110"/>
       <c r="K22" s="39"/>
@@ -5910,205 +5910,205 @@
       <c r="BM22" s="39"/>
       <c r="BN22" s="39"/>
     </row>
-    <row r="23" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A23" s="39" t="str">
-        <f t="shared" si="9"/>
-        <v>3.7</v>
-      </c>
-      <c r="B23" s="75" t="s">
-        <v>162</v>
-      </c>
-      <c r="C23" s="40" t="s">
-        <v>134</v>
-      </c>
-      <c r="D23" s="104"/>
-      <c r="E23" s="105">
-        <f>F21+1</f>
-        <v>45212</v>
-      </c>
-      <c r="F23" s="106">
-        <f t="shared" ref="F23" si="10">IF(ISBLANK(E23)," - ",IF(G23=0,E23,E23+G23-1))</f>
-        <v>45212</v>
-      </c>
-      <c r="G23" s="107">
-        <v>1</v>
-      </c>
-      <c r="H23" s="108">
-        <v>0</v>
-      </c>
-      <c r="I23" s="109">
-        <f t="shared" ref="I23" si="11">IF(OR(F23=0,E23=0)," - ",NETWORKDAYS(E23,F23))</f>
-        <v>1</v>
-      </c>
-      <c r="J23" s="110"/>
-      <c r="K23" s="39"/>
-      <c r="L23" s="39"/>
-      <c r="M23" s="39"/>
-      <c r="N23" s="39"/>
-      <c r="O23" s="39"/>
-      <c r="P23" s="39"/>
-      <c r="Q23" s="39"/>
-      <c r="R23" s="39"/>
-      <c r="S23" s="39"/>
-      <c r="T23" s="39"/>
-      <c r="U23" s="39"/>
-      <c r="V23" s="39"/>
-      <c r="W23" s="39"/>
-      <c r="X23" s="39"/>
-      <c r="Y23" s="39"/>
-      <c r="Z23" s="39"/>
-      <c r="AA23" s="39"/>
-      <c r="AB23" s="39"/>
-      <c r="AC23" s="39"/>
-      <c r="AD23" s="39"/>
-      <c r="AE23" s="39"/>
-      <c r="AF23" s="39"/>
-      <c r="AG23" s="39"/>
-      <c r="AH23" s="39"/>
-      <c r="AI23" s="39"/>
-      <c r="AJ23" s="39"/>
-      <c r="AK23" s="39"/>
-      <c r="AL23" s="39"/>
-      <c r="AM23" s="39"/>
-      <c r="AN23" s="39"/>
-      <c r="AO23" s="39"/>
-      <c r="AP23" s="39"/>
-      <c r="AQ23" s="39"/>
-      <c r="AR23" s="39"/>
-      <c r="AS23" s="39"/>
-      <c r="AT23" s="39"/>
-      <c r="AU23" s="39"/>
-      <c r="AV23" s="39"/>
-      <c r="AW23" s="39"/>
-      <c r="AX23" s="39"/>
-      <c r="AY23" s="39"/>
-      <c r="AZ23" s="39"/>
-      <c r="BA23" s="39"/>
-      <c r="BB23" s="39"/>
-      <c r="BC23" s="39"/>
-      <c r="BD23" s="39"/>
-      <c r="BE23" s="39"/>
-      <c r="BF23" s="39"/>
-      <c r="BG23" s="39"/>
-      <c r="BH23" s="39"/>
-      <c r="BI23" s="39"/>
-      <c r="BJ23" s="39"/>
-      <c r="BK23" s="39"/>
-      <c r="BL23" s="39"/>
-      <c r="BM23" s="39"/>
-      <c r="BN23" s="39"/>
-    </row>
-    <row r="24" spans="1:66" s="34" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A24" s="32" t="str">
+    <row r="23" spans="1:66" s="34" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A23" s="32" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>4</v>
-      </c>
-      <c r="B24" s="33" t="s">
-        <v>160</v>
-      </c>
-      <c r="D24" s="35"/>
-      <c r="E24" s="60">
+        <v>3</v>
+      </c>
+      <c r="B23" s="33" t="s">
+        <v>158</v>
+      </c>
+      <c r="D23" s="35"/>
+      <c r="E23" s="60">
         <v>45215</v>
       </c>
-      <c r="F24" s="60">
+      <c r="F23" s="60">
         <f t="shared" si="6"/>
         <v>45219</v>
       </c>
-      <c r="G24" s="36">
+      <c r="G23" s="36">
         <v>5</v>
       </c>
-      <c r="H24" s="37"/>
-      <c r="I24" s="38">
+      <c r="H23" s="37"/>
+      <c r="I23" s="38">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="J24" s="57"/>
-      <c r="K24" s="63"/>
-      <c r="L24" s="63"/>
-      <c r="M24" s="63"/>
-      <c r="N24" s="63"/>
-      <c r="O24" s="63"/>
-      <c r="P24" s="63"/>
-      <c r="Q24" s="63"/>
-      <c r="R24" s="63"/>
-      <c r="S24" s="63"/>
-      <c r="T24" s="63"/>
-      <c r="U24" s="63"/>
-      <c r="V24" s="63"/>
-      <c r="W24" s="63"/>
-      <c r="X24" s="63"/>
-      <c r="Y24" s="63"/>
-      <c r="Z24" s="63"/>
-      <c r="AA24" s="63"/>
-      <c r="AB24" s="63"/>
-      <c r="AC24" s="63"/>
-      <c r="AD24" s="63"/>
-      <c r="AE24" s="63"/>
-      <c r="AF24" s="63"/>
-      <c r="AG24" s="63"/>
-      <c r="AH24" s="63"/>
-      <c r="AI24" s="63"/>
-      <c r="AJ24" s="63"/>
-      <c r="AK24" s="63"/>
-      <c r="AL24" s="63"/>
-      <c r="AM24" s="63"/>
-      <c r="AN24" s="63"/>
-      <c r="AO24" s="63"/>
-      <c r="AP24" s="63"/>
-      <c r="AQ24" s="63"/>
-      <c r="AR24" s="63"/>
-      <c r="AS24" s="63"/>
-      <c r="AT24" s="63"/>
-      <c r="AU24" s="63"/>
-      <c r="AV24" s="63"/>
-      <c r="AW24" s="63"/>
-      <c r="AX24" s="63"/>
-      <c r="AY24" s="63"/>
-      <c r="AZ24" s="63"/>
-      <c r="BA24" s="63"/>
-      <c r="BB24" s="63"/>
-      <c r="BC24" s="63"/>
-      <c r="BD24" s="63"/>
-      <c r="BE24" s="63"/>
-      <c r="BF24" s="63"/>
-      <c r="BG24" s="63"/>
-      <c r="BH24" s="63"/>
-      <c r="BI24" s="63"/>
-      <c r="BJ24" s="63"/>
-      <c r="BK24" s="63"/>
-      <c r="BL24" s="63"/>
-      <c r="BM24" s="63"/>
-      <c r="BN24" s="63"/>
+      <c r="J23" s="57"/>
+      <c r="K23" s="63"/>
+      <c r="L23" s="63"/>
+      <c r="M23" s="63"/>
+      <c r="N23" s="63"/>
+      <c r="O23" s="63"/>
+      <c r="P23" s="63"/>
+      <c r="Q23" s="63"/>
+      <c r="R23" s="63"/>
+      <c r="S23" s="63"/>
+      <c r="T23" s="63"/>
+      <c r="U23" s="63"/>
+      <c r="V23" s="63"/>
+      <c r="W23" s="63"/>
+      <c r="X23" s="63"/>
+      <c r="Y23" s="63"/>
+      <c r="Z23" s="63"/>
+      <c r="AA23" s="63"/>
+      <c r="AB23" s="63"/>
+      <c r="AC23" s="63"/>
+      <c r="AD23" s="63"/>
+      <c r="AE23" s="63"/>
+      <c r="AF23" s="63"/>
+      <c r="AG23" s="63"/>
+      <c r="AH23" s="63"/>
+      <c r="AI23" s="63"/>
+      <c r="AJ23" s="63"/>
+      <c r="AK23" s="63"/>
+      <c r="AL23" s="63"/>
+      <c r="AM23" s="63"/>
+      <c r="AN23" s="63"/>
+      <c r="AO23" s="63"/>
+      <c r="AP23" s="63"/>
+      <c r="AQ23" s="63"/>
+      <c r="AR23" s="63"/>
+      <c r="AS23" s="63"/>
+      <c r="AT23" s="63"/>
+      <c r="AU23" s="63"/>
+      <c r="AV23" s="63"/>
+      <c r="AW23" s="63"/>
+      <c r="AX23" s="63"/>
+      <c r="AY23" s="63"/>
+      <c r="AZ23" s="63"/>
+      <c r="BA23" s="63"/>
+      <c r="BB23" s="63"/>
+      <c r="BC23" s="63"/>
+      <c r="BD23" s="63"/>
+      <c r="BE23" s="63"/>
+      <c r="BF23" s="63"/>
+      <c r="BG23" s="63"/>
+      <c r="BH23" s="63"/>
+      <c r="BI23" s="63"/>
+      <c r="BJ23" s="63"/>
+      <c r="BK23" s="63"/>
+      <c r="BL23" s="63"/>
+      <c r="BM23" s="63"/>
+      <c r="BN23" s="63"/>
+    </row>
+    <row r="24" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A24" s="39" t="str">
+        <f t="shared" ref="A24:A30" si="12">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>3.1</v>
+      </c>
+      <c r="B24" s="75" t="s">
+        <v>152</v>
+      </c>
+      <c r="C24" s="40" t="s">
+        <v>153</v>
+      </c>
+      <c r="D24" s="76"/>
+      <c r="E24" s="58">
+        <f>E23</f>
+        <v>45215</v>
+      </c>
+      <c r="F24" s="59">
+        <f t="shared" si="6"/>
+        <v>45216</v>
+      </c>
+      <c r="G24" s="41">
+        <v>2</v>
+      </c>
+      <c r="H24" s="42">
+        <v>0</v>
+      </c>
+      <c r="I24" s="43">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="J24" s="56"/>
+      <c r="K24" s="39"/>
+      <c r="L24" s="39"/>
+      <c r="M24" s="39"/>
+      <c r="N24" s="39"/>
+      <c r="O24" s="39"/>
+      <c r="P24" s="39"/>
+      <c r="Q24" s="39"/>
+      <c r="R24" s="39"/>
+      <c r="S24" s="39"/>
+      <c r="T24" s="39"/>
+      <c r="U24" s="39"/>
+      <c r="V24" s="39"/>
+      <c r="W24" s="39"/>
+      <c r="X24" s="39"/>
+      <c r="Y24" s="39"/>
+      <c r="Z24" s="39"/>
+      <c r="AA24" s="39"/>
+      <c r="AB24" s="39"/>
+      <c r="AC24" s="39"/>
+      <c r="AD24" s="39"/>
+      <c r="AE24" s="39"/>
+      <c r="AF24" s="39"/>
+      <c r="AG24" s="39"/>
+      <c r="AH24" s="39"/>
+      <c r="AI24" s="39"/>
+      <c r="AJ24" s="39"/>
+      <c r="AK24" s="39"/>
+      <c r="AL24" s="39"/>
+      <c r="AM24" s="39"/>
+      <c r="AN24" s="39"/>
+      <c r="AO24" s="39"/>
+      <c r="AP24" s="39"/>
+      <c r="AQ24" s="39"/>
+      <c r="AR24" s="39"/>
+      <c r="AS24" s="39"/>
+      <c r="AT24" s="39"/>
+      <c r="AU24" s="39"/>
+      <c r="AV24" s="39"/>
+      <c r="AW24" s="39"/>
+      <c r="AX24" s="39"/>
+      <c r="AY24" s="39"/>
+      <c r="AZ24" s="39"/>
+      <c r="BA24" s="39"/>
+      <c r="BB24" s="39"/>
+      <c r="BC24" s="39"/>
+      <c r="BD24" s="39"/>
+      <c r="BE24" s="39"/>
+      <c r="BF24" s="39"/>
+      <c r="BG24" s="39"/>
+      <c r="BH24" s="39"/>
+      <c r="BI24" s="39"/>
+      <c r="BJ24" s="39"/>
+      <c r="BK24" s="39"/>
+      <c r="BL24" s="39"/>
+      <c r="BM24" s="39"/>
+      <c r="BN24" s="39"/>
     </row>
     <row r="25" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" s="39" t="str">
-        <f t="shared" ref="A25:A31" si="12">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>4.1</v>
+        <f t="shared" si="12"/>
+        <v>3.2</v>
       </c>
       <c r="B25" s="75" t="s">
         <v>154</v>
       </c>
       <c r="C25" s="40" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="D25" s="76"/>
       <c r="E25" s="58">
-        <f>E24</f>
+        <f>E23</f>
         <v>45215</v>
       </c>
       <c r="F25" s="59">
         <f t="shared" si="6"/>
-        <v>45216</v>
+        <v>45215</v>
       </c>
       <c r="G25" s="41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H25" s="42">
         <v>0</v>
       </c>
       <c r="I25" s="43">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J25" s="56"/>
       <c r="K25" s="39"/>
@@ -6171,17 +6171,17 @@
     <row r="26" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" s="39" t="str">
         <f t="shared" si="12"/>
-        <v>4.2</v>
+        <v>3.3</v>
       </c>
       <c r="B26" s="75" t="s">
         <v>156</v>
       </c>
       <c r="C26" s="40" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="D26" s="76"/>
       <c r="E26" s="58">
-        <f>E24</f>
+        <f>E23</f>
         <v>45215</v>
       </c>
       <c r="F26" s="59">
@@ -6259,32 +6259,32 @@
     <row r="27" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" s="39" t="str">
         <f t="shared" si="12"/>
-        <v>4.3</v>
+        <v>3.4</v>
       </c>
       <c r="B27" s="75" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C27" s="40" t="s">
-        <v>134</v>
+        <v>150</v>
       </c>
       <c r="D27" s="76"/>
       <c r="E27" s="58">
-        <f>E24</f>
-        <v>45215</v>
+        <f>F25+1</f>
+        <v>45216</v>
       </c>
       <c r="F27" s="59">
-        <f t="shared" si="6"/>
-        <v>45215</v>
+        <f>IF(ISBLANK(E27)," - ",IF(G27=0,E27,E27+G27-1))</f>
+        <v>45217</v>
       </c>
       <c r="G27" s="41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H27" s="42">
         <v>0</v>
       </c>
       <c r="I27" s="43">
-        <f t="shared" si="4"/>
-        <v>1</v>
+        <f>IF(OR(F27=0,E27=0)," - ",NETWORKDAYS(E27,F27))</f>
+        <v>2</v>
       </c>
       <c r="J27" s="56"/>
       <c r="K27" s="39"/>
@@ -6347,13 +6347,13 @@
     <row r="28" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" s="39" t="str">
         <f t="shared" si="12"/>
-        <v>4.4</v>
+        <v>3.5</v>
       </c>
       <c r="B28" s="75" t="s">
         <v>157</v>
       </c>
       <c r="C28" s="40" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D28" s="76"/>
       <c r="E28" s="58">
@@ -6361,7 +6361,7 @@
         <v>45216</v>
       </c>
       <c r="F28" s="59">
-        <f>IF(ISBLANK(E28)," - ",IF(G28=0,E28,E28+G28-1))</f>
+        <f t="shared" si="6"/>
         <v>45217</v>
       </c>
       <c r="G28" s="41">
@@ -6371,7 +6371,7 @@
         <v>0</v>
       </c>
       <c r="I28" s="43">
-        <f>IF(OR(F28=0,E28=0)," - ",NETWORKDAYS(E28,F28))</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="J28" s="56"/>
@@ -6435,22 +6435,22 @@
     <row r="29" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" s="39" t="str">
         <f t="shared" si="12"/>
-        <v>4.5</v>
+        <v>3.6</v>
       </c>
       <c r="B29" s="75" t="s">
         <v>159</v>
       </c>
       <c r="C29" s="40" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="D29" s="76"/>
       <c r="E29" s="58">
-        <f>F27+1</f>
-        <v>45216</v>
+        <f>F28+1</f>
+        <v>45218</v>
       </c>
       <c r="F29" s="59">
-        <f t="shared" si="6"/>
-        <v>45217</v>
+        <f t="shared" ref="F29" si="13">IF(ISBLANK(E29)," - ",IF(G29=0,E29,E29+G29-1))</f>
+        <v>45219</v>
       </c>
       <c r="G29" s="41">
         <v>2</v>
@@ -6459,7 +6459,7 @@
         <v>0</v>
       </c>
       <c r="I29" s="43">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="I29" si="14">IF(OR(F29=0,E29=0)," - ",NETWORKDAYS(E29,F29))</f>
         <v>2</v>
       </c>
       <c r="J29" s="56"/>
@@ -6523,32 +6523,32 @@
     <row r="30" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" s="39" t="str">
         <f t="shared" si="12"/>
-        <v>4.6</v>
+        <v>3.7</v>
       </c>
       <c r="B30" s="75" t="s">
         <v>161</v>
       </c>
       <c r="C30" s="40" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
       <c r="D30" s="76"/>
       <c r="E30" s="58">
-        <f>F29+1</f>
-        <v>45218</v>
+        <f>F23</f>
+        <v>45219</v>
       </c>
       <c r="F30" s="59">
-        <f t="shared" ref="F30" si="13">IF(ISBLANK(E30)," - ",IF(G30=0,E30,E30+G30-1))</f>
+        <f t="shared" ref="F30:F36" si="15">IF(ISBLANK(E30)," - ",IF(G30=0,E30,E30+G30-1))</f>
         <v>45219</v>
       </c>
       <c r="G30" s="41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H30" s="42">
         <v>0</v>
       </c>
       <c r="I30" s="43">
-        <f t="shared" ref="I30" si="14">IF(OR(F30=0,E30=0)," - ",NETWORKDAYS(E30,F30))</f>
-        <v>2</v>
+        <f t="shared" ref="I30:I36" si="16">IF(OR(F30=0,E30=0)," - ",NETWORKDAYS(E30,F30))</f>
+        <v>1</v>
       </c>
       <c r="J30" s="56"/>
       <c r="K30" s="39"/>
@@ -6608,196 +6608,196 @@
       <c r="BM30" s="39"/>
       <c r="BN30" s="39"/>
     </row>
-    <row r="31" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A31" s="39" t="str">
-        <f t="shared" si="12"/>
-        <v>4.7</v>
-      </c>
-      <c r="B31" s="75" t="s">
-        <v>163</v>
-      </c>
-      <c r="C31" s="40" t="s">
-        <v>134</v>
-      </c>
-      <c r="D31" s="76"/>
-      <c r="E31" s="58">
-        <f>F24</f>
-        <v>45219</v>
-      </c>
-      <c r="F31" s="59">
-        <f t="shared" ref="F31:F37" si="15">IF(ISBLANK(E31)," - ",IF(G31=0,E31,E31+G31-1))</f>
-        <v>45219</v>
-      </c>
-      <c r="G31" s="41">
-        <v>1</v>
-      </c>
-      <c r="H31" s="42">
-        <v>0</v>
-      </c>
-      <c r="I31" s="43">
-        <f t="shared" ref="I31:I37" si="16">IF(OR(F31=0,E31=0)," - ",NETWORKDAYS(E31,F31))</f>
-        <v>1</v>
-      </c>
-      <c r="J31" s="56"/>
-      <c r="K31" s="39"/>
-      <c r="L31" s="39"/>
-      <c r="M31" s="39"/>
-      <c r="N31" s="39"/>
-      <c r="O31" s="39"/>
-      <c r="P31" s="39"/>
-      <c r="Q31" s="39"/>
-      <c r="R31" s="39"/>
-      <c r="S31" s="39"/>
-      <c r="T31" s="39"/>
-      <c r="U31" s="39"/>
-      <c r="V31" s="39"/>
-      <c r="W31" s="39"/>
-      <c r="X31" s="39"/>
-      <c r="Y31" s="39"/>
-      <c r="Z31" s="39"/>
-      <c r="AA31" s="39"/>
-      <c r="AB31" s="39"/>
-      <c r="AC31" s="39"/>
-      <c r="AD31" s="39"/>
-      <c r="AE31" s="39"/>
-      <c r="AF31" s="39"/>
-      <c r="AG31" s="39"/>
-      <c r="AH31" s="39"/>
-      <c r="AI31" s="39"/>
-      <c r="AJ31" s="39"/>
-      <c r="AK31" s="39"/>
-      <c r="AL31" s="39"/>
-      <c r="AM31" s="39"/>
-      <c r="AN31" s="39"/>
-      <c r="AO31" s="39"/>
-      <c r="AP31" s="39"/>
-      <c r="AQ31" s="39"/>
-      <c r="AR31" s="39"/>
-      <c r="AS31" s="39"/>
-      <c r="AT31" s="39"/>
-      <c r="AU31" s="39"/>
-      <c r="AV31" s="39"/>
-      <c r="AW31" s="39"/>
-      <c r="AX31" s="39"/>
-      <c r="AY31" s="39"/>
-      <c r="AZ31" s="39"/>
-      <c r="BA31" s="39"/>
-      <c r="BB31" s="39"/>
-      <c r="BC31" s="39"/>
-      <c r="BD31" s="39"/>
-      <c r="BE31" s="39"/>
-      <c r="BF31" s="39"/>
-      <c r="BG31" s="39"/>
-      <c r="BH31" s="39"/>
-      <c r="BI31" s="39"/>
-      <c r="BJ31" s="39"/>
-      <c r="BK31" s="39"/>
-      <c r="BL31" s="39"/>
-      <c r="BM31" s="39"/>
-      <c r="BN31" s="39"/>
-    </row>
-    <row r="32" spans="1:66" s="34" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A32" s="32" t="str">
+    <row r="31" spans="1:66" s="34" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A31" s="32" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>5</v>
-      </c>
-      <c r="B32" s="33" t="s">
-        <v>169</v>
-      </c>
-      <c r="D32" s="35"/>
-      <c r="E32" s="60">
-        <f>F31+3</f>
+        <v>4</v>
+      </c>
+      <c r="B31" s="33" t="s">
+        <v>167</v>
+      </c>
+      <c r="D31" s="35"/>
+      <c r="E31" s="60">
+        <f>F30+3</f>
         <v>45222</v>
       </c>
-      <c r="F32" s="60">
+      <c r="F31" s="60">
         <f t="shared" si="15"/>
         <v>45226</v>
       </c>
-      <c r="G32" s="36">
+      <c r="G31" s="36">
         <v>5</v>
       </c>
-      <c r="H32" s="37"/>
-      <c r="I32" s="38">
+      <c r="H31" s="37"/>
+      <c r="I31" s="38">
         <f t="shared" si="16"/>
         <v>5</v>
       </c>
-      <c r="J32" s="57"/>
-      <c r="K32" s="63"/>
-      <c r="L32" s="63"/>
-      <c r="M32" s="63"/>
-      <c r="N32" s="63"/>
-      <c r="O32" s="63"/>
-      <c r="P32" s="63"/>
-      <c r="Q32" s="63"/>
-      <c r="R32" s="63"/>
-      <c r="S32" s="63"/>
-      <c r="T32" s="63"/>
-      <c r="U32" s="63"/>
-      <c r="V32" s="63"/>
-      <c r="W32" s="63"/>
-      <c r="X32" s="63"/>
-      <c r="Y32" s="63"/>
-      <c r="Z32" s="63"/>
-      <c r="AA32" s="63"/>
-      <c r="AB32" s="63"/>
-      <c r="AC32" s="63"/>
-      <c r="AD32" s="63"/>
-      <c r="AE32" s="63"/>
-      <c r="AF32" s="63"/>
-      <c r="AG32" s="63"/>
-      <c r="AH32" s="63"/>
-      <c r="AI32" s="63"/>
-      <c r="AJ32" s="63"/>
-      <c r="AK32" s="63"/>
-      <c r="AL32" s="63"/>
-      <c r="AM32" s="63"/>
-      <c r="AN32" s="63"/>
-      <c r="AO32" s="63"/>
-      <c r="AP32" s="63"/>
-      <c r="AQ32" s="63"/>
-      <c r="AR32" s="63"/>
-      <c r="AS32" s="63"/>
-      <c r="AT32" s="63"/>
-      <c r="AU32" s="63"/>
-      <c r="AV32" s="63"/>
-      <c r="AW32" s="63"/>
-      <c r="AX32" s="63"/>
-      <c r="AY32" s="63"/>
-      <c r="AZ32" s="63"/>
-      <c r="BA32" s="63"/>
-      <c r="BB32" s="63"/>
-      <c r="BC32" s="63"/>
-      <c r="BD32" s="63"/>
-      <c r="BE32" s="63"/>
-      <c r="BF32" s="63"/>
-      <c r="BG32" s="63"/>
-      <c r="BH32" s="63"/>
-      <c r="BI32" s="63"/>
-      <c r="BJ32" s="63"/>
-      <c r="BK32" s="63"/>
-      <c r="BL32" s="63"/>
-      <c r="BM32" s="63"/>
-      <c r="BN32" s="63"/>
+      <c r="J31" s="57"/>
+      <c r="K31" s="63"/>
+      <c r="L31" s="63"/>
+      <c r="M31" s="63"/>
+      <c r="N31" s="63"/>
+      <c r="O31" s="63"/>
+      <c r="P31" s="63"/>
+      <c r="Q31" s="63"/>
+      <c r="R31" s="63"/>
+      <c r="S31" s="63"/>
+      <c r="T31" s="63"/>
+      <c r="U31" s="63"/>
+      <c r="V31" s="63"/>
+      <c r="W31" s="63"/>
+      <c r="X31" s="63"/>
+      <c r="Y31" s="63"/>
+      <c r="Z31" s="63"/>
+      <c r="AA31" s="63"/>
+      <c r="AB31" s="63"/>
+      <c r="AC31" s="63"/>
+      <c r="AD31" s="63"/>
+      <c r="AE31" s="63"/>
+      <c r="AF31" s="63"/>
+      <c r="AG31" s="63"/>
+      <c r="AH31" s="63"/>
+      <c r="AI31" s="63"/>
+      <c r="AJ31" s="63"/>
+      <c r="AK31" s="63"/>
+      <c r="AL31" s="63"/>
+      <c r="AM31" s="63"/>
+      <c r="AN31" s="63"/>
+      <c r="AO31" s="63"/>
+      <c r="AP31" s="63"/>
+      <c r="AQ31" s="63"/>
+      <c r="AR31" s="63"/>
+      <c r="AS31" s="63"/>
+      <c r="AT31" s="63"/>
+      <c r="AU31" s="63"/>
+      <c r="AV31" s="63"/>
+      <c r="AW31" s="63"/>
+      <c r="AX31" s="63"/>
+      <c r="AY31" s="63"/>
+      <c r="AZ31" s="63"/>
+      <c r="BA31" s="63"/>
+      <c r="BB31" s="63"/>
+      <c r="BC31" s="63"/>
+      <c r="BD31" s="63"/>
+      <c r="BE31" s="63"/>
+      <c r="BF31" s="63"/>
+      <c r="BG31" s="63"/>
+      <c r="BH31" s="63"/>
+      <c r="BI31" s="63"/>
+      <c r="BJ31" s="63"/>
+      <c r="BK31" s="63"/>
+      <c r="BL31" s="63"/>
+      <c r="BM31" s="63"/>
+      <c r="BN31" s="63"/>
+    </row>
+    <row r="32" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A32" s="39" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>4.1</v>
+      </c>
+      <c r="B32" s="75" t="s">
+        <v>162</v>
+      </c>
+      <c r="C32" s="40" t="s">
+        <v>144</v>
+      </c>
+      <c r="D32" s="76"/>
+      <c r="E32" s="58">
+        <f>E31</f>
+        <v>45222</v>
+      </c>
+      <c r="F32" s="59">
+        <f t="shared" si="15"/>
+        <v>45222</v>
+      </c>
+      <c r="G32" s="41">
+        <v>1</v>
+      </c>
+      <c r="H32" s="42">
+        <v>0</v>
+      </c>
+      <c r="I32" s="43">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="J32" s="56"/>
+      <c r="K32" s="39"/>
+      <c r="L32" s="39"/>
+      <c r="M32" s="39"/>
+      <c r="N32" s="39"/>
+      <c r="O32" s="39"/>
+      <c r="P32" s="39"/>
+      <c r="Q32" s="39"/>
+      <c r="R32" s="39"/>
+      <c r="S32" s="39"/>
+      <c r="T32" s="39"/>
+      <c r="U32" s="39"/>
+      <c r="V32" s="39"/>
+      <c r="W32" s="39"/>
+      <c r="X32" s="39"/>
+      <c r="Y32" s="39"/>
+      <c r="Z32" s="39"/>
+      <c r="AA32" s="39"/>
+      <c r="AB32" s="39"/>
+      <c r="AC32" s="39"/>
+      <c r="AD32" s="39"/>
+      <c r="AE32" s="39"/>
+      <c r="AF32" s="39"/>
+      <c r="AG32" s="39"/>
+      <c r="AH32" s="39"/>
+      <c r="AI32" s="39"/>
+      <c r="AJ32" s="39"/>
+      <c r="AK32" s="39"/>
+      <c r="AL32" s="39"/>
+      <c r="AM32" s="39"/>
+      <c r="AN32" s="39"/>
+      <c r="AO32" s="39"/>
+      <c r="AP32" s="39"/>
+      <c r="AQ32" s="39"/>
+      <c r="AR32" s="39"/>
+      <c r="AS32" s="39"/>
+      <c r="AT32" s="39"/>
+      <c r="AU32" s="39"/>
+      <c r="AV32" s="39"/>
+      <c r="AW32" s="39"/>
+      <c r="AX32" s="39"/>
+      <c r="AY32" s="39"/>
+      <c r="AZ32" s="39"/>
+      <c r="BA32" s="39"/>
+      <c r="BB32" s="39"/>
+      <c r="BC32" s="39"/>
+      <c r="BD32" s="39"/>
+      <c r="BE32" s="39"/>
+      <c r="BF32" s="39"/>
+      <c r="BG32" s="39"/>
+      <c r="BH32" s="39"/>
+      <c r="BI32" s="39"/>
+      <c r="BJ32" s="39"/>
+      <c r="BK32" s="39"/>
+      <c r="BL32" s="39"/>
+      <c r="BM32" s="39"/>
+      <c r="BN32" s="39"/>
     </row>
     <row r="33" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" s="39" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>5.1</v>
+        <v>4.2</v>
       </c>
       <c r="B33" s="75" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C33" s="40" t="s">
         <v>144</v>
       </c>
       <c r="D33" s="76"/>
       <c r="E33" s="58">
-        <f>E32</f>
-        <v>45222</v>
+        <f>F32+1</f>
+        <v>45223</v>
       </c>
       <c r="F33" s="59">
         <f t="shared" si="15"/>
-        <v>45222</v>
+        <v>45223</v>
       </c>
       <c r="G33" s="41">
         <v>1</v>
@@ -6870,32 +6870,32 @@
     <row r="34" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" s="39" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>5.2</v>
+        <v>4.3</v>
       </c>
       <c r="B34" s="75" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C34" s="40" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="D34" s="76"/>
       <c r="E34" s="58">
-        <f>F33+1</f>
+        <f>F32+1</f>
         <v>45223</v>
       </c>
       <c r="F34" s="59">
         <f t="shared" si="15"/>
-        <v>45223</v>
+        <v>45224</v>
       </c>
       <c r="G34" s="41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H34" s="42">
         <v>0</v>
       </c>
       <c r="I34" s="43">
         <f t="shared" si="16"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J34" s="56"/>
       <c r="K34" s="39"/>
@@ -6958,22 +6958,22 @@
     <row r="35" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A35" s="39" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>5.3</v>
+        <v>4.4</v>
       </c>
       <c r="B35" s="75" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C35" s="40" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D35" s="76"/>
       <c r="E35" s="58">
         <f>F33+1</f>
-        <v>45223</v>
+        <v>45224</v>
       </c>
       <c r="F35" s="59">
         <f t="shared" si="15"/>
-        <v>45224</v>
+        <v>45225</v>
       </c>
       <c r="G35" s="41">
         <v>2</v>
@@ -7043,35 +7043,35 @@
       <c r="BM35" s="39"/>
       <c r="BN35" s="39"/>
     </row>
-    <row r="36" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:66" s="40" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A36" s="39" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>5.4</v>
+        <v>4.5</v>
       </c>
       <c r="B36" s="75" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C36" s="40" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D36" s="76"/>
       <c r="E36" s="58">
-        <f>F34+1</f>
-        <v>45224</v>
+        <f>F35+1</f>
+        <v>45226</v>
       </c>
       <c r="F36" s="59">
         <f t="shared" si="15"/>
-        <v>45225</v>
+        <v>45226</v>
       </c>
       <c r="G36" s="41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H36" s="42">
         <v>0</v>
       </c>
       <c r="I36" s="43">
         <f t="shared" si="16"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J36" s="56"/>
       <c r="K36" s="39"/>
@@ -7131,206 +7131,206 @@
       <c r="BM36" s="39"/>
       <c r="BN36" s="39"/>
     </row>
-    <row r="37" spans="1:66" s="40" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A37" s="39" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>5.5</v>
-      </c>
-      <c r="B37" s="75" t="s">
+    <row r="37" spans="1:66" s="34" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A37" s="32" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>5</v>
+      </c>
+      <c r="B37" s="33" t="s">
+        <v>170</v>
+      </c>
+      <c r="D37" s="35"/>
+      <c r="E37" s="60">
+        <f>F36+3</f>
+        <v>45229</v>
+      </c>
+      <c r="F37" s="60">
+        <f t="shared" ref="F37:F42" si="17">IF(ISBLANK(E37)," - ",IF(G37=0,E37,E37+G37-1))</f>
+        <v>45233</v>
+      </c>
+      <c r="G37" s="36">
+        <v>5</v>
+      </c>
+      <c r="H37" s="37"/>
+      <c r="I37" s="38">
+        <f t="shared" ref="I37:I42" si="18">IF(OR(F37=0,E37=0)," - ",NETWORKDAYS(E37,F37))</f>
+        <v>5</v>
+      </c>
+      <c r="J37" s="57"/>
+      <c r="K37" s="63"/>
+      <c r="L37" s="63"/>
+      <c r="M37" s="63"/>
+      <c r="N37" s="63"/>
+      <c r="O37" s="63"/>
+      <c r="P37" s="63"/>
+      <c r="Q37" s="63"/>
+      <c r="R37" s="63"/>
+      <c r="S37" s="63"/>
+      <c r="T37" s="63"/>
+      <c r="U37" s="63"/>
+      <c r="V37" s="63"/>
+      <c r="W37" s="63"/>
+      <c r="X37" s="63"/>
+      <c r="Y37" s="63"/>
+      <c r="Z37" s="63"/>
+      <c r="AA37" s="63"/>
+      <c r="AB37" s="63"/>
+      <c r="AC37" s="63"/>
+      <c r="AD37" s="63"/>
+      <c r="AE37" s="63"/>
+      <c r="AF37" s="63"/>
+      <c r="AG37" s="63"/>
+      <c r="AH37" s="63"/>
+      <c r="AI37" s="63"/>
+      <c r="AJ37" s="63"/>
+      <c r="AK37" s="63"/>
+      <c r="AL37" s="63"/>
+      <c r="AM37" s="63"/>
+      <c r="AN37" s="63"/>
+      <c r="AO37" s="63"/>
+      <c r="AP37" s="63"/>
+      <c r="AQ37" s="63"/>
+      <c r="AR37" s="63"/>
+      <c r="AS37" s="63"/>
+      <c r="AT37" s="63"/>
+      <c r="AU37" s="63"/>
+      <c r="AV37" s="63"/>
+      <c r="AW37" s="63"/>
+      <c r="AX37" s="63"/>
+      <c r="AY37" s="63"/>
+      <c r="AZ37" s="63"/>
+      <c r="BA37" s="63"/>
+      <c r="BB37" s="63"/>
+      <c r="BC37" s="63"/>
+      <c r="BD37" s="63"/>
+      <c r="BE37" s="63"/>
+      <c r="BF37" s="63"/>
+      <c r="BG37" s="63"/>
+      <c r="BH37" s="63"/>
+      <c r="BI37" s="63"/>
+      <c r="BJ37" s="63"/>
+      <c r="BK37" s="63"/>
+      <c r="BL37" s="63"/>
+      <c r="BM37" s="63"/>
+      <c r="BN37" s="63"/>
+    </row>
+    <row r="38" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A38" s="39" t="str">
+        <f t="shared" ref="A38:A43" si="19">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>5.1</v>
+      </c>
+      <c r="B38" s="75" t="s">
+        <v>172</v>
+      </c>
+      <c r="C38" s="40" t="s">
+        <v>144</v>
+      </c>
+      <c r="D38" s="76"/>
+      <c r="E38" s="58">
+        <f>E37</f>
+        <v>45229</v>
+      </c>
+      <c r="F38" s="59">
+        <f>IF(ISBLANK(E38)," - ",IF(G38=0,E38,E38+G38-1))</f>
+        <v>45229</v>
+      </c>
+      <c r="G38" s="41">
+        <v>1</v>
+      </c>
+      <c r="H38" s="42">
+        <v>0</v>
+      </c>
+      <c r="I38" s="43">
+        <f>IF(OR(F38=0,E38=0)," - ",NETWORKDAYS(E38,F38))</f>
+        <v>1</v>
+      </c>
+      <c r="J38" s="56"/>
+      <c r="K38" s="39"/>
+      <c r="L38" s="39"/>
+      <c r="M38" s="39"/>
+      <c r="N38" s="39"/>
+      <c r="O38" s="39"/>
+      <c r="P38" s="39"/>
+      <c r="Q38" s="39"/>
+      <c r="R38" s="39"/>
+      <c r="S38" s="39"/>
+      <c r="T38" s="39"/>
+      <c r="U38" s="39"/>
+      <c r="V38" s="39"/>
+      <c r="W38" s="39"/>
+      <c r="X38" s="39"/>
+      <c r="Y38" s="39"/>
+      <c r="Z38" s="39"/>
+      <c r="AA38" s="39"/>
+      <c r="AB38" s="39"/>
+      <c r="AC38" s="39"/>
+      <c r="AD38" s="39"/>
+      <c r="AE38" s="39"/>
+      <c r="AF38" s="39"/>
+      <c r="AG38" s="39"/>
+      <c r="AH38" s="39"/>
+      <c r="AI38" s="39"/>
+      <c r="AJ38" s="39"/>
+      <c r="AK38" s="39"/>
+      <c r="AL38" s="39"/>
+      <c r="AM38" s="39"/>
+      <c r="AN38" s="39"/>
+      <c r="AO38" s="39"/>
+      <c r="AP38" s="39"/>
+      <c r="AQ38" s="39"/>
+      <c r="AR38" s="39"/>
+      <c r="AS38" s="39"/>
+      <c r="AT38" s="39"/>
+      <c r="AU38" s="39"/>
+      <c r="AV38" s="39"/>
+      <c r="AW38" s="39"/>
+      <c r="AX38" s="39"/>
+      <c r="AY38" s="39"/>
+      <c r="AZ38" s="39"/>
+      <c r="BA38" s="39"/>
+      <c r="BB38" s="39"/>
+      <c r="BC38" s="39"/>
+      <c r="BD38" s="39"/>
+      <c r="BE38" s="39"/>
+      <c r="BF38" s="39"/>
+      <c r="BG38" s="39"/>
+      <c r="BH38" s="39"/>
+      <c r="BI38" s="39"/>
+      <c r="BJ38" s="39"/>
+      <c r="BK38" s="39"/>
+      <c r="BL38" s="39"/>
+      <c r="BM38" s="39"/>
+      <c r="BN38" s="39"/>
+    </row>
+    <row r="39" spans="1:66" s="40" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A39" s="39" t="str">
+        <f t="shared" si="19"/>
+        <v>5.2</v>
+      </c>
+      <c r="B39" s="75" t="s">
         <v>168</v>
       </c>
-      <c r="C37" s="40" t="s">
-        <v>144</v>
-      </c>
-      <c r="D37" s="76"/>
-      <c r="E37" s="58">
-        <f>F36+1</f>
-        <v>45226</v>
-      </c>
-      <c r="F37" s="59">
-        <f t="shared" si="15"/>
-        <v>45226</v>
-      </c>
-      <c r="G37" s="41">
-        <v>1</v>
-      </c>
-      <c r="H37" s="42">
-        <v>0</v>
-      </c>
-      <c r="I37" s="43">
-        <f t="shared" si="16"/>
-        <v>1</v>
-      </c>
-      <c r="J37" s="56"/>
-      <c r="K37" s="39"/>
-      <c r="L37" s="39"/>
-      <c r="M37" s="39"/>
-      <c r="N37" s="39"/>
-      <c r="O37" s="39"/>
-      <c r="P37" s="39"/>
-      <c r="Q37" s="39"/>
-      <c r="R37" s="39"/>
-      <c r="S37" s="39"/>
-      <c r="T37" s="39"/>
-      <c r="U37" s="39"/>
-      <c r="V37" s="39"/>
-      <c r="W37" s="39"/>
-      <c r="X37" s="39"/>
-      <c r="Y37" s="39"/>
-      <c r="Z37" s="39"/>
-      <c r="AA37" s="39"/>
-      <c r="AB37" s="39"/>
-      <c r="AC37" s="39"/>
-      <c r="AD37" s="39"/>
-      <c r="AE37" s="39"/>
-      <c r="AF37" s="39"/>
-      <c r="AG37" s="39"/>
-      <c r="AH37" s="39"/>
-      <c r="AI37" s="39"/>
-      <c r="AJ37" s="39"/>
-      <c r="AK37" s="39"/>
-      <c r="AL37" s="39"/>
-      <c r="AM37" s="39"/>
-      <c r="AN37" s="39"/>
-      <c r="AO37" s="39"/>
-      <c r="AP37" s="39"/>
-      <c r="AQ37" s="39"/>
-      <c r="AR37" s="39"/>
-      <c r="AS37" s="39"/>
-      <c r="AT37" s="39"/>
-      <c r="AU37" s="39"/>
-      <c r="AV37" s="39"/>
-      <c r="AW37" s="39"/>
-      <c r="AX37" s="39"/>
-      <c r="AY37" s="39"/>
-      <c r="AZ37" s="39"/>
-      <c r="BA37" s="39"/>
-      <c r="BB37" s="39"/>
-      <c r="BC37" s="39"/>
-      <c r="BD37" s="39"/>
-      <c r="BE37" s="39"/>
-      <c r="BF37" s="39"/>
-      <c r="BG37" s="39"/>
-      <c r="BH37" s="39"/>
-      <c r="BI37" s="39"/>
-      <c r="BJ37" s="39"/>
-      <c r="BK37" s="39"/>
-      <c r="BL37" s="39"/>
-      <c r="BM37" s="39"/>
-      <c r="BN37" s="39"/>
-    </row>
-    <row r="38" spans="1:66" s="34" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A38" s="32" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>6</v>
-      </c>
-      <c r="B38" s="33" t="s">
-        <v>172</v>
-      </c>
-      <c r="D38" s="35"/>
-      <c r="E38" s="60">
-        <f>F37+3</f>
-        <v>45229</v>
-      </c>
-      <c r="F38" s="60">
-        <f t="shared" ref="F38:F43" si="17">IF(ISBLANK(E38)," - ",IF(G38=0,E38,E38+G38-1))</f>
-        <v>45233</v>
-      </c>
-      <c r="G38" s="36">
-        <v>5</v>
-      </c>
-      <c r="H38" s="37"/>
-      <c r="I38" s="38">
-        <f t="shared" ref="I38:I43" si="18">IF(OR(F38=0,E38=0)," - ",NETWORKDAYS(E38,F38))</f>
-        <v>5</v>
-      </c>
-      <c r="J38" s="57"/>
-      <c r="K38" s="63"/>
-      <c r="L38" s="63"/>
-      <c r="M38" s="63"/>
-      <c r="N38" s="63"/>
-      <c r="O38" s="63"/>
-      <c r="P38" s="63"/>
-      <c r="Q38" s="63"/>
-      <c r="R38" s="63"/>
-      <c r="S38" s="63"/>
-      <c r="T38" s="63"/>
-      <c r="U38" s="63"/>
-      <c r="V38" s="63"/>
-      <c r="W38" s="63"/>
-      <c r="X38" s="63"/>
-      <c r="Y38" s="63"/>
-      <c r="Z38" s="63"/>
-      <c r="AA38" s="63"/>
-      <c r="AB38" s="63"/>
-      <c r="AC38" s="63"/>
-      <c r="AD38" s="63"/>
-      <c r="AE38" s="63"/>
-      <c r="AF38" s="63"/>
-      <c r="AG38" s="63"/>
-      <c r="AH38" s="63"/>
-      <c r="AI38" s="63"/>
-      <c r="AJ38" s="63"/>
-      <c r="AK38" s="63"/>
-      <c r="AL38" s="63"/>
-      <c r="AM38" s="63"/>
-      <c r="AN38" s="63"/>
-      <c r="AO38" s="63"/>
-      <c r="AP38" s="63"/>
-      <c r="AQ38" s="63"/>
-      <c r="AR38" s="63"/>
-      <c r="AS38" s="63"/>
-      <c r="AT38" s="63"/>
-      <c r="AU38" s="63"/>
-      <c r="AV38" s="63"/>
-      <c r="AW38" s="63"/>
-      <c r="AX38" s="63"/>
-      <c r="AY38" s="63"/>
-      <c r="AZ38" s="63"/>
-      <c r="BA38" s="63"/>
-      <c r="BB38" s="63"/>
-      <c r="BC38" s="63"/>
-      <c r="BD38" s="63"/>
-      <c r="BE38" s="63"/>
-      <c r="BF38" s="63"/>
-      <c r="BG38" s="63"/>
-      <c r="BH38" s="63"/>
-      <c r="BI38" s="63"/>
-      <c r="BJ38" s="63"/>
-      <c r="BK38" s="63"/>
-      <c r="BL38" s="63"/>
-      <c r="BM38" s="63"/>
-      <c r="BN38" s="63"/>
-    </row>
-    <row r="39" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A39" s="39" t="str">
-        <f t="shared" ref="A39:A44" si="19">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>6.1</v>
-      </c>
-      <c r="B39" s="75" t="s">
-        <v>174</v>
-      </c>
       <c r="C39" s="40" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D39" s="76"/>
       <c r="E39" s="58">
-        <f>E38</f>
+        <f>E37</f>
         <v>45229</v>
       </c>
       <c r="F39" s="59">
-        <f>IF(ISBLANK(E39)," - ",IF(G39=0,E39,E39+G39-1))</f>
-        <v>45229</v>
+        <f t="shared" si="17"/>
+        <v>45230</v>
       </c>
       <c r="G39" s="41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H39" s="42">
         <v>0</v>
       </c>
       <c r="I39" s="43">
-        <f>IF(OR(F39=0,E39=0)," - ",NETWORKDAYS(E39,F39))</f>
-        <v>1</v>
+        <f t="shared" si="18"/>
+        <v>2</v>
       </c>
       <c r="J39" s="56"/>
       <c r="K39" s="39"/>
@@ -7390,35 +7390,35 @@
       <c r="BM39" s="39"/>
       <c r="BN39" s="39"/>
     </row>
-    <row r="40" spans="1:66" s="40" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" s="39" t="str">
         <f t="shared" si="19"/>
-        <v>6.2</v>
+        <v>5.3</v>
       </c>
       <c r="B40" s="75" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C40" s="40" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="D40" s="76"/>
       <c r="E40" s="58">
-        <f>E38</f>
+        <f>E37</f>
         <v>45229</v>
       </c>
       <c r="F40" s="59">
-        <f t="shared" si="17"/>
-        <v>45230</v>
+        <f>IF(ISBLANK(E40)," - ",IF(G40=0,E40,E40+G40-1))</f>
+        <v>45231</v>
       </c>
       <c r="G40" s="41">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H40" s="42">
         <v>0</v>
       </c>
       <c r="I40" s="43">
-        <f t="shared" si="18"/>
-        <v>2</v>
+        <f>IF(OR(F40=0,E40=0)," - ",NETWORKDAYS(E40,F40))</f>
+        <v>3</v>
       </c>
       <c r="J40" s="56"/>
       <c r="K40" s="39"/>
@@ -7481,32 +7481,32 @@
     <row r="41" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A41" s="39" t="str">
         <f t="shared" si="19"/>
-        <v>6.3</v>
+        <v>5.4</v>
       </c>
       <c r="B41" s="75" t="s">
         <v>173</v>
       </c>
       <c r="C41" s="40" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D41" s="76"/>
       <c r="E41" s="58">
-        <f>E38</f>
-        <v>45229</v>
+        <f>F38+1</f>
+        <v>45230</v>
       </c>
       <c r="F41" s="59">
         <f>IF(ISBLANK(E41)," - ",IF(G41=0,E41,E41+G41-1))</f>
         <v>45231</v>
       </c>
       <c r="G41" s="41">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H41" s="42">
         <v>0</v>
       </c>
       <c r="I41" s="43">
         <f>IF(OR(F41=0,E41=0)," - ",NETWORKDAYS(E41,F41))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J41" s="56"/>
       <c r="K41" s="39"/>
@@ -7569,32 +7569,32 @@
     <row r="42" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A42" s="39" t="str">
         <f t="shared" si="19"/>
-        <v>6.4</v>
+        <v>5.5</v>
       </c>
       <c r="B42" s="75" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="C42" s="40" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="D42" s="76"/>
       <c r="E42" s="58">
         <f>F39+1</f>
-        <v>45230</v>
+        <v>45231</v>
       </c>
       <c r="F42" s="59">
-        <f>IF(ISBLANK(E42)," - ",IF(G42=0,E42,E42+G42-1))</f>
-        <v>45231</v>
+        <f t="shared" si="17"/>
+        <v>45233</v>
       </c>
       <c r="G42" s="41">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H42" s="42">
         <v>0</v>
       </c>
       <c r="I42" s="43">
-        <f>IF(OR(F42=0,E42=0)," - ",NETWORKDAYS(E42,F42))</f>
-        <v>2</v>
+        <f t="shared" si="18"/>
+        <v>3</v>
       </c>
       <c r="J42" s="56"/>
       <c r="K42" s="39"/>
@@ -7657,32 +7657,32 @@
     <row r="43" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" s="39" t="str">
         <f t="shared" si="19"/>
-        <v>6.5</v>
+        <v>5.6</v>
       </c>
       <c r="B43" s="75" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="C43" s="40" t="s">
         <v>134</v>
       </c>
       <c r="D43" s="76"/>
       <c r="E43" s="58">
-        <f>F40+1</f>
-        <v>45231</v>
+        <f>F37</f>
+        <v>45233</v>
       </c>
       <c r="F43" s="59">
-        <f t="shared" si="17"/>
+        <f t="shared" ref="F43" si="20">IF(ISBLANK(E43)," - ",IF(G43=0,E43,E43+G43-1))</f>
         <v>45233</v>
       </c>
       <c r="G43" s="41">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H43" s="42">
         <v>0</v>
       </c>
       <c r="I43" s="43">
-        <f t="shared" si="18"/>
-        <v>3</v>
+        <f t="shared" ref="I43" si="21">IF(OR(F43=0,E43=0)," - ",NETWORKDAYS(E43,F43))</f>
+        <v>1</v>
       </c>
       <c r="J43" s="56"/>
       <c r="K43" s="39"/>
@@ -7742,206 +7742,206 @@
       <c r="BM43" s="39"/>
       <c r="BN43" s="39"/>
     </row>
-    <row r="44" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A44" s="39" t="str">
-        <f t="shared" si="19"/>
-        <v>6.6</v>
-      </c>
-      <c r="B44" s="75" t="s">
-        <v>163</v>
-      </c>
-      <c r="C44" s="40" t="s">
-        <v>134</v>
-      </c>
-      <c r="D44" s="76"/>
-      <c r="E44" s="58">
-        <f>F38</f>
-        <v>45233</v>
-      </c>
-      <c r="F44" s="59">
-        <f t="shared" ref="F44" si="20">IF(ISBLANK(E44)," - ",IF(G44=0,E44,E44+G44-1))</f>
-        <v>45233</v>
-      </c>
-      <c r="G44" s="41">
-        <v>1</v>
-      </c>
-      <c r="H44" s="42">
+    <row r="44" spans="1:66" s="34" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A44" s="32" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>6</v>
+      </c>
+      <c r="B44" s="33" t="s">
+        <v>174</v>
+      </c>
+      <c r="D44" s="35"/>
+      <c r="E44" s="60">
+        <f>F37+3</f>
+        <v>45236</v>
+      </c>
+      <c r="F44" s="60">
+        <f t="shared" ref="F44" si="22">IF(ISBLANK(E44)," - ",IF(G44=0,E44,E44+G44-1))</f>
+        <v>45240</v>
+      </c>
+      <c r="G44" s="36">
+        <v>5</v>
+      </c>
+      <c r="H44" s="37"/>
+      <c r="I44" s="38">
+        <f t="shared" ref="I44" si="23">IF(OR(F44=0,E44=0)," - ",NETWORKDAYS(E44,F44))</f>
+        <v>5</v>
+      </c>
+      <c r="J44" s="57"/>
+      <c r="K44" s="63"/>
+      <c r="L44" s="63"/>
+      <c r="M44" s="63"/>
+      <c r="N44" s="63"/>
+      <c r="O44" s="63"/>
+      <c r="P44" s="63"/>
+      <c r="Q44" s="63"/>
+      <c r="R44" s="63"/>
+      <c r="S44" s="63"/>
+      <c r="T44" s="63"/>
+      <c r="U44" s="63"/>
+      <c r="V44" s="63"/>
+      <c r="W44" s="63"/>
+      <c r="X44" s="63"/>
+      <c r="Y44" s="63"/>
+      <c r="Z44" s="63"/>
+      <c r="AA44" s="63"/>
+      <c r="AB44" s="63"/>
+      <c r="AC44" s="63"/>
+      <c r="AD44" s="63"/>
+      <c r="AE44" s="63"/>
+      <c r="AF44" s="63"/>
+      <c r="AG44" s="63"/>
+      <c r="AH44" s="63"/>
+      <c r="AI44" s="63"/>
+      <c r="AJ44" s="63"/>
+      <c r="AK44" s="63"/>
+      <c r="AL44" s="63"/>
+      <c r="AM44" s="63"/>
+      <c r="AN44" s="63"/>
+      <c r="AO44" s="63"/>
+      <c r="AP44" s="63"/>
+      <c r="AQ44" s="63"/>
+      <c r="AR44" s="63"/>
+      <c r="AS44" s="63"/>
+      <c r="AT44" s="63"/>
+      <c r="AU44" s="63"/>
+      <c r="AV44" s="63"/>
+      <c r="AW44" s="63"/>
+      <c r="AX44" s="63"/>
+      <c r="AY44" s="63"/>
+      <c r="AZ44" s="63"/>
+      <c r="BA44" s="63"/>
+      <c r="BB44" s="63"/>
+      <c r="BC44" s="63"/>
+      <c r="BD44" s="63"/>
+      <c r="BE44" s="63"/>
+      <c r="BF44" s="63"/>
+      <c r="BG44" s="63"/>
+      <c r="BH44" s="63"/>
+      <c r="BI44" s="63"/>
+      <c r="BJ44" s="63"/>
+      <c r="BK44" s="63"/>
+      <c r="BL44" s="63"/>
+      <c r="BM44" s="63"/>
+      <c r="BN44" s="63"/>
+    </row>
+    <row r="45" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A45" s="39" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>6.1</v>
+      </c>
+      <c r="B45" s="75" t="s">
+        <v>175</v>
+      </c>
+      <c r="C45" s="40" t="s">
+        <v>144</v>
+      </c>
+      <c r="D45" s="76"/>
+      <c r="E45" s="58">
+        <f>E44</f>
+        <v>45236</v>
+      </c>
+      <c r="F45" s="59">
+        <f>IF(ISBLANK(E45)," - ",IF(G45=0,E45,E45+G45-1))</f>
+        <v>45238</v>
+      </c>
+      <c r="G45" s="41">
+        <v>3</v>
+      </c>
+      <c r="H45" s="42">
         <v>0</v>
       </c>
-      <c r="I44" s="43">
-        <f t="shared" ref="I44" si="21">IF(OR(F44=0,E44=0)," - ",NETWORKDAYS(E44,F44))</f>
-        <v>1</v>
-      </c>
-      <c r="J44" s="56"/>
-      <c r="K44" s="39"/>
-      <c r="L44" s="39"/>
-      <c r="M44" s="39"/>
-      <c r="N44" s="39"/>
-      <c r="O44" s="39"/>
-      <c r="P44" s="39"/>
-      <c r="Q44" s="39"/>
-      <c r="R44" s="39"/>
-      <c r="S44" s="39"/>
-      <c r="T44" s="39"/>
-      <c r="U44" s="39"/>
-      <c r="V44" s="39"/>
-      <c r="W44" s="39"/>
-      <c r="X44" s="39"/>
-      <c r="Y44" s="39"/>
-      <c r="Z44" s="39"/>
-      <c r="AA44" s="39"/>
-      <c r="AB44" s="39"/>
-      <c r="AC44" s="39"/>
-      <c r="AD44" s="39"/>
-      <c r="AE44" s="39"/>
-      <c r="AF44" s="39"/>
-      <c r="AG44" s="39"/>
-      <c r="AH44" s="39"/>
-      <c r="AI44" s="39"/>
-      <c r="AJ44" s="39"/>
-      <c r="AK44" s="39"/>
-      <c r="AL44" s="39"/>
-      <c r="AM44" s="39"/>
-      <c r="AN44" s="39"/>
-      <c r="AO44" s="39"/>
-      <c r="AP44" s="39"/>
-      <c r="AQ44" s="39"/>
-      <c r="AR44" s="39"/>
-      <c r="AS44" s="39"/>
-      <c r="AT44" s="39"/>
-      <c r="AU44" s="39"/>
-      <c r="AV44" s="39"/>
-      <c r="AW44" s="39"/>
-      <c r="AX44" s="39"/>
-      <c r="AY44" s="39"/>
-      <c r="AZ44" s="39"/>
-      <c r="BA44" s="39"/>
-      <c r="BB44" s="39"/>
-      <c r="BC44" s="39"/>
-      <c r="BD44" s="39"/>
-      <c r="BE44" s="39"/>
-      <c r="BF44" s="39"/>
-      <c r="BG44" s="39"/>
-      <c r="BH44" s="39"/>
-      <c r="BI44" s="39"/>
-      <c r="BJ44" s="39"/>
-      <c r="BK44" s="39"/>
-      <c r="BL44" s="39"/>
-      <c r="BM44" s="39"/>
-      <c r="BN44" s="39"/>
-    </row>
-    <row r="45" spans="1:66" s="34" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A45" s="32" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>7</v>
-      </c>
-      <c r="B45" s="33" t="s">
-        <v>176</v>
-      </c>
-      <c r="D45" s="35"/>
-      <c r="E45" s="60">
-        <f>F38+3</f>
-        <v>45236</v>
-      </c>
-      <c r="F45" s="60">
-        <f t="shared" ref="F45" si="22">IF(ISBLANK(E45)," - ",IF(G45=0,E45,E45+G45-1))</f>
-        <v>45240</v>
-      </c>
-      <c r="G45" s="36">
-        <v>5</v>
-      </c>
-      <c r="H45" s="37"/>
-      <c r="I45" s="38">
-        <f t="shared" ref="I45" si="23">IF(OR(F45=0,E45=0)," - ",NETWORKDAYS(E45,F45))</f>
-        <v>5</v>
-      </c>
-      <c r="J45" s="57"/>
-      <c r="K45" s="63"/>
-      <c r="L45" s="63"/>
-      <c r="M45" s="63"/>
-      <c r="N45" s="63"/>
-      <c r="O45" s="63"/>
-      <c r="P45" s="63"/>
-      <c r="Q45" s="63"/>
-      <c r="R45" s="63"/>
-      <c r="S45" s="63"/>
-      <c r="T45" s="63"/>
-      <c r="U45" s="63"/>
-      <c r="V45" s="63"/>
-      <c r="W45" s="63"/>
-      <c r="X45" s="63"/>
-      <c r="Y45" s="63"/>
-      <c r="Z45" s="63"/>
-      <c r="AA45" s="63"/>
-      <c r="AB45" s="63"/>
-      <c r="AC45" s="63"/>
-      <c r="AD45" s="63"/>
-      <c r="AE45" s="63"/>
-      <c r="AF45" s="63"/>
-      <c r="AG45" s="63"/>
-      <c r="AH45" s="63"/>
-      <c r="AI45" s="63"/>
-      <c r="AJ45" s="63"/>
-      <c r="AK45" s="63"/>
-      <c r="AL45" s="63"/>
-      <c r="AM45" s="63"/>
-      <c r="AN45" s="63"/>
-      <c r="AO45" s="63"/>
-      <c r="AP45" s="63"/>
-      <c r="AQ45" s="63"/>
-      <c r="AR45" s="63"/>
-      <c r="AS45" s="63"/>
-      <c r="AT45" s="63"/>
-      <c r="AU45" s="63"/>
-      <c r="AV45" s="63"/>
-      <c r="AW45" s="63"/>
-      <c r="AX45" s="63"/>
-      <c r="AY45" s="63"/>
-      <c r="AZ45" s="63"/>
-      <c r="BA45" s="63"/>
-      <c r="BB45" s="63"/>
-      <c r="BC45" s="63"/>
-      <c r="BD45" s="63"/>
-      <c r="BE45" s="63"/>
-      <c r="BF45" s="63"/>
-      <c r="BG45" s="63"/>
-      <c r="BH45" s="63"/>
-      <c r="BI45" s="63"/>
-      <c r="BJ45" s="63"/>
-      <c r="BK45" s="63"/>
-      <c r="BL45" s="63"/>
-      <c r="BM45" s="63"/>
-      <c r="BN45" s="63"/>
-    </row>
-    <row r="46" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="I45" s="43">
+        <f>IF(OR(F45=0,E45=0)," - ",NETWORKDAYS(E45,F45))</f>
+        <v>3</v>
+      </c>
+      <c r="J45" s="56"/>
+      <c r="K45" s="39"/>
+      <c r="L45" s="39"/>
+      <c r="M45" s="39"/>
+      <c r="N45" s="39"/>
+      <c r="O45" s="39"/>
+      <c r="P45" s="39"/>
+      <c r="Q45" s="39"/>
+      <c r="R45" s="39"/>
+      <c r="S45" s="39"/>
+      <c r="T45" s="39"/>
+      <c r="U45" s="39"/>
+      <c r="V45" s="39"/>
+      <c r="W45" s="39"/>
+      <c r="X45" s="39"/>
+      <c r="Y45" s="39"/>
+      <c r="Z45" s="39"/>
+      <c r="AA45" s="39"/>
+      <c r="AB45" s="39"/>
+      <c r="AC45" s="39"/>
+      <c r="AD45" s="39"/>
+      <c r="AE45" s="39"/>
+      <c r="AF45" s="39"/>
+      <c r="AG45" s="39"/>
+      <c r="AH45" s="39"/>
+      <c r="AI45" s="39"/>
+      <c r="AJ45" s="39"/>
+      <c r="AK45" s="39"/>
+      <c r="AL45" s="39"/>
+      <c r="AM45" s="39"/>
+      <c r="AN45" s="39"/>
+      <c r="AO45" s="39"/>
+      <c r="AP45" s="39"/>
+      <c r="AQ45" s="39"/>
+      <c r="AR45" s="39"/>
+      <c r="AS45" s="39"/>
+      <c r="AT45" s="39"/>
+      <c r="AU45" s="39"/>
+      <c r="AV45" s="39"/>
+      <c r="AW45" s="39"/>
+      <c r="AX45" s="39"/>
+      <c r="AY45" s="39"/>
+      <c r="AZ45" s="39"/>
+      <c r="BA45" s="39"/>
+      <c r="BB45" s="39"/>
+      <c r="BC45" s="39"/>
+      <c r="BD45" s="39"/>
+      <c r="BE45" s="39"/>
+      <c r="BF45" s="39"/>
+      <c r="BG45" s="39"/>
+      <c r="BH45" s="39"/>
+      <c r="BI45" s="39"/>
+      <c r="BJ45" s="39"/>
+      <c r="BK45" s="39"/>
+      <c r="BL45" s="39"/>
+      <c r="BM45" s="39"/>
+      <c r="BN45" s="39"/>
+    </row>
+    <row r="46" spans="1:66" s="40" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A46" s="39" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>7.1</v>
+        <v>6.2</v>
       </c>
       <c r="B46" s="75" t="s">
+        <v>176</v>
+      </c>
+      <c r="C46" s="40" t="s">
         <v>177</v>
-      </c>
-      <c r="C46" s="40" t="s">
-        <v>144</v>
       </c>
       <c r="D46" s="76"/>
       <c r="E46" s="58">
-        <f>E45</f>
-        <v>45236</v>
+        <f>E45+1</f>
+        <v>45237</v>
       </c>
       <c r="F46" s="59">
-        <f>IF(ISBLANK(E46)," - ",IF(G46=0,E46,E46+G46-1))</f>
-        <v>45238</v>
+        <f t="shared" ref="F46" si="24">IF(ISBLANK(E46)," - ",IF(G46=0,E46,E46+G46-1))</f>
+        <v>45240</v>
       </c>
       <c r="G46" s="41">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H46" s="42">
         <v>0</v>
       </c>
       <c r="I46" s="43">
-        <f>IF(OR(F46=0,E46=0)," - ",NETWORKDAYS(E46,F46))</f>
-        <v>3</v>
+        <f t="shared" ref="I46" si="25">IF(OR(F46=0,E46=0)," - ",NETWORKDAYS(E46,F46))</f>
+        <v>4</v>
       </c>
       <c r="J46" s="56"/>
       <c r="K46" s="39"/>
@@ -8001,35 +8001,35 @@
       <c r="BM46" s="39"/>
       <c r="BN46" s="39"/>
     </row>
-    <row r="47" spans="1:66" s="40" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" s="39" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>7.2</v>
+        <v>6.3</v>
       </c>
       <c r="B47" s="75" t="s">
         <v>178</v>
       </c>
       <c r="C47" s="40" t="s">
-        <v>179</v>
+        <v>153</v>
       </c>
       <c r="D47" s="76"/>
       <c r="E47" s="58">
-        <f>E46+1</f>
-        <v>45237</v>
+        <f>E44</f>
+        <v>45236</v>
       </c>
       <c r="F47" s="59">
-        <f t="shared" ref="F47" si="24">IF(ISBLANK(E47)," - ",IF(G47=0,E47,E47+G47-1))</f>
-        <v>45240</v>
+        <f>IF(ISBLANK(E47)," - ",IF(G47=0,E47,E47+G47-1))</f>
+        <v>45238</v>
       </c>
       <c r="G47" s="41">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H47" s="42">
         <v>0</v>
       </c>
       <c r="I47" s="43">
-        <f t="shared" ref="I47" si="25">IF(OR(F47=0,E47=0)," - ",NETWORKDAYS(E47,F47))</f>
-        <v>4</v>
+        <f>IF(OR(F47=0,E47=0)," - ",NETWORKDAYS(E47,F47))</f>
+        <v>3</v>
       </c>
       <c r="J47" s="56"/>
       <c r="K47" s="39"/>
@@ -8092,32 +8092,32 @@
     <row r="48" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A48" s="39" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>7.3</v>
+        <v>6.4</v>
       </c>
       <c r="B48" s="75" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C48" s="40" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D48" s="76"/>
       <c r="E48" s="58">
-        <f>E45</f>
-        <v>45236</v>
+        <f>F47+1</f>
+        <v>45239</v>
       </c>
       <c r="F48" s="59">
         <f>IF(ISBLANK(E48)," - ",IF(G48=0,E48,E48+G48-1))</f>
-        <v>45238</v>
+        <v>45240</v>
       </c>
       <c r="G48" s="41">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H48" s="42">
         <v>0</v>
       </c>
       <c r="I48" s="43">
         <f>IF(OR(F48=0,E48=0)," - ",NETWORKDAYS(E48,F48))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J48" s="56"/>
       <c r="K48" s="39"/>
@@ -8177,195 +8177,195 @@
       <c r="BM48" s="39"/>
       <c r="BN48" s="39"/>
     </row>
-    <row r="49" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A49" s="39" t="str">
+    <row r="49" spans="1:66" s="34" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A49" s="32" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>7</v>
+      </c>
+      <c r="B49" s="33" t="s">
+        <v>182</v>
+      </c>
+      <c r="D49" s="35"/>
+      <c r="E49" s="60">
+        <f>F48+3</f>
+        <v>45243</v>
+      </c>
+      <c r="F49" s="60">
+        <f t="shared" ref="F49" si="26">IF(ISBLANK(E49)," - ",IF(G49=0,E49,E49+G49-1))</f>
+        <v>45247</v>
+      </c>
+      <c r="G49" s="36">
+        <v>5</v>
+      </c>
+      <c r="H49" s="37"/>
+      <c r="I49" s="38">
+        <f t="shared" ref="I49" si="27">IF(OR(F49=0,E49=0)," - ",NETWORKDAYS(E49,F49))</f>
+        <v>5</v>
+      </c>
+      <c r="J49" s="57"/>
+      <c r="K49" s="63"/>
+      <c r="L49" s="63"/>
+      <c r="M49" s="63"/>
+      <c r="N49" s="63"/>
+      <c r="O49" s="63"/>
+      <c r="P49" s="63"/>
+      <c r="Q49" s="63"/>
+      <c r="R49" s="63"/>
+      <c r="S49" s="63"/>
+      <c r="T49" s="63"/>
+      <c r="U49" s="63"/>
+      <c r="V49" s="63"/>
+      <c r="W49" s="63"/>
+      <c r="X49" s="63"/>
+      <c r="Y49" s="63"/>
+      <c r="Z49" s="63"/>
+      <c r="AA49" s="63"/>
+      <c r="AB49" s="63"/>
+      <c r="AC49" s="63"/>
+      <c r="AD49" s="63"/>
+      <c r="AE49" s="63"/>
+      <c r="AF49" s="63"/>
+      <c r="AG49" s="63"/>
+      <c r="AH49" s="63"/>
+      <c r="AI49" s="63"/>
+      <c r="AJ49" s="63"/>
+      <c r="AK49" s="63"/>
+      <c r="AL49" s="63"/>
+      <c r="AM49" s="63"/>
+      <c r="AN49" s="63"/>
+      <c r="AO49" s="63"/>
+      <c r="AP49" s="63"/>
+      <c r="AQ49" s="63"/>
+      <c r="AR49" s="63"/>
+      <c r="AS49" s="63"/>
+      <c r="AT49" s="63"/>
+      <c r="AU49" s="63"/>
+      <c r="AV49" s="63"/>
+      <c r="AW49" s="63"/>
+      <c r="AX49" s="63"/>
+      <c r="AY49" s="63"/>
+      <c r="AZ49" s="63"/>
+      <c r="BA49" s="63"/>
+      <c r="BB49" s="63"/>
+      <c r="BC49" s="63"/>
+      <c r="BD49" s="63"/>
+      <c r="BE49" s="63"/>
+      <c r="BF49" s="63"/>
+      <c r="BG49" s="63"/>
+      <c r="BH49" s="63"/>
+      <c r="BI49" s="63"/>
+      <c r="BJ49" s="63"/>
+      <c r="BK49" s="63"/>
+      <c r="BL49" s="63"/>
+      <c r="BM49" s="63"/>
+      <c r="BN49" s="63"/>
+    </row>
+    <row r="50" spans="1:66" s="40" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A50" s="39" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>7.4</v>
-      </c>
-      <c r="B49" s="75" t="s">
-        <v>181</v>
-      </c>
-      <c r="C49" s="40" t="s">
-        <v>155</v>
-      </c>
-      <c r="D49" s="76"/>
-      <c r="E49" s="58">
-        <f>F48+1</f>
-        <v>45239</v>
-      </c>
-      <c r="F49" s="59">
-        <f>IF(ISBLANK(E49)," - ",IF(G49=0,E49,E49+G49-1))</f>
-        <v>45240</v>
-      </c>
-      <c r="G49" s="41">
-        <v>2</v>
-      </c>
-      <c r="H49" s="42">
+        <v>7.1</v>
+      </c>
+      <c r="B50" s="75" t="s">
+        <v>180</v>
+      </c>
+      <c r="C50" s="40" t="s">
+        <v>153</v>
+      </c>
+      <c r="D50" s="76"/>
+      <c r="E50" s="58">
+        <f>E49</f>
+        <v>45243</v>
+      </c>
+      <c r="F50" s="59">
+        <f>IF(ISBLANK(E50)," - ",IF(G50=0,E50,E50+G50-1))</f>
+        <v>45245</v>
+      </c>
+      <c r="G50" s="41">
+        <v>3</v>
+      </c>
+      <c r="H50" s="42">
         <v>0</v>
       </c>
-      <c r="I49" s="43">
-        <f>IF(OR(F49=0,E49=0)," - ",NETWORKDAYS(E49,F49))</f>
-        <v>2</v>
-      </c>
-      <c r="J49" s="56"/>
-      <c r="K49" s="39"/>
-      <c r="L49" s="39"/>
-      <c r="M49" s="39"/>
-      <c r="N49" s="39"/>
-      <c r="O49" s="39"/>
-      <c r="P49" s="39"/>
-      <c r="Q49" s="39"/>
-      <c r="R49" s="39"/>
-      <c r="S49" s="39"/>
-      <c r="T49" s="39"/>
-      <c r="U49" s="39"/>
-      <c r="V49" s="39"/>
-      <c r="W49" s="39"/>
-      <c r="X49" s="39"/>
-      <c r="Y49" s="39"/>
-      <c r="Z49" s="39"/>
-      <c r="AA49" s="39"/>
-      <c r="AB49" s="39"/>
-      <c r="AC49" s="39"/>
-      <c r="AD49" s="39"/>
-      <c r="AE49" s="39"/>
-      <c r="AF49" s="39"/>
-      <c r="AG49" s="39"/>
-      <c r="AH49" s="39"/>
-      <c r="AI49" s="39"/>
-      <c r="AJ49" s="39"/>
-      <c r="AK49" s="39"/>
-      <c r="AL49" s="39"/>
-      <c r="AM49" s="39"/>
-      <c r="AN49" s="39"/>
-      <c r="AO49" s="39"/>
-      <c r="AP49" s="39"/>
-      <c r="AQ49" s="39"/>
-      <c r="AR49" s="39"/>
-      <c r="AS49" s="39"/>
-      <c r="AT49" s="39"/>
-      <c r="AU49" s="39"/>
-      <c r="AV49" s="39"/>
-      <c r="AW49" s="39"/>
-      <c r="AX49" s="39"/>
-      <c r="AY49" s="39"/>
-      <c r="AZ49" s="39"/>
-      <c r="BA49" s="39"/>
-      <c r="BB49" s="39"/>
-      <c r="BC49" s="39"/>
-      <c r="BD49" s="39"/>
-      <c r="BE49" s="39"/>
-      <c r="BF49" s="39"/>
-      <c r="BG49" s="39"/>
-      <c r="BH49" s="39"/>
-      <c r="BI49" s="39"/>
-      <c r="BJ49" s="39"/>
-      <c r="BK49" s="39"/>
-      <c r="BL49" s="39"/>
-      <c r="BM49" s="39"/>
-      <c r="BN49" s="39"/>
-    </row>
-    <row r="50" spans="1:66" s="34" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A50" s="32" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>8</v>
-      </c>
-      <c r="B50" s="33" t="s">
-        <v>184</v>
-      </c>
-      <c r="D50" s="35"/>
-      <c r="E50" s="60">
-        <f>F49+3</f>
-        <v>45243</v>
-      </c>
-      <c r="F50" s="60">
-        <f t="shared" ref="F50" si="26">IF(ISBLANK(E50)," - ",IF(G50=0,E50,E50+G50-1))</f>
-        <v>45247</v>
-      </c>
-      <c r="G50" s="36">
-        <v>5</v>
-      </c>
-      <c r="H50" s="37"/>
-      <c r="I50" s="38">
-        <f t="shared" ref="I50" si="27">IF(OR(F50=0,E50=0)," - ",NETWORKDAYS(E50,F50))</f>
-        <v>5</v>
-      </c>
-      <c r="J50" s="57"/>
-      <c r="K50" s="63"/>
-      <c r="L50" s="63"/>
-      <c r="M50" s="63"/>
-      <c r="N50" s="63"/>
-      <c r="O50" s="63"/>
-      <c r="P50" s="63"/>
-      <c r="Q50" s="63"/>
-      <c r="R50" s="63"/>
-      <c r="S50" s="63"/>
-      <c r="T50" s="63"/>
-      <c r="U50" s="63"/>
-      <c r="V50" s="63"/>
-      <c r="W50" s="63"/>
-      <c r="X50" s="63"/>
-      <c r="Y50" s="63"/>
-      <c r="Z50" s="63"/>
-      <c r="AA50" s="63"/>
-      <c r="AB50" s="63"/>
-      <c r="AC50" s="63"/>
-      <c r="AD50" s="63"/>
-      <c r="AE50" s="63"/>
-      <c r="AF50" s="63"/>
-      <c r="AG50" s="63"/>
-      <c r="AH50" s="63"/>
-      <c r="AI50" s="63"/>
-      <c r="AJ50" s="63"/>
-      <c r="AK50" s="63"/>
-      <c r="AL50" s="63"/>
-      <c r="AM50" s="63"/>
-      <c r="AN50" s="63"/>
-      <c r="AO50" s="63"/>
-      <c r="AP50" s="63"/>
-      <c r="AQ50" s="63"/>
-      <c r="AR50" s="63"/>
-      <c r="AS50" s="63"/>
-      <c r="AT50" s="63"/>
-      <c r="AU50" s="63"/>
-      <c r="AV50" s="63"/>
-      <c r="AW50" s="63"/>
-      <c r="AX50" s="63"/>
-      <c r="AY50" s="63"/>
-      <c r="AZ50" s="63"/>
-      <c r="BA50" s="63"/>
-      <c r="BB50" s="63"/>
-      <c r="BC50" s="63"/>
-      <c r="BD50" s="63"/>
-      <c r="BE50" s="63"/>
-      <c r="BF50" s="63"/>
-      <c r="BG50" s="63"/>
-      <c r="BH50" s="63"/>
-      <c r="BI50" s="63"/>
-      <c r="BJ50" s="63"/>
-      <c r="BK50" s="63"/>
-      <c r="BL50" s="63"/>
-      <c r="BM50" s="63"/>
-      <c r="BN50" s="63"/>
+      <c r="I50" s="43">
+        <f>IF(OR(F50=0,E50=0)," - ",NETWORKDAYS(E50,F50))</f>
+        <v>3</v>
+      </c>
+      <c r="J50" s="56"/>
+      <c r="K50" s="39"/>
+      <c r="L50" s="39"/>
+      <c r="M50" s="39"/>
+      <c r="N50" s="39"/>
+      <c r="O50" s="39"/>
+      <c r="P50" s="39"/>
+      <c r="Q50" s="39"/>
+      <c r="R50" s="39"/>
+      <c r="S50" s="39"/>
+      <c r="T50" s="39"/>
+      <c r="U50" s="39"/>
+      <c r="V50" s="39"/>
+      <c r="W50" s="39"/>
+      <c r="X50" s="39"/>
+      <c r="Y50" s="39"/>
+      <c r="Z50" s="39"/>
+      <c r="AA50" s="39"/>
+      <c r="AB50" s="39"/>
+      <c r="AC50" s="39"/>
+      <c r="AD50" s="39"/>
+      <c r="AE50" s="39"/>
+      <c r="AF50" s="39"/>
+      <c r="AG50" s="39"/>
+      <c r="AH50" s="39"/>
+      <c r="AI50" s="39"/>
+      <c r="AJ50" s="39"/>
+      <c r="AK50" s="39"/>
+      <c r="AL50" s="39"/>
+      <c r="AM50" s="39"/>
+      <c r="AN50" s="39"/>
+      <c r="AO50" s="39"/>
+      <c r="AP50" s="39"/>
+      <c r="AQ50" s="39"/>
+      <c r="AR50" s="39"/>
+      <c r="AS50" s="39"/>
+      <c r="AT50" s="39"/>
+      <c r="AU50" s="39"/>
+      <c r="AV50" s="39"/>
+      <c r="AW50" s="39"/>
+      <c r="AX50" s="39"/>
+      <c r="AY50" s="39"/>
+      <c r="AZ50" s="39"/>
+      <c r="BA50" s="39"/>
+      <c r="BB50" s="39"/>
+      <c r="BC50" s="39"/>
+      <c r="BD50" s="39"/>
+      <c r="BE50" s="39"/>
+      <c r="BF50" s="39"/>
+      <c r="BG50" s="39"/>
+      <c r="BH50" s="39"/>
+      <c r="BI50" s="39"/>
+      <c r="BJ50" s="39"/>
+      <c r="BK50" s="39"/>
+      <c r="BL50" s="39"/>
+      <c r="BM50" s="39"/>
+      <c r="BN50" s="39"/>
     </row>
     <row r="51" spans="1:66" s="40" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A51" s="39" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>8.1</v>
+        <v>7.2</v>
       </c>
       <c r="B51" s="75" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C51" s="40" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
       <c r="D51" s="76"/>
       <c r="E51" s="58">
-        <f>E50</f>
+        <f>E49</f>
         <v>45243</v>
       </c>
       <c r="F51" s="59">
-        <f>IF(ISBLANK(E51)," - ",IF(G51=0,E51,E51+G51-1))</f>
+        <f t="shared" ref="F51" si="28">IF(ISBLANK(E51)," - ",IF(G51=0,E51,E51+G51-1))</f>
         <v>45245</v>
       </c>
       <c r="G51" s="41">
@@ -8375,7 +8375,7 @@
         <v>0</v>
       </c>
       <c r="I51" s="43">
-        <f>IF(OR(F51=0,E51=0)," - ",NETWORKDAYS(E51,F51))</f>
+        <f t="shared" ref="I51" si="29">IF(OR(F51=0,E51=0)," - ",NETWORKDAYS(E51,F51))</f>
         <v>3</v>
       </c>
       <c r="J51" s="56"/>
@@ -8436,10 +8436,10 @@
       <c r="BM51" s="39"/>
       <c r="BN51" s="39"/>
     </row>
-    <row r="52" spans="1:66" s="40" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A52" s="39" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>8.2</v>
+        <v>7.3</v>
       </c>
       <c r="B52" s="75" t="s">
         <v>183</v>
@@ -8449,22 +8449,22 @@
       </c>
       <c r="D52" s="76"/>
       <c r="E52" s="58">
-        <f>E50</f>
-        <v>45243</v>
+        <f>F51+1</f>
+        <v>45246</v>
       </c>
       <c r="F52" s="59">
-        <f t="shared" ref="F52" si="28">IF(ISBLANK(E52)," - ",IF(G52=0,E52,E52+G52-1))</f>
-        <v>45245</v>
+        <f>IF(ISBLANK(E52)," - ",IF(G52=0,E52,E52+G52-1))</f>
+        <v>45246</v>
       </c>
       <c r="G52" s="41">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H52" s="42">
         <v>0</v>
       </c>
       <c r="I52" s="43">
-        <f t="shared" ref="I52" si="29">IF(OR(F52=0,E52=0)," - ",NETWORKDAYS(E52,F52))</f>
-        <v>3</v>
+        <f>IF(OR(F52=0,E52=0)," - ",NETWORKDAYS(E52,F52))</f>
+        <v>1</v>
       </c>
       <c r="J52" s="56"/>
       <c r="K52" s="39"/>
@@ -8527,10 +8527,10 @@
     <row r="53" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A53" s="39" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>8.3</v>
+        <v>7.4</v>
       </c>
       <c r="B53" s="75" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C53" s="40" t="s">
         <v>134</v>
@@ -8538,11 +8538,11 @@
       <c r="D53" s="76"/>
       <c r="E53" s="58">
         <f>F52+1</f>
-        <v>45246</v>
+        <v>45247</v>
       </c>
       <c r="F53" s="59">
         <f>IF(ISBLANK(E53)," - ",IF(G53=0,E53,E53+G53-1))</f>
-        <v>45246</v>
+        <v>45247</v>
       </c>
       <c r="G53" s="41">
         <v>1</v>
@@ -8612,97 +8612,18 @@
       <c r="BM53" s="39"/>
       <c r="BN53" s="39"/>
     </row>
-    <row r="54" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A54" s="39" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>8.4</v>
-      </c>
-      <c r="B54" s="75" t="s">
-        <v>186</v>
-      </c>
-      <c r="C54" s="40" t="s">
-        <v>134</v>
-      </c>
-      <c r="D54" s="76"/>
-      <c r="E54" s="58">
-        <f>F53+1</f>
-        <v>45247</v>
-      </c>
-      <c r="F54" s="59">
-        <f>IF(ISBLANK(E54)," - ",IF(G54=0,E54,E54+G54-1))</f>
-        <v>45247</v>
-      </c>
-      <c r="G54" s="41">
-        <v>1</v>
-      </c>
-      <c r="H54" s="42">
-        <v>0</v>
-      </c>
-      <c r="I54" s="43">
-        <f>IF(OR(F54=0,E54=0)," - ",NETWORKDAYS(E54,F54))</f>
-        <v>1</v>
-      </c>
-      <c r="J54" s="56"/>
-      <c r="K54" s="39"/>
-      <c r="L54" s="39"/>
-      <c r="M54" s="39"/>
-      <c r="N54" s="39"/>
-      <c r="O54" s="39"/>
-      <c r="P54" s="39"/>
-      <c r="Q54" s="39"/>
-      <c r="R54" s="39"/>
-      <c r="S54" s="39"/>
-      <c r="T54" s="39"/>
-      <c r="U54" s="39"/>
-      <c r="V54" s="39"/>
-      <c r="W54" s="39"/>
-      <c r="X54" s="39"/>
-      <c r="Y54" s="39"/>
-      <c r="Z54" s="39"/>
-      <c r="AA54" s="39"/>
-      <c r="AB54" s="39"/>
-      <c r="AC54" s="39"/>
-      <c r="AD54" s="39"/>
-      <c r="AE54" s="39"/>
-      <c r="AF54" s="39"/>
-      <c r="AG54" s="39"/>
-      <c r="AH54" s="39"/>
-      <c r="AI54" s="39"/>
-      <c r="AJ54" s="39"/>
-      <c r="AK54" s="39"/>
-      <c r="AL54" s="39"/>
-      <c r="AM54" s="39"/>
-      <c r="AN54" s="39"/>
-      <c r="AO54" s="39"/>
-      <c r="AP54" s="39"/>
-      <c r="AQ54" s="39"/>
-      <c r="AR54" s="39"/>
-      <c r="AS54" s="39"/>
-      <c r="AT54" s="39"/>
-      <c r="AU54" s="39"/>
-      <c r="AV54" s="39"/>
-      <c r="AW54" s="39"/>
-      <c r="AX54" s="39"/>
-      <c r="AY54" s="39"/>
-      <c r="AZ54" s="39"/>
-      <c r="BA54" s="39"/>
-      <c r="BB54" s="39"/>
-      <c r="BC54" s="39"/>
-      <c r="BD54" s="39"/>
-      <c r="BE54" s="39"/>
-      <c r="BF54" s="39"/>
-      <c r="BG54" s="39"/>
-      <c r="BH54" s="39"/>
-      <c r="BI54" s="39"/>
-      <c r="BJ54" s="39"/>
-      <c r="BK54" s="39"/>
-      <c r="BL54" s="39"/>
-      <c r="BM54" s="39"/>
-      <c r="BN54" s="39"/>
-    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -8713,18 +8634,9 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="H8:H13 H15:H22 H24:H29 H38:H43">
+  <conditionalFormatting sqref="H8:H13 H23:H28 H37:H42 H15:H21">
     <cfRule type="dataBar" priority="66">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8739,20 +8651,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:BN7">
-    <cfRule type="expression" dxfId="15" priority="109">
+    <cfRule type="expression" dxfId="13" priority="109">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K8:BN13 K15:BN22 K24:BN54">
-    <cfRule type="expression" dxfId="14" priority="112">
+  <conditionalFormatting sqref="K8:BN13 K15:BN53">
+    <cfRule type="expression" dxfId="12" priority="112">
       <formula>AND($E8&lt;=K$6,ROUNDDOWN(($F8-$E8+1)*$H8,0)+$E8-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="113">
+    <cfRule type="expression" dxfId="11" priority="113">
       <formula>AND(NOT(ISBLANK($E8)),$E8&lt;=K$6,$F8&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K6:BN13 K15:BN22 K24:BN29 K38:BN43">
-    <cfRule type="expression" dxfId="12" priority="72">
+  <conditionalFormatting sqref="K6:BN13 K23:BN28 K37:BN42 K15:BN21">
+    <cfRule type="expression" dxfId="10" priority="72">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8771,19 +8683,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14:BN14">
-    <cfRule type="expression" dxfId="11" priority="63">
+    <cfRule type="expression" dxfId="9" priority="63">
       <formula>AND($E14&lt;=K$6,ROUNDDOWN(($F14-$E14+1)*$H14,0)+$E14-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="64">
+    <cfRule type="expression" dxfId="8" priority="64">
       <formula>AND(NOT(ISBLANK($E14)),$E14&lt;=K$6,$F14&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14:BN14">
-    <cfRule type="expression" dxfId="9" priority="62">
+    <cfRule type="expression" dxfId="7" priority="62">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H30">
+  <conditionalFormatting sqref="H29">
     <cfRule type="dataBar" priority="53">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8797,12 +8709,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K30:BN30">
-    <cfRule type="expression" dxfId="8" priority="54">
+  <conditionalFormatting sqref="K29:BN29">
+    <cfRule type="expression" dxfId="6" priority="54">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H23">
+  <conditionalFormatting sqref="H22">
     <cfRule type="dataBar" priority="49">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8816,20 +8728,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K23:BN23">
-    <cfRule type="expression" dxfId="7" priority="51">
-      <formula>AND($E23&lt;=K$6,ROUNDDOWN(($F23-$E23+1)*$H23,0)+$E23-1&gt;=K$6)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="52">
-      <formula>AND(NOT(ISBLANK($E23)),$E23&lt;=K$6,$F23&gt;=K$6)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K23:BN23">
+  <conditionalFormatting sqref="K22:BN22">
     <cfRule type="expression" dxfId="5" priority="50">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H31">
+  <conditionalFormatting sqref="H30">
     <cfRule type="dataBar" priority="45">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8843,12 +8747,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K31:BN31">
+  <conditionalFormatting sqref="K30:BN30">
     <cfRule type="expression" dxfId="4" priority="46">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H32:H37">
+  <conditionalFormatting sqref="H31:H36">
     <cfRule type="dataBar" priority="41">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8862,12 +8766,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K32:BN37">
+  <conditionalFormatting sqref="K31:BN36">
     <cfRule type="expression" dxfId="3" priority="42">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H44">
+  <conditionalFormatting sqref="H43">
     <cfRule type="dataBar" priority="25">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8881,12 +8785,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K44:BN44">
+  <conditionalFormatting sqref="K43:BN43">
     <cfRule type="expression" dxfId="2" priority="26">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H45:H49">
+  <conditionalFormatting sqref="H44:H48">
     <cfRule type="dataBar" priority="13">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8900,12 +8804,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K45:BN49">
+  <conditionalFormatting sqref="K44:BN48">
     <cfRule type="expression" dxfId="1" priority="14">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H50:H54">
+  <conditionalFormatting sqref="H49:H53">
     <cfRule type="dataBar" priority="7">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8919,7 +8823,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K50:BN54">
+  <conditionalFormatting sqref="K49:BN53">
     <cfRule type="expression" dxfId="0" priority="8">
       <formula>K$6=TODAY()</formula>
     </cfRule>
@@ -8934,8 +8838,8 @@
   <pageSetup scale="63" fitToHeight="0" orientation="landscape" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <ignoredErrors>
-    <ignoredError sqref="H9 H12 H16 G26:H26 H24 H25 G27:H27" unlockedFormula="1"/>
-    <ignoredError sqref="A24 A16 A12" formula="1"/>
+    <ignoredError sqref="H9 H12 G25:H25 H23 H24 G26:H26" unlockedFormula="1"/>
+    <ignoredError sqref="A23 A12" formula="1"/>
   </ignoredErrors>
   <drawing r:id="rId3"/>
   <legacyDrawing r:id="rId4"/>
@@ -8983,7 +8887,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H8:H13 H15:H22 H24:H29 H38:H43</xm:sqref>
+          <xm:sqref>H8:H13 H23:H28 H37:H42 H15:H21</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{8B894183-9857-4A8A-A710-A8E0A3639C63}">
@@ -9013,7 +8917,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H30</xm:sqref>
+          <xm:sqref>H29</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{58F6D71C-71C0-4BA6-AC57-EB4D3A5320ED}">
@@ -9028,7 +8932,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H23</xm:sqref>
+          <xm:sqref>H22</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{E9C1D637-3290-4949-BEC6-A595D31B5774}">
@@ -9043,7 +8947,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H31</xm:sqref>
+          <xm:sqref>H30</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{FBE85918-163F-478B-A582-154FD7C53A35}">
@@ -9058,7 +8962,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H32:H37</xm:sqref>
+          <xm:sqref>H31:H36</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{A4A83124-B4A0-493D-B2D7-1FCDD34DB4E8}">
@@ -9073,7 +8977,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H44</xm:sqref>
+          <xm:sqref>H43</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{B70A3E7C-A0AE-4626-880F-AF80C166C625}">
@@ -9088,7 +8992,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H45:H49</xm:sqref>
+          <xm:sqref>H44:H48</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{120CCD98-F855-4770-BAE7-6F6EA0A92E96}">
@@ -9103,7 +9007,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H50:H54</xm:sqref>
+          <xm:sqref>H49:H53</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
docs (gantt): revisi sesuai asprak
</commit_message>
<xml_diff>
--- a/docs/Gantt Chart.xlsx
+++ b/docs/Gantt Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\punch\Documents\GitHub\warawiriweb\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ABBEF32-3082-4DEF-8C64-C5527D35A1D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A904E9-DEEA-4E7B-9178-95B0A776C6BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -454,7 +454,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="191">
   <si>
     <t>WBS</t>
   </si>
@@ -1588,9 +1588,6 @@
     <t>Blog Frontend</t>
   </si>
   <si>
-    <t>Web Build 2 (Fe Be)</t>
-  </si>
-  <si>
     <t>Backend Blog</t>
   </si>
   <si>
@@ -1615,18 +1612,12 @@
     <t>Admin Homepage Mockup</t>
   </si>
   <si>
-    <t>Web Build 3 (admin)</t>
-  </si>
-  <si>
     <t>Admin Homepage Frontend</t>
   </si>
   <si>
     <t>Authorization Access</t>
   </si>
   <si>
-    <t>Web Build 4 (auth)</t>
-  </si>
-  <si>
     <t>Blog Util</t>
   </si>
   <si>
@@ -1636,9 +1627,6 @@
     <t>Paket Frontend</t>
   </si>
   <si>
-    <t>Utilization Fe Be</t>
-  </si>
-  <si>
     <t>Admin Pages Mockup</t>
   </si>
   <si>
@@ -1660,16 +1648,43 @@
     <t>Admin CRUD Paket Utils</t>
   </si>
   <si>
-    <t>Finalizing</t>
-  </si>
-  <si>
-    <t>Demonstration Client</t>
-  </si>
-  <si>
     <t>Deploy</t>
   </si>
   <si>
-    <t>Web Build 1</t>
+    <t>Home &amp; About Us</t>
+  </si>
+  <si>
+    <t>FAQ &amp; Blog</t>
+  </si>
+  <si>
+    <t>Contact, Admin, Auth</t>
+  </si>
+  <si>
+    <t>Admin &amp; User Sync</t>
+  </si>
+  <si>
+    <t>Client Meet 4</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Initialize JEST</t>
+  </si>
+  <si>
+    <t>Run JEST</t>
+  </si>
+  <si>
+    <t>Fixes (if any)</t>
+  </si>
+  <si>
+    <t>Joy &amp; Christian</t>
+  </si>
+  <si>
+    <t>Post-fix JEST (if any)</t>
+  </si>
+  <si>
+    <t>Post-fix Deploy (if any)</t>
   </si>
 </sst>
 </file>
@@ -2860,6 +2875,13 @@
     <xf numFmtId="1" fontId="50" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="45" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2869,6 +2891,10 @@
     <xf numFmtId="0" fontId="48" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="45" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="167" fontId="45" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2877,17 +2903,6 @@
     </xf>
     <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="45" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="45" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2939,7 +2954,19 @@
     <cellStyle name="Total" xfId="42" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="43" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="15">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <border>
         <left style="thin">
@@ -3174,7 +3201,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$H$4" horiz="1" max="100" min="1" page="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$H$4" horiz="1" max="100" min="1" page="0" val="5"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3830,11 +3857,11 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BN53"/>
+  <dimension ref="A1:BN57"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
+      <pane ySplit="7" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O61" sqref="O61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3861,29 +3888,29 @@
       <c r="E1" s="29"/>
       <c r="F1" s="29"/>
       <c r="I1" s="78"/>
-      <c r="K1" s="117" t="s">
+      <c r="K1" s="111" t="s">
         <v>71</v>
       </c>
-      <c r="L1" s="117"/>
-      <c r="M1" s="117"/>
-      <c r="N1" s="117"/>
-      <c r="O1" s="117"/>
-      <c r="P1" s="117"/>
-      <c r="Q1" s="117"/>
-      <c r="R1" s="117"/>
-      <c r="S1" s="117"/>
-      <c r="T1" s="117"/>
-      <c r="U1" s="117"/>
-      <c r="V1" s="117"/>
-      <c r="W1" s="117"/>
-      <c r="X1" s="117"/>
-      <c r="Y1" s="117"/>
-      <c r="Z1" s="117"/>
-      <c r="AA1" s="117"/>
-      <c r="AB1" s="117"/>
-      <c r="AC1" s="117"/>
-      <c r="AD1" s="117"/>
-      <c r="AE1" s="117"/>
+      <c r="L1" s="111"/>
+      <c r="M1" s="111"/>
+      <c r="N1" s="111"/>
+      <c r="O1" s="111"/>
+      <c r="P1" s="111"/>
+      <c r="Q1" s="111"/>
+      <c r="R1" s="111"/>
+      <c r="S1" s="111"/>
+      <c r="T1" s="111"/>
+      <c r="U1" s="111"/>
+      <c r="V1" s="111"/>
+      <c r="W1" s="111"/>
+      <c r="X1" s="111"/>
+      <c r="Y1" s="111"/>
+      <c r="Z1" s="111"/>
+      <c r="AA1" s="111"/>
+      <c r="AB1" s="111"/>
+      <c r="AC1" s="111"/>
+      <c r="AD1" s="111"/>
+      <c r="AE1" s="111"/>
     </row>
     <row r="2" spans="1:66" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
@@ -3923,196 +3950,196 @@
       <c r="B4" s="65" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="119">
+      <c r="C4" s="116">
         <v>45194</v>
       </c>
-      <c r="D4" s="119"/>
-      <c r="E4" s="119"/>
+      <c r="D4" s="116"/>
+      <c r="E4" s="116"/>
       <c r="F4" s="64"/>
       <c r="G4" s="65" t="s">
         <v>68</v>
       </c>
       <c r="H4" s="77">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="30"/>
-      <c r="K4" s="111" t="str">
+      <c r="K4" s="113" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 1</v>
-      </c>
-      <c r="L4" s="112"/>
-      <c r="M4" s="112"/>
-      <c r="N4" s="112"/>
-      <c r="O4" s="112"/>
-      <c r="P4" s="112"/>
-      <c r="Q4" s="113"/>
-      <c r="R4" s="111" t="str">
+        <v>Week 5</v>
+      </c>
+      <c r="L4" s="114"/>
+      <c r="M4" s="114"/>
+      <c r="N4" s="114"/>
+      <c r="O4" s="114"/>
+      <c r="P4" s="114"/>
+      <c r="Q4" s="115"/>
+      <c r="R4" s="113" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 2</v>
-      </c>
-      <c r="S4" s="112"/>
-      <c r="T4" s="112"/>
-      <c r="U4" s="112"/>
-      <c r="V4" s="112"/>
-      <c r="W4" s="112"/>
-      <c r="X4" s="113"/>
-      <c r="Y4" s="111" t="str">
+        <v>Week 6</v>
+      </c>
+      <c r="S4" s="114"/>
+      <c r="T4" s="114"/>
+      <c r="U4" s="114"/>
+      <c r="V4" s="114"/>
+      <c r="W4" s="114"/>
+      <c r="X4" s="115"/>
+      <c r="Y4" s="113" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 3</v>
-      </c>
-      <c r="Z4" s="112"/>
-      <c r="AA4" s="112"/>
-      <c r="AB4" s="112"/>
-      <c r="AC4" s="112"/>
-      <c r="AD4" s="112"/>
-      <c r="AE4" s="113"/>
-      <c r="AF4" s="111" t="str">
+        <v>Week 7</v>
+      </c>
+      <c r="Z4" s="114"/>
+      <c r="AA4" s="114"/>
+      <c r="AB4" s="114"/>
+      <c r="AC4" s="114"/>
+      <c r="AD4" s="114"/>
+      <c r="AE4" s="115"/>
+      <c r="AF4" s="113" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 4</v>
-      </c>
-      <c r="AG4" s="112"/>
-      <c r="AH4" s="112"/>
-      <c r="AI4" s="112"/>
-      <c r="AJ4" s="112"/>
-      <c r="AK4" s="112"/>
-      <c r="AL4" s="113"/>
-      <c r="AM4" s="111" t="str">
+        <v>Week 8</v>
+      </c>
+      <c r="AG4" s="114"/>
+      <c r="AH4" s="114"/>
+      <c r="AI4" s="114"/>
+      <c r="AJ4" s="114"/>
+      <c r="AK4" s="114"/>
+      <c r="AL4" s="115"/>
+      <c r="AM4" s="113" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 5</v>
-      </c>
-      <c r="AN4" s="112"/>
-      <c r="AO4" s="112"/>
-      <c r="AP4" s="112"/>
-      <c r="AQ4" s="112"/>
-      <c r="AR4" s="112"/>
-      <c r="AS4" s="113"/>
-      <c r="AT4" s="111" t="str">
+        <v>Week 9</v>
+      </c>
+      <c r="AN4" s="114"/>
+      <c r="AO4" s="114"/>
+      <c r="AP4" s="114"/>
+      <c r="AQ4" s="114"/>
+      <c r="AR4" s="114"/>
+      <c r="AS4" s="115"/>
+      <c r="AT4" s="113" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 6</v>
-      </c>
-      <c r="AU4" s="112"/>
-      <c r="AV4" s="112"/>
-      <c r="AW4" s="112"/>
-      <c r="AX4" s="112"/>
-      <c r="AY4" s="112"/>
-      <c r="AZ4" s="113"/>
-      <c r="BA4" s="111" t="str">
+        <v>Week 10</v>
+      </c>
+      <c r="AU4" s="114"/>
+      <c r="AV4" s="114"/>
+      <c r="AW4" s="114"/>
+      <c r="AX4" s="114"/>
+      <c r="AY4" s="114"/>
+      <c r="AZ4" s="115"/>
+      <c r="BA4" s="113" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 7</v>
-      </c>
-      <c r="BB4" s="112"/>
-      <c r="BC4" s="112"/>
-      <c r="BD4" s="112"/>
-      <c r="BE4" s="112"/>
-      <c r="BF4" s="112"/>
-      <c r="BG4" s="113"/>
-      <c r="BH4" s="111" t="str">
+        <v>Week 11</v>
+      </c>
+      <c r="BB4" s="114"/>
+      <c r="BC4" s="114"/>
+      <c r="BD4" s="114"/>
+      <c r="BE4" s="114"/>
+      <c r="BF4" s="114"/>
+      <c r="BG4" s="115"/>
+      <c r="BH4" s="113" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 8</v>
-      </c>
-      <c r="BI4" s="112"/>
-      <c r="BJ4" s="112"/>
-      <c r="BK4" s="112"/>
-      <c r="BL4" s="112"/>
-      <c r="BM4" s="112"/>
-      <c r="BN4" s="113"/>
+        <v>Week 12</v>
+      </c>
+      <c r="BI4" s="114"/>
+      <c r="BJ4" s="114"/>
+      <c r="BK4" s="114"/>
+      <c r="BL4" s="114"/>
+      <c r="BM4" s="114"/>
+      <c r="BN4" s="115"/>
     </row>
     <row r="5" spans="1:66" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="64"/>
       <c r="B5" s="65" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="118" t="s">
+      <c r="C5" s="112" t="s">
         <v>132</v>
       </c>
-      <c r="D5" s="118"/>
-      <c r="E5" s="118"/>
+      <c r="D5" s="112"/>
+      <c r="E5" s="112"/>
       <c r="F5" s="64"/>
       <c r="G5" s="64"/>
       <c r="H5" s="64"/>
       <c r="I5" s="64"/>
       <c r="J5" s="30"/>
-      <c r="K5" s="114">
+      <c r="K5" s="117">
         <f>K6</f>
-        <v>45194</v>
-      </c>
-      <c r="L5" s="115"/>
-      <c r="M5" s="115"/>
-      <c r="N5" s="115"/>
-      <c r="O5" s="115"/>
-      <c r="P5" s="115"/>
-      <c r="Q5" s="116"/>
-      <c r="R5" s="114">
+        <v>45222</v>
+      </c>
+      <c r="L5" s="118"/>
+      <c r="M5" s="118"/>
+      <c r="N5" s="118"/>
+      <c r="O5" s="118"/>
+      <c r="P5" s="118"/>
+      <c r="Q5" s="119"/>
+      <c r="R5" s="117">
         <f>R6</f>
-        <v>45201</v>
-      </c>
-      <c r="S5" s="115"/>
-      <c r="T5" s="115"/>
-      <c r="U5" s="115"/>
-      <c r="V5" s="115"/>
-      <c r="W5" s="115"/>
-      <c r="X5" s="116"/>
-      <c r="Y5" s="114">
+        <v>45229</v>
+      </c>
+      <c r="S5" s="118"/>
+      <c r="T5" s="118"/>
+      <c r="U5" s="118"/>
+      <c r="V5" s="118"/>
+      <c r="W5" s="118"/>
+      <c r="X5" s="119"/>
+      <c r="Y5" s="117">
         <f>Y6</f>
-        <v>45208</v>
-      </c>
-      <c r="Z5" s="115"/>
-      <c r="AA5" s="115"/>
-      <c r="AB5" s="115"/>
-      <c r="AC5" s="115"/>
-      <c r="AD5" s="115"/>
-      <c r="AE5" s="116"/>
-      <c r="AF5" s="114">
+        <v>45236</v>
+      </c>
+      <c r="Z5" s="118"/>
+      <c r="AA5" s="118"/>
+      <c r="AB5" s="118"/>
+      <c r="AC5" s="118"/>
+      <c r="AD5" s="118"/>
+      <c r="AE5" s="119"/>
+      <c r="AF5" s="117">
         <f>AF6</f>
-        <v>45215</v>
-      </c>
-      <c r="AG5" s="115"/>
-      <c r="AH5" s="115"/>
-      <c r="AI5" s="115"/>
-      <c r="AJ5" s="115"/>
-      <c r="AK5" s="115"/>
-      <c r="AL5" s="116"/>
-      <c r="AM5" s="114">
+        <v>45243</v>
+      </c>
+      <c r="AG5" s="118"/>
+      <c r="AH5" s="118"/>
+      <c r="AI5" s="118"/>
+      <c r="AJ5" s="118"/>
+      <c r="AK5" s="118"/>
+      <c r="AL5" s="119"/>
+      <c r="AM5" s="117">
         <f>AM6</f>
-        <v>45222</v>
-      </c>
-      <c r="AN5" s="115"/>
-      <c r="AO5" s="115"/>
-      <c r="AP5" s="115"/>
-      <c r="AQ5" s="115"/>
-      <c r="AR5" s="115"/>
-      <c r="AS5" s="116"/>
-      <c r="AT5" s="114">
+        <v>45250</v>
+      </c>
+      <c r="AN5" s="118"/>
+      <c r="AO5" s="118"/>
+      <c r="AP5" s="118"/>
+      <c r="AQ5" s="118"/>
+      <c r="AR5" s="118"/>
+      <c r="AS5" s="119"/>
+      <c r="AT5" s="117">
         <f>AT6</f>
-        <v>45229</v>
-      </c>
-      <c r="AU5" s="115"/>
-      <c r="AV5" s="115"/>
-      <c r="AW5" s="115"/>
-      <c r="AX5" s="115"/>
-      <c r="AY5" s="115"/>
-      <c r="AZ5" s="116"/>
-      <c r="BA5" s="114">
+        <v>45257</v>
+      </c>
+      <c r="AU5" s="118"/>
+      <c r="AV5" s="118"/>
+      <c r="AW5" s="118"/>
+      <c r="AX5" s="118"/>
+      <c r="AY5" s="118"/>
+      <c r="AZ5" s="119"/>
+      <c r="BA5" s="117">
         <f>BA6</f>
-        <v>45236</v>
-      </c>
-      <c r="BB5" s="115"/>
-      <c r="BC5" s="115"/>
-      <c r="BD5" s="115"/>
-      <c r="BE5" s="115"/>
-      <c r="BF5" s="115"/>
-      <c r="BG5" s="116"/>
-      <c r="BH5" s="114">
+        <v>45264</v>
+      </c>
+      <c r="BB5" s="118"/>
+      <c r="BC5" s="118"/>
+      <c r="BD5" s="118"/>
+      <c r="BE5" s="118"/>
+      <c r="BF5" s="118"/>
+      <c r="BG5" s="119"/>
+      <c r="BH5" s="117">
         <f>BH6</f>
-        <v>45243</v>
-      </c>
-      <c r="BI5" s="115"/>
-      <c r="BJ5" s="115"/>
-      <c r="BK5" s="115"/>
-      <c r="BL5" s="115"/>
-      <c r="BM5" s="115"/>
-      <c r="BN5" s="116"/>
+        <v>45271</v>
+      </c>
+      <c r="BI5" s="118"/>
+      <c r="BJ5" s="118"/>
+      <c r="BK5" s="118"/>
+      <c r="BL5" s="118"/>
+      <c r="BM5" s="118"/>
+      <c r="BN5" s="119"/>
     </row>
     <row r="6" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A6" s="30"/>
@@ -4127,227 +4154,227 @@
       <c r="J6" s="30"/>
       <c r="K6" s="53">
         <f>C4-WEEKDAY(C4,1)+2+7*(H4-1)</f>
-        <v>45194</v>
+        <v>45222</v>
       </c>
       <c r="L6" s="44">
         <f t="shared" ref="L6:AQ6" si="0">K6+1</f>
-        <v>45195</v>
+        <v>45223</v>
       </c>
       <c r="M6" s="44">
         <f t="shared" si="0"/>
-        <v>45196</v>
+        <v>45224</v>
       </c>
       <c r="N6" s="44">
         <f t="shared" si="0"/>
-        <v>45197</v>
+        <v>45225</v>
       </c>
       <c r="O6" s="44">
         <f t="shared" si="0"/>
-        <v>45198</v>
+        <v>45226</v>
       </c>
       <c r="P6" s="44">
         <f t="shared" si="0"/>
-        <v>45199</v>
+        <v>45227</v>
       </c>
       <c r="Q6" s="54">
         <f t="shared" si="0"/>
-        <v>45200</v>
+        <v>45228</v>
       </c>
       <c r="R6" s="53">
         <f t="shared" si="0"/>
-        <v>45201</v>
+        <v>45229</v>
       </c>
       <c r="S6" s="44">
         <f t="shared" si="0"/>
-        <v>45202</v>
+        <v>45230</v>
       </c>
       <c r="T6" s="44">
         <f t="shared" si="0"/>
-        <v>45203</v>
+        <v>45231</v>
       </c>
       <c r="U6" s="44">
         <f t="shared" si="0"/>
-        <v>45204</v>
+        <v>45232</v>
       </c>
       <c r="V6" s="44">
         <f t="shared" si="0"/>
-        <v>45205</v>
+        <v>45233</v>
       </c>
       <c r="W6" s="44">
         <f t="shared" si="0"/>
-        <v>45206</v>
+        <v>45234</v>
       </c>
       <c r="X6" s="54">
         <f t="shared" si="0"/>
-        <v>45207</v>
+        <v>45235</v>
       </c>
       <c r="Y6" s="53">
         <f t="shared" si="0"/>
-        <v>45208</v>
+        <v>45236</v>
       </c>
       <c r="Z6" s="44">
         <f t="shared" si="0"/>
-        <v>45209</v>
+        <v>45237</v>
       </c>
       <c r="AA6" s="44">
         <f t="shared" si="0"/>
-        <v>45210</v>
+        <v>45238</v>
       </c>
       <c r="AB6" s="44">
         <f t="shared" si="0"/>
-        <v>45211</v>
+        <v>45239</v>
       </c>
       <c r="AC6" s="44">
         <f t="shared" si="0"/>
-        <v>45212</v>
+        <v>45240</v>
       </c>
       <c r="AD6" s="44">
         <f t="shared" si="0"/>
-        <v>45213</v>
+        <v>45241</v>
       </c>
       <c r="AE6" s="54">
         <f t="shared" si="0"/>
-        <v>45214</v>
+        <v>45242</v>
       </c>
       <c r="AF6" s="53">
         <f t="shared" si="0"/>
-        <v>45215</v>
+        <v>45243</v>
       </c>
       <c r="AG6" s="44">
         <f t="shared" si="0"/>
-        <v>45216</v>
+        <v>45244</v>
       </c>
       <c r="AH6" s="44">
         <f t="shared" si="0"/>
-        <v>45217</v>
+        <v>45245</v>
       </c>
       <c r="AI6" s="44">
         <f t="shared" si="0"/>
-        <v>45218</v>
+        <v>45246</v>
       </c>
       <c r="AJ6" s="44">
         <f t="shared" si="0"/>
-        <v>45219</v>
+        <v>45247</v>
       </c>
       <c r="AK6" s="44">
         <f t="shared" si="0"/>
-        <v>45220</v>
+        <v>45248</v>
       </c>
       <c r="AL6" s="54">
         <f t="shared" si="0"/>
-        <v>45221</v>
+        <v>45249</v>
       </c>
       <c r="AM6" s="53">
         <f t="shared" si="0"/>
-        <v>45222</v>
+        <v>45250</v>
       </c>
       <c r="AN6" s="44">
         <f t="shared" si="0"/>
-        <v>45223</v>
+        <v>45251</v>
       </c>
       <c r="AO6" s="44">
         <f t="shared" si="0"/>
-        <v>45224</v>
+        <v>45252</v>
       </c>
       <c r="AP6" s="44">
         <f t="shared" si="0"/>
-        <v>45225</v>
+        <v>45253</v>
       </c>
       <c r="AQ6" s="44">
         <f t="shared" si="0"/>
-        <v>45226</v>
+        <v>45254</v>
       </c>
       <c r="AR6" s="44">
         <f t="shared" ref="AR6:BN6" si="1">AQ6+1</f>
-        <v>45227</v>
+        <v>45255</v>
       </c>
       <c r="AS6" s="54">
         <f t="shared" si="1"/>
-        <v>45228</v>
+        <v>45256</v>
       </c>
       <c r="AT6" s="53">
         <f t="shared" si="1"/>
-        <v>45229</v>
+        <v>45257</v>
       </c>
       <c r="AU6" s="44">
         <f t="shared" si="1"/>
-        <v>45230</v>
+        <v>45258</v>
       </c>
       <c r="AV6" s="44">
         <f t="shared" si="1"/>
-        <v>45231</v>
+        <v>45259</v>
       </c>
       <c r="AW6" s="44">
         <f t="shared" si="1"/>
-        <v>45232</v>
+        <v>45260</v>
       </c>
       <c r="AX6" s="44">
         <f t="shared" si="1"/>
-        <v>45233</v>
+        <v>45261</v>
       </c>
       <c r="AY6" s="44">
         <f t="shared" si="1"/>
-        <v>45234</v>
+        <v>45262</v>
       </c>
       <c r="AZ6" s="54">
         <f t="shared" si="1"/>
-        <v>45235</v>
+        <v>45263</v>
       </c>
       <c r="BA6" s="53">
         <f t="shared" si="1"/>
-        <v>45236</v>
+        <v>45264</v>
       </c>
       <c r="BB6" s="44">
         <f t="shared" si="1"/>
-        <v>45237</v>
+        <v>45265</v>
       </c>
       <c r="BC6" s="44">
         <f t="shared" si="1"/>
-        <v>45238</v>
+        <v>45266</v>
       </c>
       <c r="BD6" s="44">
         <f t="shared" si="1"/>
-        <v>45239</v>
+        <v>45267</v>
       </c>
       <c r="BE6" s="44">
         <f t="shared" si="1"/>
-        <v>45240</v>
+        <v>45268</v>
       </c>
       <c r="BF6" s="44">
         <f t="shared" si="1"/>
-        <v>45241</v>
+        <v>45269</v>
       </c>
       <c r="BG6" s="54">
         <f t="shared" si="1"/>
-        <v>45242</v>
+        <v>45270</v>
       </c>
       <c r="BH6" s="53">
         <f t="shared" si="1"/>
-        <v>45243</v>
+        <v>45271</v>
       </c>
       <c r="BI6" s="44">
         <f t="shared" si="1"/>
-        <v>45244</v>
+        <v>45272</v>
       </c>
       <c r="BJ6" s="44">
         <f t="shared" si="1"/>
-        <v>45245</v>
+        <v>45273</v>
       </c>
       <c r="BK6" s="44">
         <f t="shared" si="1"/>
-        <v>45246</v>
+        <v>45274</v>
       </c>
       <c r="BL6" s="44">
         <f t="shared" si="1"/>
-        <v>45247</v>
+        <v>45275</v>
       </c>
       <c r="BM6" s="44">
         <f t="shared" si="1"/>
-        <v>45248</v>
+        <v>45276</v>
       </c>
       <c r="BN6" s="54">
         <f t="shared" si="1"/>
-        <v>45249</v>
+        <v>45277</v>
       </c>
     </row>
     <row r="7" spans="1:66" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -4954,7 +4981,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D12" s="35"/>
       <c r="E12" s="60">
@@ -5828,7 +5855,7 @@
         <v>2.10</v>
       </c>
       <c r="B22" s="75" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C22" s="40" t="s">
         <v>134</v>
@@ -5916,7 +5943,7 @@
         <v>3</v>
       </c>
       <c r="B23" s="33" t="s">
-        <v>158</v>
+        <v>180</v>
       </c>
       <c r="D23" s="35"/>
       <c r="E23" s="60">
@@ -6438,7 +6465,7 @@
         <v>3.6</v>
       </c>
       <c r="B29" s="75" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C29" s="40" t="s">
         <v>153</v>
@@ -6526,7 +6553,7 @@
         <v>3.7</v>
       </c>
       <c r="B30" s="75" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C30" s="40" t="s">
         <v>134</v>
@@ -6614,7 +6641,7 @@
         <v>4</v>
       </c>
       <c r="B31" s="33" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
       <c r="D31" s="35"/>
       <c r="E31" s="60">
@@ -6623,15 +6650,15 @@
       </c>
       <c r="F31" s="60">
         <f t="shared" si="15"/>
-        <v>45226</v>
+        <v>45233</v>
       </c>
       <c r="G31" s="36">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="H31" s="37"/>
       <c r="I31" s="38">
         <f t="shared" si="16"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J31" s="57"/>
       <c r="K31" s="63"/>
@@ -6697,7 +6724,7 @@
         <v>4.1</v>
       </c>
       <c r="B32" s="75" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C32" s="40" t="s">
         <v>144</v>
@@ -6785,7 +6812,7 @@
         <v>4.2</v>
       </c>
       <c r="B33" s="75" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C33" s="40" t="s">
         <v>144</v>
@@ -6873,7 +6900,7 @@
         <v>4.3</v>
       </c>
       <c r="B34" s="75" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C34" s="40" t="s">
         <v>150</v>
@@ -6961,7 +6988,7 @@
         <v>4.4</v>
       </c>
       <c r="B35" s="75" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C35" s="40" t="s">
         <v>148</v>
@@ -7049,7 +7076,7 @@
         <v>4.5</v>
       </c>
       <c r="B36" s="75" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C36" s="40" t="s">
         <v>144</v>
@@ -7131,118 +7158,123 @@
       <c r="BM36" s="39"/>
       <c r="BN36" s="39"/>
     </row>
-    <row r="37" spans="1:66" s="34" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A37" s="32" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>5</v>
-      </c>
-      <c r="B37" s="33" t="s">
-        <v>170</v>
-      </c>
-      <c r="D37" s="35"/>
-      <c r="E37" s="60">
+    <row r="37" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A37" s="39" t="str">
+        <f t="shared" ref="A37:A42" si="17">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>4.6</v>
+      </c>
+      <c r="B37" s="75" t="s">
+        <v>169</v>
+      </c>
+      <c r="C37" s="40" t="s">
+        <v>144</v>
+      </c>
+      <c r="D37" s="76"/>
+      <c r="E37" s="58">
         <f>F36+3</f>
         <v>45229</v>
       </c>
-      <c r="F37" s="60">
-        <f t="shared" ref="F37:F42" si="17">IF(ISBLANK(E37)," - ",IF(G37=0,E37,E37+G37-1))</f>
-        <v>45233</v>
-      </c>
-      <c r="G37" s="36">
-        <v>5</v>
-      </c>
-      <c r="H37" s="37"/>
-      <c r="I37" s="38">
-        <f t="shared" ref="I37:I42" si="18">IF(OR(F37=0,E37=0)," - ",NETWORKDAYS(E37,F37))</f>
-        <v>5</v>
-      </c>
-      <c r="J37" s="57"/>
-      <c r="K37" s="63"/>
-      <c r="L37" s="63"/>
-      <c r="M37" s="63"/>
-      <c r="N37" s="63"/>
-      <c r="O37" s="63"/>
-      <c r="P37" s="63"/>
-      <c r="Q37" s="63"/>
-      <c r="R37" s="63"/>
-      <c r="S37" s="63"/>
-      <c r="T37" s="63"/>
-      <c r="U37" s="63"/>
-      <c r="V37" s="63"/>
-      <c r="W37" s="63"/>
-      <c r="X37" s="63"/>
-      <c r="Y37" s="63"/>
-      <c r="Z37" s="63"/>
-      <c r="AA37" s="63"/>
-      <c r="AB37" s="63"/>
-      <c r="AC37" s="63"/>
-      <c r="AD37" s="63"/>
-      <c r="AE37" s="63"/>
-      <c r="AF37" s="63"/>
-      <c r="AG37" s="63"/>
-      <c r="AH37" s="63"/>
-      <c r="AI37" s="63"/>
-      <c r="AJ37" s="63"/>
-      <c r="AK37" s="63"/>
-      <c r="AL37" s="63"/>
-      <c r="AM37" s="63"/>
-      <c r="AN37" s="63"/>
-      <c r="AO37" s="63"/>
-      <c r="AP37" s="63"/>
-      <c r="AQ37" s="63"/>
-      <c r="AR37" s="63"/>
-      <c r="AS37" s="63"/>
-      <c r="AT37" s="63"/>
-      <c r="AU37" s="63"/>
-      <c r="AV37" s="63"/>
-      <c r="AW37" s="63"/>
-      <c r="AX37" s="63"/>
-      <c r="AY37" s="63"/>
-      <c r="AZ37" s="63"/>
-      <c r="BA37" s="63"/>
-      <c r="BB37" s="63"/>
-      <c r="BC37" s="63"/>
-      <c r="BD37" s="63"/>
-      <c r="BE37" s="63"/>
-      <c r="BF37" s="63"/>
-      <c r="BG37" s="63"/>
-      <c r="BH37" s="63"/>
-      <c r="BI37" s="63"/>
-      <c r="BJ37" s="63"/>
-      <c r="BK37" s="63"/>
-      <c r="BL37" s="63"/>
-      <c r="BM37" s="63"/>
-      <c r="BN37" s="63"/>
-    </row>
-    <row r="38" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="F37" s="59">
+        <f>IF(ISBLANK(E37)," - ",IF(G37=0,E37,E37+G37-1))</f>
+        <v>45229</v>
+      </c>
+      <c r="G37" s="41">
+        <v>1</v>
+      </c>
+      <c r="H37" s="42">
+        <v>0</v>
+      </c>
+      <c r="I37" s="43">
+        <f>IF(OR(F37=0,E37=0)," - ",NETWORKDAYS(E37,F37))</f>
+        <v>1</v>
+      </c>
+      <c r="J37" s="56"/>
+      <c r="K37" s="39"/>
+      <c r="L37" s="39"/>
+      <c r="M37" s="39"/>
+      <c r="N37" s="39"/>
+      <c r="O37" s="39"/>
+      <c r="P37" s="39"/>
+      <c r="Q37" s="39"/>
+      <c r="R37" s="39"/>
+      <c r="S37" s="39"/>
+      <c r="T37" s="39"/>
+      <c r="U37" s="39"/>
+      <c r="V37" s="39"/>
+      <c r="W37" s="39"/>
+      <c r="X37" s="39"/>
+      <c r="Y37" s="39"/>
+      <c r="Z37" s="39"/>
+      <c r="AA37" s="39"/>
+      <c r="AB37" s="39"/>
+      <c r="AC37" s="39"/>
+      <c r="AD37" s="39"/>
+      <c r="AE37" s="39"/>
+      <c r="AF37" s="39"/>
+      <c r="AG37" s="39"/>
+      <c r="AH37" s="39"/>
+      <c r="AI37" s="39"/>
+      <c r="AJ37" s="39"/>
+      <c r="AK37" s="39"/>
+      <c r="AL37" s="39"/>
+      <c r="AM37" s="39"/>
+      <c r="AN37" s="39"/>
+      <c r="AO37" s="39"/>
+      <c r="AP37" s="39"/>
+      <c r="AQ37" s="39"/>
+      <c r="AR37" s="39"/>
+      <c r="AS37" s="39"/>
+      <c r="AT37" s="39"/>
+      <c r="AU37" s="39"/>
+      <c r="AV37" s="39"/>
+      <c r="AW37" s="39"/>
+      <c r="AX37" s="39"/>
+      <c r="AY37" s="39"/>
+      <c r="AZ37" s="39"/>
+      <c r="BA37" s="39"/>
+      <c r="BB37" s="39"/>
+      <c r="BC37" s="39"/>
+      <c r="BD37" s="39"/>
+      <c r="BE37" s="39"/>
+      <c r="BF37" s="39"/>
+      <c r="BG37" s="39"/>
+      <c r="BH37" s="39"/>
+      <c r="BI37" s="39"/>
+      <c r="BJ37" s="39"/>
+      <c r="BK37" s="39"/>
+      <c r="BL37" s="39"/>
+      <c r="BM37" s="39"/>
+      <c r="BN37" s="39"/>
+    </row>
+    <row r="38" spans="1:66" s="40" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A38" s="39" t="str">
-        <f t="shared" ref="A38:A43" si="19">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>5.1</v>
+        <f t="shared" si="17"/>
+        <v>4.7</v>
       </c>
       <c r="B38" s="75" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="C38" s="40" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D38" s="76"/>
       <c r="E38" s="58">
-        <f>E37</f>
+        <f>F36+3</f>
         <v>45229</v>
       </c>
       <c r="F38" s="59">
-        <f>IF(ISBLANK(E38)," - ",IF(G38=0,E38,E38+G38-1))</f>
-        <v>45229</v>
+        <f t="shared" ref="F38:F41" si="18">IF(ISBLANK(E38)," - ",IF(G38=0,E38,E38+G38-1))</f>
+        <v>45230</v>
       </c>
       <c r="G38" s="41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H38" s="42">
         <v>0</v>
       </c>
       <c r="I38" s="43">
-        <f>IF(OR(F38=0,E38=0)," - ",NETWORKDAYS(E38,F38))</f>
-        <v>1</v>
+        <f t="shared" ref="I38:I41" si="19">IF(OR(F38=0,E38=0)," - ",NETWORKDAYS(E38,F38))</f>
+        <v>2</v>
       </c>
       <c r="J38" s="56"/>
       <c r="K38" s="39"/>
@@ -7302,35 +7334,35 @@
       <c r="BM38" s="39"/>
       <c r="BN38" s="39"/>
     </row>
-    <row r="39" spans="1:66" s="40" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A39" s="39" t="str">
-        <f t="shared" si="19"/>
-        <v>5.2</v>
+        <f t="shared" si="17"/>
+        <v>4.8</v>
       </c>
       <c r="B39" s="75" t="s">
         <v>168</v>
       </c>
       <c r="C39" s="40" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="D39" s="76"/>
       <c r="E39" s="58">
-        <f>E37</f>
+        <f>F36+3</f>
         <v>45229</v>
       </c>
       <c r="F39" s="59">
-        <f t="shared" si="17"/>
-        <v>45230</v>
+        <f>IF(ISBLANK(E39)," - ",IF(G39=0,E39,E39+G39-1))</f>
+        <v>45231</v>
       </c>
       <c r="G39" s="41">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H39" s="42">
         <v>0</v>
       </c>
       <c r="I39" s="43">
-        <f t="shared" si="18"/>
-        <v>2</v>
+        <f>IF(OR(F39=0,E39=0)," - ",NETWORKDAYS(E39,F39))</f>
+        <v>3</v>
       </c>
       <c r="J39" s="56"/>
       <c r="K39" s="39"/>
@@ -7392,33 +7424,33 @@
     </row>
     <row r="40" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" s="39" t="str">
-        <f t="shared" si="19"/>
-        <v>5.3</v>
+        <f t="shared" si="17"/>
+        <v>4.9</v>
       </c>
       <c r="B40" s="75" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C40" s="40" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D40" s="76"/>
       <c r="E40" s="58">
-        <f>E37</f>
-        <v>45229</v>
+        <f>F37+1</f>
+        <v>45230</v>
       </c>
       <c r="F40" s="59">
         <f>IF(ISBLANK(E40)," - ",IF(G40=0,E40,E40+G40-1))</f>
         <v>45231</v>
       </c>
       <c r="G40" s="41">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H40" s="42">
         <v>0</v>
       </c>
       <c r="I40" s="43">
         <f>IF(OR(F40=0,E40=0)," - ",NETWORKDAYS(E40,F40))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J40" s="56"/>
       <c r="K40" s="39"/>
@@ -7480,33 +7512,33 @@
     </row>
     <row r="41" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A41" s="39" t="str">
-        <f t="shared" si="19"/>
-        <v>5.4</v>
+        <f t="shared" si="17"/>
+        <v>4.10</v>
       </c>
       <c r="B41" s="75" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="C41" s="40" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="D41" s="76"/>
       <c r="E41" s="58">
         <f>F38+1</f>
-        <v>45230</v>
+        <v>45231</v>
       </c>
       <c r="F41" s="59">
-        <f>IF(ISBLANK(E41)," - ",IF(G41=0,E41,E41+G41-1))</f>
-        <v>45231</v>
+        <f t="shared" si="18"/>
+        <v>45233</v>
       </c>
       <c r="G41" s="41">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H41" s="42">
         <v>0</v>
       </c>
       <c r="I41" s="43">
-        <f>IF(OR(F41=0,E41=0)," - ",NETWORKDAYS(E41,F41))</f>
-        <v>2</v>
+        <f t="shared" si="19"/>
+        <v>3</v>
       </c>
       <c r="J41" s="56"/>
       <c r="K41" s="39"/>
@@ -7568,33 +7600,33 @@
     </row>
     <row r="42" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A42" s="39" t="str">
-        <f t="shared" si="19"/>
-        <v>5.5</v>
+        <f t="shared" si="17"/>
+        <v>4.11</v>
       </c>
       <c r="B42" s="75" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="C42" s="40" t="s">
         <v>134</v>
       </c>
       <c r="D42" s="76"/>
       <c r="E42" s="58">
-        <f>F39+1</f>
-        <v>45231</v>
+        <f>F31</f>
+        <v>45233</v>
       </c>
       <c r="F42" s="59">
-        <f t="shared" si="17"/>
+        <f t="shared" ref="F42" si="20">IF(ISBLANK(E42)," - ",IF(G42=0,E42,E42+G42-1))</f>
         <v>45233</v>
       </c>
       <c r="G42" s="41">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H42" s="42">
         <v>0</v>
       </c>
       <c r="I42" s="43">
-        <f t="shared" si="18"/>
-        <v>3</v>
+        <f t="shared" ref="I42" si="21">IF(OR(F42=0,E42=0)," - ",NETWORKDAYS(E42,F42))</f>
+        <v>1</v>
       </c>
       <c r="J42" s="56"/>
       <c r="K42" s="39"/>
@@ -7654,206 +7686,206 @@
       <c r="BM42" s="39"/>
       <c r="BN42" s="39"/>
     </row>
-    <row r="43" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A43" s="39" t="str">
-        <f t="shared" si="19"/>
-        <v>5.6</v>
-      </c>
-      <c r="B43" s="75" t="s">
-        <v>161</v>
-      </c>
-      <c r="C43" s="40" t="s">
-        <v>134</v>
-      </c>
-      <c r="D43" s="76"/>
-      <c r="E43" s="58">
-        <f>F37</f>
-        <v>45233</v>
-      </c>
-      <c r="F43" s="59">
-        <f t="shared" ref="F43" si="20">IF(ISBLANK(E43)," - ",IF(G43=0,E43,E43+G43-1))</f>
-        <v>45233</v>
-      </c>
-      <c r="G43" s="41">
-        <v>1</v>
-      </c>
-      <c r="H43" s="42">
+    <row r="43" spans="1:66" s="34" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A43" s="32" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>5</v>
+      </c>
+      <c r="B43" s="33" t="s">
+        <v>182</v>
+      </c>
+      <c r="D43" s="35"/>
+      <c r="E43" s="60">
+        <f>F31+3</f>
+        <v>45236</v>
+      </c>
+      <c r="F43" s="60">
+        <f t="shared" ref="F43" si="22">IF(ISBLANK(E43)," - ",IF(G43=0,E43,E43+G43-1))</f>
+        <v>45247</v>
+      </c>
+      <c r="G43" s="36">
+        <v>12</v>
+      </c>
+      <c r="H43" s="37"/>
+      <c r="I43" s="38">
+        <f t="shared" ref="I43" si="23">IF(OR(F43=0,E43=0)," - ",NETWORKDAYS(E43,F43))</f>
+        <v>10</v>
+      </c>
+      <c r="J43" s="57"/>
+      <c r="K43" s="63"/>
+      <c r="L43" s="63"/>
+      <c r="M43" s="63"/>
+      <c r="N43" s="63"/>
+      <c r="O43" s="63"/>
+      <c r="P43" s="63"/>
+      <c r="Q43" s="63"/>
+      <c r="R43" s="63"/>
+      <c r="S43" s="63"/>
+      <c r="T43" s="63"/>
+      <c r="U43" s="63"/>
+      <c r="V43" s="63"/>
+      <c r="W43" s="63"/>
+      <c r="X43" s="63"/>
+      <c r="Y43" s="63"/>
+      <c r="Z43" s="63"/>
+      <c r="AA43" s="63"/>
+      <c r="AB43" s="63"/>
+      <c r="AC43" s="63"/>
+      <c r="AD43" s="63"/>
+      <c r="AE43" s="63"/>
+      <c r="AF43" s="63"/>
+      <c r="AG43" s="63"/>
+      <c r="AH43" s="63"/>
+      <c r="AI43" s="63"/>
+      <c r="AJ43" s="63"/>
+      <c r="AK43" s="63"/>
+      <c r="AL43" s="63"/>
+      <c r="AM43" s="63"/>
+      <c r="AN43" s="63"/>
+      <c r="AO43" s="63"/>
+      <c r="AP43" s="63"/>
+      <c r="AQ43" s="63"/>
+      <c r="AR43" s="63"/>
+      <c r="AS43" s="63"/>
+      <c r="AT43" s="63"/>
+      <c r="AU43" s="63"/>
+      <c r="AV43" s="63"/>
+      <c r="AW43" s="63"/>
+      <c r="AX43" s="63"/>
+      <c r="AY43" s="63"/>
+      <c r="AZ43" s="63"/>
+      <c r="BA43" s="63"/>
+      <c r="BB43" s="63"/>
+      <c r="BC43" s="63"/>
+      <c r="BD43" s="63"/>
+      <c r="BE43" s="63"/>
+      <c r="BF43" s="63"/>
+      <c r="BG43" s="63"/>
+      <c r="BH43" s="63"/>
+      <c r="BI43" s="63"/>
+      <c r="BJ43" s="63"/>
+      <c r="BK43" s="63"/>
+      <c r="BL43" s="63"/>
+      <c r="BM43" s="63"/>
+      <c r="BN43" s="63"/>
+    </row>
+    <row r="44" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A44" s="39" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>5.1</v>
+      </c>
+      <c r="B44" s="75" t="s">
+        <v>171</v>
+      </c>
+      <c r="C44" s="40" t="s">
+        <v>144</v>
+      </c>
+      <c r="D44" s="76"/>
+      <c r="E44" s="58">
+        <f>E43</f>
+        <v>45236</v>
+      </c>
+      <c r="F44" s="59">
+        <f>IF(ISBLANK(E44)," - ",IF(G44=0,E44,E44+G44-1))</f>
+        <v>45238</v>
+      </c>
+      <c r="G44" s="41">
+        <v>3</v>
+      </c>
+      <c r="H44" s="42">
         <v>0</v>
       </c>
-      <c r="I43" s="43">
-        <f t="shared" ref="I43" si="21">IF(OR(F43=0,E43=0)," - ",NETWORKDAYS(E43,F43))</f>
-        <v>1</v>
-      </c>
-      <c r="J43" s="56"/>
-      <c r="K43" s="39"/>
-      <c r="L43" s="39"/>
-      <c r="M43" s="39"/>
-      <c r="N43" s="39"/>
-      <c r="O43" s="39"/>
-      <c r="P43" s="39"/>
-      <c r="Q43" s="39"/>
-      <c r="R43" s="39"/>
-      <c r="S43" s="39"/>
-      <c r="T43" s="39"/>
-      <c r="U43" s="39"/>
-      <c r="V43" s="39"/>
-      <c r="W43" s="39"/>
-      <c r="X43" s="39"/>
-      <c r="Y43" s="39"/>
-      <c r="Z43" s="39"/>
-      <c r="AA43" s="39"/>
-      <c r="AB43" s="39"/>
-      <c r="AC43" s="39"/>
-      <c r="AD43" s="39"/>
-      <c r="AE43" s="39"/>
-      <c r="AF43" s="39"/>
-      <c r="AG43" s="39"/>
-      <c r="AH43" s="39"/>
-      <c r="AI43" s="39"/>
-      <c r="AJ43" s="39"/>
-      <c r="AK43" s="39"/>
-      <c r="AL43" s="39"/>
-      <c r="AM43" s="39"/>
-      <c r="AN43" s="39"/>
-      <c r="AO43" s="39"/>
-      <c r="AP43" s="39"/>
-      <c r="AQ43" s="39"/>
-      <c r="AR43" s="39"/>
-      <c r="AS43" s="39"/>
-      <c r="AT43" s="39"/>
-      <c r="AU43" s="39"/>
-      <c r="AV43" s="39"/>
-      <c r="AW43" s="39"/>
-      <c r="AX43" s="39"/>
-      <c r="AY43" s="39"/>
-      <c r="AZ43" s="39"/>
-      <c r="BA43" s="39"/>
-      <c r="BB43" s="39"/>
-      <c r="BC43" s="39"/>
-      <c r="BD43" s="39"/>
-      <c r="BE43" s="39"/>
-      <c r="BF43" s="39"/>
-      <c r="BG43" s="39"/>
-      <c r="BH43" s="39"/>
-      <c r="BI43" s="39"/>
-      <c r="BJ43" s="39"/>
-      <c r="BK43" s="39"/>
-      <c r="BL43" s="39"/>
-      <c r="BM43" s="39"/>
-      <c r="BN43" s="39"/>
-    </row>
-    <row r="44" spans="1:66" s="34" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A44" s="32" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>6</v>
-      </c>
-      <c r="B44" s="33" t="s">
-        <v>174</v>
-      </c>
-      <c r="D44" s="35"/>
-      <c r="E44" s="60">
-        <f>F37+3</f>
-        <v>45236</v>
-      </c>
-      <c r="F44" s="60">
-        <f t="shared" ref="F44" si="22">IF(ISBLANK(E44)," - ",IF(G44=0,E44,E44+G44-1))</f>
-        <v>45240</v>
-      </c>
-      <c r="G44" s="36">
-        <v>5</v>
-      </c>
-      <c r="H44" s="37"/>
-      <c r="I44" s="38">
-        <f t="shared" ref="I44" si="23">IF(OR(F44=0,E44=0)," - ",NETWORKDAYS(E44,F44))</f>
-        <v>5</v>
-      </c>
-      <c r="J44" s="57"/>
-      <c r="K44" s="63"/>
-      <c r="L44" s="63"/>
-      <c r="M44" s="63"/>
-      <c r="N44" s="63"/>
-      <c r="O44" s="63"/>
-      <c r="P44" s="63"/>
-      <c r="Q44" s="63"/>
-      <c r="R44" s="63"/>
-      <c r="S44" s="63"/>
-      <c r="T44" s="63"/>
-      <c r="U44" s="63"/>
-      <c r="V44" s="63"/>
-      <c r="W44" s="63"/>
-      <c r="X44" s="63"/>
-      <c r="Y44" s="63"/>
-      <c r="Z44" s="63"/>
-      <c r="AA44" s="63"/>
-      <c r="AB44" s="63"/>
-      <c r="AC44" s="63"/>
-      <c r="AD44" s="63"/>
-      <c r="AE44" s="63"/>
-      <c r="AF44" s="63"/>
-      <c r="AG44" s="63"/>
-      <c r="AH44" s="63"/>
-      <c r="AI44" s="63"/>
-      <c r="AJ44" s="63"/>
-      <c r="AK44" s="63"/>
-      <c r="AL44" s="63"/>
-      <c r="AM44" s="63"/>
-      <c r="AN44" s="63"/>
-      <c r="AO44" s="63"/>
-      <c r="AP44" s="63"/>
-      <c r="AQ44" s="63"/>
-      <c r="AR44" s="63"/>
-      <c r="AS44" s="63"/>
-      <c r="AT44" s="63"/>
-      <c r="AU44" s="63"/>
-      <c r="AV44" s="63"/>
-      <c r="AW44" s="63"/>
-      <c r="AX44" s="63"/>
-      <c r="AY44" s="63"/>
-      <c r="AZ44" s="63"/>
-      <c r="BA44" s="63"/>
-      <c r="BB44" s="63"/>
-      <c r="BC44" s="63"/>
-      <c r="BD44" s="63"/>
-      <c r="BE44" s="63"/>
-      <c r="BF44" s="63"/>
-      <c r="BG44" s="63"/>
-      <c r="BH44" s="63"/>
-      <c r="BI44" s="63"/>
-      <c r="BJ44" s="63"/>
-      <c r="BK44" s="63"/>
-      <c r="BL44" s="63"/>
-      <c r="BM44" s="63"/>
-      <c r="BN44" s="63"/>
-    </row>
-    <row r="45" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="I44" s="43">
+        <f>IF(OR(F44=0,E44=0)," - ",NETWORKDAYS(E44,F44))</f>
+        <v>3</v>
+      </c>
+      <c r="J44" s="56"/>
+      <c r="K44" s="39"/>
+      <c r="L44" s="39"/>
+      <c r="M44" s="39"/>
+      <c r="N44" s="39"/>
+      <c r="O44" s="39"/>
+      <c r="P44" s="39"/>
+      <c r="Q44" s="39"/>
+      <c r="R44" s="39"/>
+      <c r="S44" s="39"/>
+      <c r="T44" s="39"/>
+      <c r="U44" s="39"/>
+      <c r="V44" s="39"/>
+      <c r="W44" s="39"/>
+      <c r="X44" s="39"/>
+      <c r="Y44" s="39"/>
+      <c r="Z44" s="39"/>
+      <c r="AA44" s="39"/>
+      <c r="AB44" s="39"/>
+      <c r="AC44" s="39"/>
+      <c r="AD44" s="39"/>
+      <c r="AE44" s="39"/>
+      <c r="AF44" s="39"/>
+      <c r="AG44" s="39"/>
+      <c r="AH44" s="39"/>
+      <c r="AI44" s="39"/>
+      <c r="AJ44" s="39"/>
+      <c r="AK44" s="39"/>
+      <c r="AL44" s="39"/>
+      <c r="AM44" s="39"/>
+      <c r="AN44" s="39"/>
+      <c r="AO44" s="39"/>
+      <c r="AP44" s="39"/>
+      <c r="AQ44" s="39"/>
+      <c r="AR44" s="39"/>
+      <c r="AS44" s="39"/>
+      <c r="AT44" s="39"/>
+      <c r="AU44" s="39"/>
+      <c r="AV44" s="39"/>
+      <c r="AW44" s="39"/>
+      <c r="AX44" s="39"/>
+      <c r="AY44" s="39"/>
+      <c r="AZ44" s="39"/>
+      <c r="BA44" s="39"/>
+      <c r="BB44" s="39"/>
+      <c r="BC44" s="39"/>
+      <c r="BD44" s="39"/>
+      <c r="BE44" s="39"/>
+      <c r="BF44" s="39"/>
+      <c r="BG44" s="39"/>
+      <c r="BH44" s="39"/>
+      <c r="BI44" s="39"/>
+      <c r="BJ44" s="39"/>
+      <c r="BK44" s="39"/>
+      <c r="BL44" s="39"/>
+      <c r="BM44" s="39"/>
+      <c r="BN44" s="39"/>
+    </row>
+    <row r="45" spans="1:66" s="40" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A45" s="39" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>6.1</v>
+        <v>5.2</v>
       </c>
       <c r="B45" s="75" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C45" s="40" t="s">
-        <v>144</v>
+        <v>173</v>
       </c>
       <c r="D45" s="76"/>
       <c r="E45" s="58">
-        <f>E44</f>
-        <v>45236</v>
+        <f>E44+1</f>
+        <v>45237</v>
       </c>
       <c r="F45" s="59">
-        <f>IF(ISBLANK(E45)," - ",IF(G45=0,E45,E45+G45-1))</f>
-        <v>45238</v>
+        <f t="shared" ref="F45" si="24">IF(ISBLANK(E45)," - ",IF(G45=0,E45,E45+G45-1))</f>
+        <v>45240</v>
       </c>
       <c r="G45" s="41">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H45" s="42">
         <v>0</v>
       </c>
       <c r="I45" s="43">
-        <f>IF(OR(F45=0,E45=0)," - ",NETWORKDAYS(E45,F45))</f>
-        <v>3</v>
+        <f t="shared" ref="I45" si="25">IF(OR(F45=0,E45=0)," - ",NETWORKDAYS(E45,F45))</f>
+        <v>4</v>
       </c>
       <c r="J45" s="56"/>
       <c r="K45" s="39"/>
@@ -7913,35 +7945,35 @@
       <c r="BM45" s="39"/>
       <c r="BN45" s="39"/>
     </row>
-    <row r="46" spans="1:66" s="40" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" s="39" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>6.2</v>
+        <v>5.3</v>
       </c>
       <c r="B46" s="75" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C46" s="40" t="s">
-        <v>177</v>
+        <v>153</v>
       </c>
       <c r="D46" s="76"/>
       <c r="E46" s="58">
-        <f>E45+1</f>
-        <v>45237</v>
+        <f>E43</f>
+        <v>45236</v>
       </c>
       <c r="F46" s="59">
-        <f t="shared" ref="F46" si="24">IF(ISBLANK(E46)," - ",IF(G46=0,E46,E46+G46-1))</f>
-        <v>45240</v>
+        <f>IF(ISBLANK(E46)," - ",IF(G46=0,E46,E46+G46-1))</f>
+        <v>45238</v>
       </c>
       <c r="G46" s="41">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H46" s="42">
         <v>0</v>
       </c>
       <c r="I46" s="43">
-        <f t="shared" ref="I46" si="25">IF(OR(F46=0,E46=0)," - ",NETWORKDAYS(E46,F46))</f>
-        <v>4</v>
+        <f>IF(OR(F46=0,E46=0)," - ",NETWORKDAYS(E46,F46))</f>
+        <v>3</v>
       </c>
       <c r="J46" s="56"/>
       <c r="K46" s="39"/>
@@ -8004,32 +8036,32 @@
     <row r="47" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" s="39" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>6.3</v>
+        <v>5.4</v>
       </c>
       <c r="B47" s="75" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C47" s="40" t="s">
         <v>153</v>
       </c>
       <c r="D47" s="76"/>
       <c r="E47" s="58">
-        <f>E44</f>
-        <v>45236</v>
+        <f>F46+1</f>
+        <v>45239</v>
       </c>
       <c r="F47" s="59">
         <f>IF(ISBLANK(E47)," - ",IF(G47=0,E47,E47+G47-1))</f>
-        <v>45238</v>
+        <v>45240</v>
       </c>
       <c r="G47" s="41">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H47" s="42">
         <v>0</v>
       </c>
       <c r="I47" s="43">
         <f>IF(OR(F47=0,E47=0)," - ",NETWORKDAYS(E47,F47))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J47" s="56"/>
       <c r="K47" s="39"/>
@@ -8089,35 +8121,35 @@
       <c r="BM47" s="39"/>
       <c r="BN47" s="39"/>
     </row>
-    <row r="48" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:66" s="40" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A48" s="39" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>6.4</v>
+        <v>5.5</v>
       </c>
       <c r="B48" s="75" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C48" s="40" t="s">
         <v>153</v>
       </c>
       <c r="D48" s="76"/>
       <c r="E48" s="58">
-        <f>F47+1</f>
-        <v>45239</v>
+        <f>F47+3</f>
+        <v>45243</v>
       </c>
       <c r="F48" s="59">
         <f>IF(ISBLANK(E48)," - ",IF(G48=0,E48,E48+G48-1))</f>
-        <v>45240</v>
+        <v>45245</v>
       </c>
       <c r="G48" s="41">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H48" s="42">
         <v>0</v>
       </c>
       <c r="I48" s="43">
         <f>IF(OR(F48=0,E48=0)," - ",NETWORKDAYS(E48,F48))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J48" s="56"/>
       <c r="K48" s="39"/>
@@ -8177,118 +8209,123 @@
       <c r="BM48" s="39"/>
       <c r="BN48" s="39"/>
     </row>
-    <row r="49" spans="1:66" s="34" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A49" s="32" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>7</v>
-      </c>
-      <c r="B49" s="33" t="s">
-        <v>182</v>
-      </c>
-      <c r="D49" s="35"/>
-      <c r="E49" s="60">
-        <f>F48+3</f>
+    <row r="49" spans="1:66" s="40" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A49" s="39" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>5.6</v>
+      </c>
+      <c r="B49" s="75" t="s">
+        <v>177</v>
+      </c>
+      <c r="C49" s="40" t="s">
+        <v>134</v>
+      </c>
+      <c r="D49" s="76"/>
+      <c r="E49" s="58">
+        <f>F47+3</f>
         <v>45243</v>
       </c>
-      <c r="F49" s="60">
+      <c r="F49" s="59">
         <f t="shared" ref="F49" si="26">IF(ISBLANK(E49)," - ",IF(G49=0,E49,E49+G49-1))</f>
-        <v>45247</v>
-      </c>
-      <c r="G49" s="36">
-        <v>5</v>
-      </c>
-      <c r="H49" s="37"/>
-      <c r="I49" s="38">
+        <v>45245</v>
+      </c>
+      <c r="G49" s="41">
+        <v>3</v>
+      </c>
+      <c r="H49" s="42">
+        <v>0</v>
+      </c>
+      <c r="I49" s="43">
         <f t="shared" ref="I49" si="27">IF(OR(F49=0,E49=0)," - ",NETWORKDAYS(E49,F49))</f>
-        <v>5</v>
-      </c>
-      <c r="J49" s="57"/>
-      <c r="K49" s="63"/>
-      <c r="L49" s="63"/>
-      <c r="M49" s="63"/>
-      <c r="N49" s="63"/>
-      <c r="O49" s="63"/>
-      <c r="P49" s="63"/>
-      <c r="Q49" s="63"/>
-      <c r="R49" s="63"/>
-      <c r="S49" s="63"/>
-      <c r="T49" s="63"/>
-      <c r="U49" s="63"/>
-      <c r="V49" s="63"/>
-      <c r="W49" s="63"/>
-      <c r="X49" s="63"/>
-      <c r="Y49" s="63"/>
-      <c r="Z49" s="63"/>
-      <c r="AA49" s="63"/>
-      <c r="AB49" s="63"/>
-      <c r="AC49" s="63"/>
-      <c r="AD49" s="63"/>
-      <c r="AE49" s="63"/>
-      <c r="AF49" s="63"/>
-      <c r="AG49" s="63"/>
-      <c r="AH49" s="63"/>
-      <c r="AI49" s="63"/>
-      <c r="AJ49" s="63"/>
-      <c r="AK49" s="63"/>
-      <c r="AL49" s="63"/>
-      <c r="AM49" s="63"/>
-      <c r="AN49" s="63"/>
-      <c r="AO49" s="63"/>
-      <c r="AP49" s="63"/>
-      <c r="AQ49" s="63"/>
-      <c r="AR49" s="63"/>
-      <c r="AS49" s="63"/>
-      <c r="AT49" s="63"/>
-      <c r="AU49" s="63"/>
-      <c r="AV49" s="63"/>
-      <c r="AW49" s="63"/>
-      <c r="AX49" s="63"/>
-      <c r="AY49" s="63"/>
-      <c r="AZ49" s="63"/>
-      <c r="BA49" s="63"/>
-      <c r="BB49" s="63"/>
-      <c r="BC49" s="63"/>
-      <c r="BD49" s="63"/>
-      <c r="BE49" s="63"/>
-      <c r="BF49" s="63"/>
-      <c r="BG49" s="63"/>
-      <c r="BH49" s="63"/>
-      <c r="BI49" s="63"/>
-      <c r="BJ49" s="63"/>
-      <c r="BK49" s="63"/>
-      <c r="BL49" s="63"/>
-      <c r="BM49" s="63"/>
-      <c r="BN49" s="63"/>
-    </row>
-    <row r="50" spans="1:66" s="40" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="J49" s="56"/>
+      <c r="K49" s="39"/>
+      <c r="L49" s="39"/>
+      <c r="M49" s="39"/>
+      <c r="N49" s="39"/>
+      <c r="O49" s="39"/>
+      <c r="P49" s="39"/>
+      <c r="Q49" s="39"/>
+      <c r="R49" s="39"/>
+      <c r="S49" s="39"/>
+      <c r="T49" s="39"/>
+      <c r="U49" s="39"/>
+      <c r="V49" s="39"/>
+      <c r="W49" s="39"/>
+      <c r="X49" s="39"/>
+      <c r="Y49" s="39"/>
+      <c r="Z49" s="39"/>
+      <c r="AA49" s="39"/>
+      <c r="AB49" s="39"/>
+      <c r="AC49" s="39"/>
+      <c r="AD49" s="39"/>
+      <c r="AE49" s="39"/>
+      <c r="AF49" s="39"/>
+      <c r="AG49" s="39"/>
+      <c r="AH49" s="39"/>
+      <c r="AI49" s="39"/>
+      <c r="AJ49" s="39"/>
+      <c r="AK49" s="39"/>
+      <c r="AL49" s="39"/>
+      <c r="AM49" s="39"/>
+      <c r="AN49" s="39"/>
+      <c r="AO49" s="39"/>
+      <c r="AP49" s="39"/>
+      <c r="AQ49" s="39"/>
+      <c r="AR49" s="39"/>
+      <c r="AS49" s="39"/>
+      <c r="AT49" s="39"/>
+      <c r="AU49" s="39"/>
+      <c r="AV49" s="39"/>
+      <c r="AW49" s="39"/>
+      <c r="AX49" s="39"/>
+      <c r="AY49" s="39"/>
+      <c r="AZ49" s="39"/>
+      <c r="BA49" s="39"/>
+      <c r="BB49" s="39"/>
+      <c r="BC49" s="39"/>
+      <c r="BD49" s="39"/>
+      <c r="BE49" s="39"/>
+      <c r="BF49" s="39"/>
+      <c r="BG49" s="39"/>
+      <c r="BH49" s="39"/>
+      <c r="BI49" s="39"/>
+      <c r="BJ49" s="39"/>
+      <c r="BK49" s="39"/>
+      <c r="BL49" s="39"/>
+      <c r="BM49" s="39"/>
+      <c r="BN49" s="39"/>
+    </row>
+    <row r="50" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A50" s="39" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>7.1</v>
+        <v>5.7</v>
       </c>
       <c r="B50" s="75" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C50" s="40" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="D50" s="76"/>
       <c r="E50" s="58">
-        <f>E49</f>
-        <v>45243</v>
+        <f>F49+1</f>
+        <v>45246</v>
       </c>
       <c r="F50" s="59">
         <f>IF(ISBLANK(E50)," - ",IF(G50=0,E50,E50+G50-1))</f>
-        <v>45245</v>
+        <v>45246</v>
       </c>
       <c r="G50" s="41">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H50" s="42">
         <v>0</v>
       </c>
       <c r="I50" s="43">
         <f>IF(OR(F50=0,E50=0)," - ",NETWORKDAYS(E50,F50))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J50" s="56"/>
       <c r="K50" s="39"/>
@@ -8348,35 +8385,35 @@
       <c r="BM50" s="39"/>
       <c r="BN50" s="39"/>
     </row>
-    <row r="51" spans="1:66" s="40" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A51" s="39" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>7.2</v>
+        <v>5.8</v>
       </c>
       <c r="B51" s="75" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C51" s="40" t="s">
         <v>134</v>
       </c>
       <c r="D51" s="76"/>
       <c r="E51" s="58">
-        <f>E49</f>
-        <v>45243</v>
+        <f>F50+1</f>
+        <v>45247</v>
       </c>
       <c r="F51" s="59">
-        <f t="shared" ref="F51" si="28">IF(ISBLANK(E51)," - ",IF(G51=0,E51,E51+G51-1))</f>
-        <v>45245</v>
+        <f>IF(ISBLANK(E51)," - ",IF(G51=0,E51,E51+G51-1))</f>
+        <v>45247</v>
       </c>
       <c r="G51" s="41">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H51" s="42">
         <v>0</v>
       </c>
       <c r="I51" s="43">
-        <f t="shared" ref="I51" si="29">IF(OR(F51=0,E51=0)," - ",NETWORKDAYS(E51,F51))</f>
-        <v>3</v>
+        <f>IF(OR(F51=0,E51=0)," - ",NETWORKDAYS(E51,F51))</f>
+        <v>1</v>
       </c>
       <c r="J51" s="56"/>
       <c r="K51" s="39"/>
@@ -8436,123 +8473,118 @@
       <c r="BM51" s="39"/>
       <c r="BN51" s="39"/>
     </row>
-    <row r="52" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A52" s="39" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>7.3</v>
-      </c>
-      <c r="B52" s="75" t="s">
-        <v>183</v>
-      </c>
-      <c r="C52" s="40" t="s">
-        <v>134</v>
-      </c>
-      <c r="D52" s="76"/>
-      <c r="E52" s="58">
-        <f>F51+1</f>
-        <v>45246</v>
-      </c>
-      <c r="F52" s="59">
-        <f>IF(ISBLANK(E52)," - ",IF(G52=0,E52,E52+G52-1))</f>
-        <v>45246</v>
-      </c>
-      <c r="G52" s="41">
-        <v>1</v>
-      </c>
-      <c r="H52" s="42">
-        <v>0</v>
-      </c>
-      <c r="I52" s="43">
-        <f>IF(OR(F52=0,E52=0)," - ",NETWORKDAYS(E52,F52))</f>
-        <v>1</v>
-      </c>
-      <c r="J52" s="56"/>
-      <c r="K52" s="39"/>
-      <c r="L52" s="39"/>
-      <c r="M52" s="39"/>
-      <c r="N52" s="39"/>
-      <c r="O52" s="39"/>
-      <c r="P52" s="39"/>
-      <c r="Q52" s="39"/>
-      <c r="R52" s="39"/>
-      <c r="S52" s="39"/>
-      <c r="T52" s="39"/>
-      <c r="U52" s="39"/>
-      <c r="V52" s="39"/>
-      <c r="W52" s="39"/>
-      <c r="X52" s="39"/>
-      <c r="Y52" s="39"/>
-      <c r="Z52" s="39"/>
-      <c r="AA52" s="39"/>
-      <c r="AB52" s="39"/>
-      <c r="AC52" s="39"/>
-      <c r="AD52" s="39"/>
-      <c r="AE52" s="39"/>
-      <c r="AF52" s="39"/>
-      <c r="AG52" s="39"/>
-      <c r="AH52" s="39"/>
-      <c r="AI52" s="39"/>
-      <c r="AJ52" s="39"/>
-      <c r="AK52" s="39"/>
-      <c r="AL52" s="39"/>
-      <c r="AM52" s="39"/>
-      <c r="AN52" s="39"/>
-      <c r="AO52" s="39"/>
-      <c r="AP52" s="39"/>
-      <c r="AQ52" s="39"/>
-      <c r="AR52" s="39"/>
-      <c r="AS52" s="39"/>
-      <c r="AT52" s="39"/>
-      <c r="AU52" s="39"/>
-      <c r="AV52" s="39"/>
-      <c r="AW52" s="39"/>
-      <c r="AX52" s="39"/>
-      <c r="AY52" s="39"/>
-      <c r="AZ52" s="39"/>
-      <c r="BA52" s="39"/>
-      <c r="BB52" s="39"/>
-      <c r="BC52" s="39"/>
-      <c r="BD52" s="39"/>
-      <c r="BE52" s="39"/>
-      <c r="BF52" s="39"/>
-      <c r="BG52" s="39"/>
-      <c r="BH52" s="39"/>
-      <c r="BI52" s="39"/>
-      <c r="BJ52" s="39"/>
-      <c r="BK52" s="39"/>
-      <c r="BL52" s="39"/>
-      <c r="BM52" s="39"/>
-      <c r="BN52" s="39"/>
+    <row r="52" spans="1:66" s="34" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A52" s="32" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>6</v>
+      </c>
+      <c r="B52" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="D52" s="35"/>
+      <c r="E52" s="60">
+        <f>F43+3</f>
+        <v>45250</v>
+      </c>
+      <c r="F52" s="60">
+        <f t="shared" ref="F52" si="28">IF(ISBLANK(E52)," - ",IF(G52=0,E52,E52+G52-1))</f>
+        <v>45254</v>
+      </c>
+      <c r="G52" s="36">
+        <v>5</v>
+      </c>
+      <c r="H52" s="37"/>
+      <c r="I52" s="38">
+        <f t="shared" ref="I52" si="29">IF(OR(F52=0,E52=0)," - ",NETWORKDAYS(E52,F52))</f>
+        <v>5</v>
+      </c>
+      <c r="J52" s="57"/>
+      <c r="K52" s="63"/>
+      <c r="L52" s="63"/>
+      <c r="M52" s="63"/>
+      <c r="N52" s="63"/>
+      <c r="O52" s="63"/>
+      <c r="P52" s="63"/>
+      <c r="Q52" s="63"/>
+      <c r="R52" s="63"/>
+      <c r="S52" s="63"/>
+      <c r="T52" s="63"/>
+      <c r="U52" s="63"/>
+      <c r="V52" s="63"/>
+      <c r="W52" s="63"/>
+      <c r="X52" s="63"/>
+      <c r="Y52" s="63"/>
+      <c r="Z52" s="63"/>
+      <c r="AA52" s="63"/>
+      <c r="AB52" s="63"/>
+      <c r="AC52" s="63"/>
+      <c r="AD52" s="63"/>
+      <c r="AE52" s="63"/>
+      <c r="AF52" s="63"/>
+      <c r="AG52" s="63"/>
+      <c r="AH52" s="63"/>
+      <c r="AI52" s="63"/>
+      <c r="AJ52" s="63"/>
+      <c r="AK52" s="63"/>
+      <c r="AL52" s="63"/>
+      <c r="AM52" s="63"/>
+      <c r="AN52" s="63"/>
+      <c r="AO52" s="63"/>
+      <c r="AP52" s="63"/>
+      <c r="AQ52" s="63"/>
+      <c r="AR52" s="63"/>
+      <c r="AS52" s="63"/>
+      <c r="AT52" s="63"/>
+      <c r="AU52" s="63"/>
+      <c r="AV52" s="63"/>
+      <c r="AW52" s="63"/>
+      <c r="AX52" s="63"/>
+      <c r="AY52" s="63"/>
+      <c r="AZ52" s="63"/>
+      <c r="BA52" s="63"/>
+      <c r="BB52" s="63"/>
+      <c r="BC52" s="63"/>
+      <c r="BD52" s="63"/>
+      <c r="BE52" s="63"/>
+      <c r="BF52" s="63"/>
+      <c r="BG52" s="63"/>
+      <c r="BH52" s="63"/>
+      <c r="BI52" s="63"/>
+      <c r="BJ52" s="63"/>
+      <c r="BK52" s="63"/>
+      <c r="BL52" s="63"/>
+      <c r="BM52" s="63"/>
+      <c r="BN52" s="63"/>
     </row>
     <row r="53" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A53" s="39" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>7.4</v>
+        <v>6.1</v>
       </c>
       <c r="B53" s="75" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C53" s="40" t="s">
         <v>134</v>
       </c>
       <c r="D53" s="76"/>
       <c r="E53" s="58">
-        <f>F52+1</f>
-        <v>45247</v>
+        <f>E52</f>
+        <v>45250</v>
       </c>
       <c r="F53" s="59">
         <f>IF(ISBLANK(E53)," - ",IF(G53=0,E53,E53+G53-1))</f>
-        <v>45247</v>
+        <v>45251</v>
       </c>
       <c r="G53" s="41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H53" s="42">
         <v>0</v>
       </c>
       <c r="I53" s="43">
         <f>IF(OR(F53=0,E53=0)," - ",NETWORKDAYS(E53,F53))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J53" s="56"/>
       <c r="K53" s="39"/>
@@ -8612,18 +8644,361 @@
       <c r="BM53" s="39"/>
       <c r="BN53" s="39"/>
     </row>
+    <row r="54" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A54" s="39" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>6.2</v>
+      </c>
+      <c r="B54" s="75" t="s">
+        <v>186</v>
+      </c>
+      <c r="C54" s="40" t="s">
+        <v>134</v>
+      </c>
+      <c r="D54" s="76"/>
+      <c r="E54" s="58">
+        <f>F53+1</f>
+        <v>45252</v>
+      </c>
+      <c r="F54" s="59">
+        <f t="shared" ref="F54" si="30">IF(ISBLANK(E54)," - ",IF(G54=0,E54,E54+G54-1))</f>
+        <v>45252</v>
+      </c>
+      <c r="G54" s="41">
+        <v>1</v>
+      </c>
+      <c r="H54" s="42">
+        <v>0</v>
+      </c>
+      <c r="I54" s="43">
+        <f t="shared" ref="I54" si="31">IF(OR(F54=0,E54=0)," - ",NETWORKDAYS(E54,F54))</f>
+        <v>1</v>
+      </c>
+      <c r="J54" s="56"/>
+      <c r="K54" s="39"/>
+      <c r="L54" s="39"/>
+      <c r="M54" s="39"/>
+      <c r="N54" s="39"/>
+      <c r="O54" s="39"/>
+      <c r="P54" s="39"/>
+      <c r="Q54" s="39"/>
+      <c r="R54" s="39"/>
+      <c r="S54" s="39"/>
+      <c r="T54" s="39"/>
+      <c r="U54" s="39"/>
+      <c r="V54" s="39"/>
+      <c r="W54" s="39"/>
+      <c r="X54" s="39"/>
+      <c r="Y54" s="39"/>
+      <c r="Z54" s="39"/>
+      <c r="AA54" s="39"/>
+      <c r="AB54" s="39"/>
+      <c r="AC54" s="39"/>
+      <c r="AD54" s="39"/>
+      <c r="AE54" s="39"/>
+      <c r="AF54" s="39"/>
+      <c r="AG54" s="39"/>
+      <c r="AH54" s="39"/>
+      <c r="AI54" s="39"/>
+      <c r="AJ54" s="39"/>
+      <c r="AK54" s="39"/>
+      <c r="AL54" s="39"/>
+      <c r="AM54" s="39"/>
+      <c r="AN54" s="39"/>
+      <c r="AO54" s="39"/>
+      <c r="AP54" s="39"/>
+      <c r="AQ54" s="39"/>
+      <c r="AR54" s="39"/>
+      <c r="AS54" s="39"/>
+      <c r="AT54" s="39"/>
+      <c r="AU54" s="39"/>
+      <c r="AV54" s="39"/>
+      <c r="AW54" s="39"/>
+      <c r="AX54" s="39"/>
+      <c r="AY54" s="39"/>
+      <c r="AZ54" s="39"/>
+      <c r="BA54" s="39"/>
+      <c r="BB54" s="39"/>
+      <c r="BC54" s="39"/>
+      <c r="BD54" s="39"/>
+      <c r="BE54" s="39"/>
+      <c r="BF54" s="39"/>
+      <c r="BG54" s="39"/>
+      <c r="BH54" s="39"/>
+      <c r="BI54" s="39"/>
+      <c r="BJ54" s="39"/>
+      <c r="BK54" s="39"/>
+      <c r="BL54" s="39"/>
+      <c r="BM54" s="39"/>
+      <c r="BN54" s="39"/>
+    </row>
+    <row r="55" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A55" s="39" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>6.3</v>
+      </c>
+      <c r="B55" s="75" t="s">
+        <v>187</v>
+      </c>
+      <c r="C55" s="40" t="s">
+        <v>188</v>
+      </c>
+      <c r="D55" s="76"/>
+      <c r="E55" s="58">
+        <f>F54+1</f>
+        <v>45253</v>
+      </c>
+      <c r="F55" s="59">
+        <f>IF(ISBLANK(E55)," - ",IF(G55=0,E55,E55+G55-1))</f>
+        <v>45253</v>
+      </c>
+      <c r="G55" s="41">
+        <v>1</v>
+      </c>
+      <c r="H55" s="42">
+        <v>0</v>
+      </c>
+      <c r="I55" s="43">
+        <f>IF(OR(F55=0,E55=0)," - ",NETWORKDAYS(E55,F55))</f>
+        <v>1</v>
+      </c>
+      <c r="J55" s="56"/>
+      <c r="K55" s="39"/>
+      <c r="L55" s="39"/>
+      <c r="M55" s="39"/>
+      <c r="N55" s="39"/>
+      <c r="O55" s="39"/>
+      <c r="P55" s="39"/>
+      <c r="Q55" s="39"/>
+      <c r="R55" s="39"/>
+      <c r="S55" s="39"/>
+      <c r="T55" s="39"/>
+      <c r="U55" s="39"/>
+      <c r="V55" s="39"/>
+      <c r="W55" s="39"/>
+      <c r="X55" s="39"/>
+      <c r="Y55" s="39"/>
+      <c r="Z55" s="39"/>
+      <c r="AA55" s="39"/>
+      <c r="AB55" s="39"/>
+      <c r="AC55" s="39"/>
+      <c r="AD55" s="39"/>
+      <c r="AE55" s="39"/>
+      <c r="AF55" s="39"/>
+      <c r="AG55" s="39"/>
+      <c r="AH55" s="39"/>
+      <c r="AI55" s="39"/>
+      <c r="AJ55" s="39"/>
+      <c r="AK55" s="39"/>
+      <c r="AL55" s="39"/>
+      <c r="AM55" s="39"/>
+      <c r="AN55" s="39"/>
+      <c r="AO55" s="39"/>
+      <c r="AP55" s="39"/>
+      <c r="AQ55" s="39"/>
+      <c r="AR55" s="39"/>
+      <c r="AS55" s="39"/>
+      <c r="AT55" s="39"/>
+      <c r="AU55" s="39"/>
+      <c r="AV55" s="39"/>
+      <c r="AW55" s="39"/>
+      <c r="AX55" s="39"/>
+      <c r="AY55" s="39"/>
+      <c r="AZ55" s="39"/>
+      <c r="BA55" s="39"/>
+      <c r="BB55" s="39"/>
+      <c r="BC55" s="39"/>
+      <c r="BD55" s="39"/>
+      <c r="BE55" s="39"/>
+      <c r="BF55" s="39"/>
+      <c r="BG55" s="39"/>
+      <c r="BH55" s="39"/>
+      <c r="BI55" s="39"/>
+      <c r="BJ55" s="39"/>
+      <c r="BK55" s="39"/>
+      <c r="BL55" s="39"/>
+      <c r="BM55" s="39"/>
+      <c r="BN55" s="39"/>
+    </row>
+    <row r="56" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A56" s="39" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>6.4</v>
+      </c>
+      <c r="B56" s="75" t="s">
+        <v>189</v>
+      </c>
+      <c r="C56" s="40" t="s">
+        <v>134</v>
+      </c>
+      <c r="D56" s="76"/>
+      <c r="E56" s="58">
+        <f>F55+1</f>
+        <v>45254</v>
+      </c>
+      <c r="F56" s="59">
+        <f>IF(ISBLANK(E56)," - ",IF(G56=0,E56,E56+G56-1))</f>
+        <v>45254</v>
+      </c>
+      <c r="G56" s="41">
+        <v>1</v>
+      </c>
+      <c r="H56" s="42">
+        <v>0</v>
+      </c>
+      <c r="I56" s="43">
+        <f>IF(OR(F56=0,E56=0)," - ",NETWORKDAYS(E56,F56))</f>
+        <v>1</v>
+      </c>
+      <c r="J56" s="56"/>
+      <c r="K56" s="39"/>
+      <c r="L56" s="39"/>
+      <c r="M56" s="39"/>
+      <c r="N56" s="39"/>
+      <c r="O56" s="39"/>
+      <c r="P56" s="39"/>
+      <c r="Q56" s="39"/>
+      <c r="R56" s="39"/>
+      <c r="S56" s="39"/>
+      <c r="T56" s="39"/>
+      <c r="U56" s="39"/>
+      <c r="V56" s="39"/>
+      <c r="W56" s="39"/>
+      <c r="X56" s="39"/>
+      <c r="Y56" s="39"/>
+      <c r="Z56" s="39"/>
+      <c r="AA56" s="39"/>
+      <c r="AB56" s="39"/>
+      <c r="AC56" s="39"/>
+      <c r="AD56" s="39"/>
+      <c r="AE56" s="39"/>
+      <c r="AF56" s="39"/>
+      <c r="AG56" s="39"/>
+      <c r="AH56" s="39"/>
+      <c r="AI56" s="39"/>
+      <c r="AJ56" s="39"/>
+      <c r="AK56" s="39"/>
+      <c r="AL56" s="39"/>
+      <c r="AM56" s="39"/>
+      <c r="AN56" s="39"/>
+      <c r="AO56" s="39"/>
+      <c r="AP56" s="39"/>
+      <c r="AQ56" s="39"/>
+      <c r="AR56" s="39"/>
+      <c r="AS56" s="39"/>
+      <c r="AT56" s="39"/>
+      <c r="AU56" s="39"/>
+      <c r="AV56" s="39"/>
+      <c r="AW56" s="39"/>
+      <c r="AX56" s="39"/>
+      <c r="AY56" s="39"/>
+      <c r="AZ56" s="39"/>
+      <c r="BA56" s="39"/>
+      <c r="BB56" s="39"/>
+      <c r="BC56" s="39"/>
+      <c r="BD56" s="39"/>
+      <c r="BE56" s="39"/>
+      <c r="BF56" s="39"/>
+      <c r="BG56" s="39"/>
+      <c r="BH56" s="39"/>
+      <c r="BI56" s="39"/>
+      <c r="BJ56" s="39"/>
+      <c r="BK56" s="39"/>
+      <c r="BL56" s="39"/>
+      <c r="BM56" s="39"/>
+      <c r="BN56" s="39"/>
+    </row>
+    <row r="57" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A57" s="39" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>6.5</v>
+      </c>
+      <c r="B57" s="75" t="s">
+        <v>190</v>
+      </c>
+      <c r="C57" s="40" t="s">
+        <v>134</v>
+      </c>
+      <c r="D57" s="76"/>
+      <c r="E57" s="58">
+        <f>F55+1</f>
+        <v>45254</v>
+      </c>
+      <c r="F57" s="59">
+        <f>IF(ISBLANK(E57)," - ",IF(G57=0,E57,E57+G57-1))</f>
+        <v>45254</v>
+      </c>
+      <c r="G57" s="41">
+        <v>1</v>
+      </c>
+      <c r="H57" s="42">
+        <v>0</v>
+      </c>
+      <c r="I57" s="43">
+        <f>IF(OR(F57=0,E57=0)," - ",NETWORKDAYS(E57,F57))</f>
+        <v>1</v>
+      </c>
+      <c r="J57" s="56"/>
+      <c r="K57" s="39"/>
+      <c r="L57" s="39"/>
+      <c r="M57" s="39"/>
+      <c r="N57" s="39"/>
+      <c r="O57" s="39"/>
+      <c r="P57" s="39"/>
+      <c r="Q57" s="39"/>
+      <c r="R57" s="39"/>
+      <c r="S57" s="39"/>
+      <c r="T57" s="39"/>
+      <c r="U57" s="39"/>
+      <c r="V57" s="39"/>
+      <c r="W57" s="39"/>
+      <c r="X57" s="39"/>
+      <c r="Y57" s="39"/>
+      <c r="Z57" s="39"/>
+      <c r="AA57" s="39"/>
+      <c r="AB57" s="39"/>
+      <c r="AC57" s="39"/>
+      <c r="AD57" s="39"/>
+      <c r="AE57" s="39"/>
+      <c r="AF57" s="39"/>
+      <c r="AG57" s="39"/>
+      <c r="AH57" s="39"/>
+      <c r="AI57" s="39"/>
+      <c r="AJ57" s="39"/>
+      <c r="AK57" s="39"/>
+      <c r="AL57" s="39"/>
+      <c r="AM57" s="39"/>
+      <c r="AN57" s="39"/>
+      <c r="AO57" s="39"/>
+      <c r="AP57" s="39"/>
+      <c r="AQ57" s="39"/>
+      <c r="AR57" s="39"/>
+      <c r="AS57" s="39"/>
+      <c r="AT57" s="39"/>
+      <c r="AU57" s="39"/>
+      <c r="AV57" s="39"/>
+      <c r="AW57" s="39"/>
+      <c r="AX57" s="39"/>
+      <c r="AY57" s="39"/>
+      <c r="AZ57" s="39"/>
+      <c r="BA57" s="39"/>
+      <c r="BB57" s="39"/>
+      <c r="BC57" s="39"/>
+      <c r="BD57" s="39"/>
+      <c r="BE57" s="39"/>
+      <c r="BF57" s="39"/>
+      <c r="BG57" s="39"/>
+      <c r="BH57" s="39"/>
+      <c r="BI57" s="39"/>
+      <c r="BJ57" s="39"/>
+      <c r="BK57" s="39"/>
+      <c r="BL57" s="39"/>
+      <c r="BM57" s="39"/>
+      <c r="BN57" s="39"/>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -8634,10 +9009,19 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="H8:H13 H23:H28 H37:H42 H15:H21">
-    <cfRule type="dataBar" priority="66">
+  <conditionalFormatting sqref="H8:H13 H23:H28 H15:H21 H37:H41 H48:H51">
+    <cfRule type="dataBar" priority="76">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8651,25 +9035,25 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:BN7">
-    <cfRule type="expression" dxfId="13" priority="109">
+    <cfRule type="expression" dxfId="14" priority="119">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K8:BN13 K15:BN53">
-    <cfRule type="expression" dxfId="12" priority="112">
+  <conditionalFormatting sqref="K8:BN13 K15:BN57">
+    <cfRule type="expression" dxfId="13" priority="122">
       <formula>AND($E8&lt;=K$6,ROUNDDOWN(($F8-$E8+1)*$H8,0)+$E8-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="113">
+    <cfRule type="expression" dxfId="12" priority="123">
       <formula>AND(NOT(ISBLANK($E8)),$E8&lt;=K$6,$F8&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K6:BN13 K23:BN28 K37:BN42 K15:BN21">
-    <cfRule type="expression" dxfId="10" priority="72">
+  <conditionalFormatting sqref="K6:BN13 K23:BN28 K15:BN21 K37:BN41 K48:BN51">
+    <cfRule type="expression" dxfId="11" priority="82">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14">
-    <cfRule type="dataBar" priority="61">
+    <cfRule type="dataBar" priority="71">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8683,20 +9067,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14:BN14">
-    <cfRule type="expression" dxfId="9" priority="63">
+    <cfRule type="expression" dxfId="10" priority="73">
       <formula>AND($E14&lt;=K$6,ROUNDDOWN(($F14-$E14+1)*$H14,0)+$E14-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="64">
+    <cfRule type="expression" dxfId="9" priority="74">
       <formula>AND(NOT(ISBLANK($E14)),$E14&lt;=K$6,$F14&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14:BN14">
-    <cfRule type="expression" dxfId="7" priority="62">
+    <cfRule type="expression" dxfId="8" priority="72">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="dataBar" priority="53">
+    <cfRule type="dataBar" priority="63">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8710,12 +9094,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K29:BN29">
-    <cfRule type="expression" dxfId="6" priority="54">
+    <cfRule type="expression" dxfId="7" priority="64">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="dataBar" priority="49">
+    <cfRule type="dataBar" priority="59">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8729,12 +9113,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K22:BN22">
-    <cfRule type="expression" dxfId="5" priority="50">
+    <cfRule type="expression" dxfId="6" priority="60">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30">
-    <cfRule type="dataBar" priority="45">
+    <cfRule type="dataBar" priority="55">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8748,12 +9132,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30:BN30">
-    <cfRule type="expression" dxfId="4" priority="46">
+    <cfRule type="expression" dxfId="5" priority="56">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H31:H36">
-    <cfRule type="dataBar" priority="41">
+    <cfRule type="dataBar" priority="51">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8767,12 +9151,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31:BN36">
-    <cfRule type="expression" dxfId="3" priority="42">
+    <cfRule type="expression" dxfId="4" priority="52">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H43">
-    <cfRule type="dataBar" priority="25">
+  <conditionalFormatting sqref="H42">
+    <cfRule type="dataBar" priority="35">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8785,13 +9169,13 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K43:BN43">
-    <cfRule type="expression" dxfId="2" priority="26">
+  <conditionalFormatting sqref="K42:BN42">
+    <cfRule type="expression" dxfId="3" priority="36">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H44:H48">
-    <cfRule type="dataBar" priority="13">
+  <conditionalFormatting sqref="H43:H47">
+    <cfRule type="dataBar" priority="23">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8804,13 +9188,13 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K44:BN48">
-    <cfRule type="expression" dxfId="1" priority="14">
+  <conditionalFormatting sqref="K43:BN47">
+    <cfRule type="expression" dxfId="2" priority="24">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H49:H53">
-    <cfRule type="dataBar" priority="7">
+  <conditionalFormatting sqref="H57">
+    <cfRule type="dataBar" priority="3">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -8818,13 +9202,32 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{120CCD98-F855-4770-BAE7-6F6EA0A92E96}</x14:id>
+          <x14:id>{6DBBCF31-E55C-4294-8FCB-F0FA362C5C95}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K49:BN53">
-    <cfRule type="expression" dxfId="0" priority="8">
+  <conditionalFormatting sqref="K57:BN57">
+    <cfRule type="expression" dxfId="1" priority="4">
+      <formula>K$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H52:H56">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{64B6C333-2C16-4864-8114-3AB7CB8DBBAB}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K52:BN56">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8887,7 +9290,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H8:H13 H23:H28 H37:H42 H15:H21</xm:sqref>
+          <xm:sqref>H8:H13 H23:H28 H15:H21 H37:H41 H48:H51</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{8B894183-9857-4A8A-A710-A8E0A3639C63}">
@@ -8977,7 +9380,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H43</xm:sqref>
+          <xm:sqref>H42</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{B70A3E7C-A0AE-4626-880F-AF80C166C625}">
@@ -8992,10 +9395,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H44:H48</xm:sqref>
+          <xm:sqref>H43:H47</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{120CCD98-F855-4770-BAE7-6F6EA0A92E96}">
+          <x14:cfRule type="dataBar" id="{6DBBCF31-E55C-4294-8FCB-F0FA362C5C95}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -9007,7 +9410,22 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H49:H53</xm:sqref>
+          <xm:sqref>H57</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{64B6C333-2C16-4864-8114-3AB7CB8DBBAB}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H52:H56</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
docs: update workload status
</commit_message>
<xml_diff>
--- a/docs/Gantt Chart.xlsx
+++ b/docs/Gantt Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\punch\Documents\GitHub\warawiriweb\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A904E9-DEEA-4E7B-9178-95B0A776C6BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ECF10C8-DCBF-4F39-B07E-5B79D7F254CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2875,13 +2875,6 @@
     <xf numFmtId="1" fontId="50" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="45" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2891,10 +2884,6 @@
     <xf numFmtId="0" fontId="48" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="45" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="167" fontId="45" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2903,6 +2892,17 @@
     </xf>
     <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="45" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="45" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3201,7 +3201,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$H$4" horiz="1" max="100" min="1" page="0" val="5"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$H$4" horiz="1" max="100" min="1" page="0" val="4"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3860,8 +3860,8 @@
   <dimension ref="A1:BN57"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O61" sqref="O61"/>
+      <pane ySplit="7" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T30" sqref="T30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3888,29 +3888,29 @@
       <c r="E1" s="29"/>
       <c r="F1" s="29"/>
       <c r="I1" s="78"/>
-      <c r="K1" s="111" t="s">
+      <c r="K1" s="117" t="s">
         <v>71</v>
       </c>
-      <c r="L1" s="111"/>
-      <c r="M1" s="111"/>
-      <c r="N1" s="111"/>
-      <c r="O1" s="111"/>
-      <c r="P1" s="111"/>
-      <c r="Q1" s="111"/>
-      <c r="R1" s="111"/>
-      <c r="S1" s="111"/>
-      <c r="T1" s="111"/>
-      <c r="U1" s="111"/>
-      <c r="V1" s="111"/>
-      <c r="W1" s="111"/>
-      <c r="X1" s="111"/>
-      <c r="Y1" s="111"/>
-      <c r="Z1" s="111"/>
-      <c r="AA1" s="111"/>
-      <c r="AB1" s="111"/>
-      <c r="AC1" s="111"/>
-      <c r="AD1" s="111"/>
-      <c r="AE1" s="111"/>
+      <c r="L1" s="117"/>
+      <c r="M1" s="117"/>
+      <c r="N1" s="117"/>
+      <c r="O1" s="117"/>
+      <c r="P1" s="117"/>
+      <c r="Q1" s="117"/>
+      <c r="R1" s="117"/>
+      <c r="S1" s="117"/>
+      <c r="T1" s="117"/>
+      <c r="U1" s="117"/>
+      <c r="V1" s="117"/>
+      <c r="W1" s="117"/>
+      <c r="X1" s="117"/>
+      <c r="Y1" s="117"/>
+      <c r="Z1" s="117"/>
+      <c r="AA1" s="117"/>
+      <c r="AB1" s="117"/>
+      <c r="AC1" s="117"/>
+      <c r="AD1" s="117"/>
+      <c r="AE1" s="117"/>
     </row>
     <row r="2" spans="1:66" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
@@ -3950,196 +3950,196 @@
       <c r="B4" s="65" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="116">
+      <c r="C4" s="119">
         <v>45194</v>
       </c>
-      <c r="D4" s="116"/>
-      <c r="E4" s="116"/>
+      <c r="D4" s="119"/>
+      <c r="E4" s="119"/>
       <c r="F4" s="64"/>
       <c r="G4" s="65" t="s">
         <v>68</v>
       </c>
       <c r="H4" s="77">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="30"/>
-      <c r="K4" s="113" t="str">
+      <c r="K4" s="111" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+        <v>Week 4</v>
+      </c>
+      <c r="L4" s="112"/>
+      <c r="M4" s="112"/>
+      <c r="N4" s="112"/>
+      <c r="O4" s="112"/>
+      <c r="P4" s="112"/>
+      <c r="Q4" s="113"/>
+      <c r="R4" s="111" t="str">
+        <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="L4" s="114"/>
-      <c r="M4" s="114"/>
-      <c r="N4" s="114"/>
-      <c r="O4" s="114"/>
-      <c r="P4" s="114"/>
-      <c r="Q4" s="115"/>
-      <c r="R4" s="113" t="str">
-        <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="S4" s="112"/>
+      <c r="T4" s="112"/>
+      <c r="U4" s="112"/>
+      <c r="V4" s="112"/>
+      <c r="W4" s="112"/>
+      <c r="X4" s="113"/>
+      <c r="Y4" s="111" t="str">
+        <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="S4" s="114"/>
-      <c r="T4" s="114"/>
-      <c r="U4" s="114"/>
-      <c r="V4" s="114"/>
-      <c r="W4" s="114"/>
-      <c r="X4" s="115"/>
-      <c r="Y4" s="113" t="str">
-        <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="Z4" s="112"/>
+      <c r="AA4" s="112"/>
+      <c r="AB4" s="112"/>
+      <c r="AC4" s="112"/>
+      <c r="AD4" s="112"/>
+      <c r="AE4" s="113"/>
+      <c r="AF4" s="111" t="str">
+        <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="Z4" s="114"/>
-      <c r="AA4" s="114"/>
-      <c r="AB4" s="114"/>
-      <c r="AC4" s="114"/>
-      <c r="AD4" s="114"/>
-      <c r="AE4" s="115"/>
-      <c r="AF4" s="113" t="str">
-        <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="AG4" s="112"/>
+      <c r="AH4" s="112"/>
+      <c r="AI4" s="112"/>
+      <c r="AJ4" s="112"/>
+      <c r="AK4" s="112"/>
+      <c r="AL4" s="113"/>
+      <c r="AM4" s="111" t="str">
+        <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="AG4" s="114"/>
-      <c r="AH4" s="114"/>
-      <c r="AI4" s="114"/>
-      <c r="AJ4" s="114"/>
-      <c r="AK4" s="114"/>
-      <c r="AL4" s="115"/>
-      <c r="AM4" s="113" t="str">
-        <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="AN4" s="112"/>
+      <c r="AO4" s="112"/>
+      <c r="AP4" s="112"/>
+      <c r="AQ4" s="112"/>
+      <c r="AR4" s="112"/>
+      <c r="AS4" s="113"/>
+      <c r="AT4" s="111" t="str">
+        <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 9</v>
       </c>
-      <c r="AN4" s="114"/>
-      <c r="AO4" s="114"/>
-      <c r="AP4" s="114"/>
-      <c r="AQ4" s="114"/>
-      <c r="AR4" s="114"/>
-      <c r="AS4" s="115"/>
-      <c r="AT4" s="113" t="str">
-        <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="AU4" s="112"/>
+      <c r="AV4" s="112"/>
+      <c r="AW4" s="112"/>
+      <c r="AX4" s="112"/>
+      <c r="AY4" s="112"/>
+      <c r="AZ4" s="113"/>
+      <c r="BA4" s="111" t="str">
+        <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 10</v>
       </c>
-      <c r="AU4" s="114"/>
-      <c r="AV4" s="114"/>
-      <c r="AW4" s="114"/>
-      <c r="AX4" s="114"/>
-      <c r="AY4" s="114"/>
-      <c r="AZ4" s="115"/>
-      <c r="BA4" s="113" t="str">
-        <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="BB4" s="112"/>
+      <c r="BC4" s="112"/>
+      <c r="BD4" s="112"/>
+      <c r="BE4" s="112"/>
+      <c r="BF4" s="112"/>
+      <c r="BG4" s="113"/>
+      <c r="BH4" s="111" t="str">
+        <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 11</v>
       </c>
-      <c r="BB4" s="114"/>
-      <c r="BC4" s="114"/>
-      <c r="BD4" s="114"/>
-      <c r="BE4" s="114"/>
-      <c r="BF4" s="114"/>
-      <c r="BG4" s="115"/>
-      <c r="BH4" s="113" t="str">
-        <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 12</v>
-      </c>
-      <c r="BI4" s="114"/>
-      <c r="BJ4" s="114"/>
-      <c r="BK4" s="114"/>
-      <c r="BL4" s="114"/>
-      <c r="BM4" s="114"/>
-      <c r="BN4" s="115"/>
+      <c r="BI4" s="112"/>
+      <c r="BJ4" s="112"/>
+      <c r="BK4" s="112"/>
+      <c r="BL4" s="112"/>
+      <c r="BM4" s="112"/>
+      <c r="BN4" s="113"/>
     </row>
     <row r="5" spans="1:66" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="64"/>
       <c r="B5" s="65" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="112" t="s">
+      <c r="C5" s="118" t="s">
         <v>132</v>
       </c>
-      <c r="D5" s="112"/>
-      <c r="E5" s="112"/>
+      <c r="D5" s="118"/>
+      <c r="E5" s="118"/>
       <c r="F5" s="64"/>
       <c r="G5" s="64"/>
       <c r="H5" s="64"/>
       <c r="I5" s="64"/>
       <c r="J5" s="30"/>
-      <c r="K5" s="117">
+      <c r="K5" s="114">
         <f>K6</f>
+        <v>45215</v>
+      </c>
+      <c r="L5" s="115"/>
+      <c r="M5" s="115"/>
+      <c r="N5" s="115"/>
+      <c r="O5" s="115"/>
+      <c r="P5" s="115"/>
+      <c r="Q5" s="116"/>
+      <c r="R5" s="114">
+        <f>R6</f>
         <v>45222</v>
       </c>
-      <c r="L5" s="118"/>
-      <c r="M5" s="118"/>
-      <c r="N5" s="118"/>
-      <c r="O5" s="118"/>
-      <c r="P5" s="118"/>
-      <c r="Q5" s="119"/>
-      <c r="R5" s="117">
-        <f>R6</f>
+      <c r="S5" s="115"/>
+      <c r="T5" s="115"/>
+      <c r="U5" s="115"/>
+      <c r="V5" s="115"/>
+      <c r="W5" s="115"/>
+      <c r="X5" s="116"/>
+      <c r="Y5" s="114">
+        <f>Y6</f>
         <v>45229</v>
       </c>
-      <c r="S5" s="118"/>
-      <c r="T5" s="118"/>
-      <c r="U5" s="118"/>
-      <c r="V5" s="118"/>
-      <c r="W5" s="118"/>
-      <c r="X5" s="119"/>
-      <c r="Y5" s="117">
-        <f>Y6</f>
+      <c r="Z5" s="115"/>
+      <c r="AA5" s="115"/>
+      <c r="AB5" s="115"/>
+      <c r="AC5" s="115"/>
+      <c r="AD5" s="115"/>
+      <c r="AE5" s="116"/>
+      <c r="AF5" s="114">
+        <f>AF6</f>
         <v>45236</v>
       </c>
-      <c r="Z5" s="118"/>
-      <c r="AA5" s="118"/>
-      <c r="AB5" s="118"/>
-      <c r="AC5" s="118"/>
-      <c r="AD5" s="118"/>
-      <c r="AE5" s="119"/>
-      <c r="AF5" s="117">
-        <f>AF6</f>
+      <c r="AG5" s="115"/>
+      <c r="AH5" s="115"/>
+      <c r="AI5" s="115"/>
+      <c r="AJ5" s="115"/>
+      <c r="AK5" s="115"/>
+      <c r="AL5" s="116"/>
+      <c r="AM5" s="114">
+        <f>AM6</f>
         <v>45243</v>
       </c>
-      <c r="AG5" s="118"/>
-      <c r="AH5" s="118"/>
-      <c r="AI5" s="118"/>
-      <c r="AJ5" s="118"/>
-      <c r="AK5" s="118"/>
-      <c r="AL5" s="119"/>
-      <c r="AM5" s="117">
-        <f>AM6</f>
+      <c r="AN5" s="115"/>
+      <c r="AO5" s="115"/>
+      <c r="AP5" s="115"/>
+      <c r="AQ5" s="115"/>
+      <c r="AR5" s="115"/>
+      <c r="AS5" s="116"/>
+      <c r="AT5" s="114">
+        <f>AT6</f>
         <v>45250</v>
       </c>
-      <c r="AN5" s="118"/>
-      <c r="AO5" s="118"/>
-      <c r="AP5" s="118"/>
-      <c r="AQ5" s="118"/>
-      <c r="AR5" s="118"/>
-      <c r="AS5" s="119"/>
-      <c r="AT5" s="117">
-        <f>AT6</f>
+      <c r="AU5" s="115"/>
+      <c r="AV5" s="115"/>
+      <c r="AW5" s="115"/>
+      <c r="AX5" s="115"/>
+      <c r="AY5" s="115"/>
+      <c r="AZ5" s="116"/>
+      <c r="BA5" s="114">
+        <f>BA6</f>
         <v>45257</v>
       </c>
-      <c r="AU5" s="118"/>
-      <c r="AV5" s="118"/>
-      <c r="AW5" s="118"/>
-      <c r="AX5" s="118"/>
-      <c r="AY5" s="118"/>
-      <c r="AZ5" s="119"/>
-      <c r="BA5" s="117">
-        <f>BA6</f>
+      <c r="BB5" s="115"/>
+      <c r="BC5" s="115"/>
+      <c r="BD5" s="115"/>
+      <c r="BE5" s="115"/>
+      <c r="BF5" s="115"/>
+      <c r="BG5" s="116"/>
+      <c r="BH5" s="114">
+        <f>BH6</f>
         <v>45264</v>
       </c>
-      <c r="BB5" s="118"/>
-      <c r="BC5" s="118"/>
-      <c r="BD5" s="118"/>
-      <c r="BE5" s="118"/>
-      <c r="BF5" s="118"/>
-      <c r="BG5" s="119"/>
-      <c r="BH5" s="117">
-        <f>BH6</f>
-        <v>45271</v>
-      </c>
-      <c r="BI5" s="118"/>
-      <c r="BJ5" s="118"/>
-      <c r="BK5" s="118"/>
-      <c r="BL5" s="118"/>
-      <c r="BM5" s="118"/>
-      <c r="BN5" s="119"/>
+      <c r="BI5" s="115"/>
+      <c r="BJ5" s="115"/>
+      <c r="BK5" s="115"/>
+      <c r="BL5" s="115"/>
+      <c r="BM5" s="115"/>
+      <c r="BN5" s="116"/>
     </row>
     <row r="6" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A6" s="30"/>
@@ -4154,227 +4154,227 @@
       <c r="J6" s="30"/>
       <c r="K6" s="53">
         <f>C4-WEEKDAY(C4,1)+2+7*(H4-1)</f>
-        <v>45222</v>
+        <v>45215</v>
       </c>
       <c r="L6" s="44">
         <f t="shared" ref="L6:AQ6" si="0">K6+1</f>
-        <v>45223</v>
+        <v>45216</v>
       </c>
       <c r="M6" s="44">
         <f t="shared" si="0"/>
-        <v>45224</v>
+        <v>45217</v>
       </c>
       <c r="N6" s="44">
         <f t="shared" si="0"/>
-        <v>45225</v>
+        <v>45218</v>
       </c>
       <c r="O6" s="44">
         <f t="shared" si="0"/>
-        <v>45226</v>
+        <v>45219</v>
       </c>
       <c r="P6" s="44">
         <f t="shared" si="0"/>
-        <v>45227</v>
+        <v>45220</v>
       </c>
       <c r="Q6" s="54">
         <f t="shared" si="0"/>
-        <v>45228</v>
+        <v>45221</v>
       </c>
       <c r="R6" s="53">
         <f t="shared" si="0"/>
-        <v>45229</v>
+        <v>45222</v>
       </c>
       <c r="S6" s="44">
         <f t="shared" si="0"/>
-        <v>45230</v>
+        <v>45223</v>
       </c>
       <c r="T6" s="44">
         <f t="shared" si="0"/>
-        <v>45231</v>
+        <v>45224</v>
       </c>
       <c r="U6" s="44">
         <f t="shared" si="0"/>
-        <v>45232</v>
+        <v>45225</v>
       </c>
       <c r="V6" s="44">
         <f t="shared" si="0"/>
-        <v>45233</v>
+        <v>45226</v>
       </c>
       <c r="W6" s="44">
         <f t="shared" si="0"/>
-        <v>45234</v>
+        <v>45227</v>
       </c>
       <c r="X6" s="54">
         <f t="shared" si="0"/>
-        <v>45235</v>
+        <v>45228</v>
       </c>
       <c r="Y6" s="53">
         <f t="shared" si="0"/>
-        <v>45236</v>
+        <v>45229</v>
       </c>
       <c r="Z6" s="44">
         <f t="shared" si="0"/>
-        <v>45237</v>
+        <v>45230</v>
       </c>
       <c r="AA6" s="44">
         <f t="shared" si="0"/>
-        <v>45238</v>
+        <v>45231</v>
       </c>
       <c r="AB6" s="44">
         <f t="shared" si="0"/>
-        <v>45239</v>
+        <v>45232</v>
       </c>
       <c r="AC6" s="44">
         <f t="shared" si="0"/>
-        <v>45240</v>
+        <v>45233</v>
       </c>
       <c r="AD6" s="44">
         <f t="shared" si="0"/>
-        <v>45241</v>
+        <v>45234</v>
       </c>
       <c r="AE6" s="54">
         <f t="shared" si="0"/>
-        <v>45242</v>
+        <v>45235</v>
       </c>
       <c r="AF6" s="53">
         <f t="shared" si="0"/>
-        <v>45243</v>
+        <v>45236</v>
       </c>
       <c r="AG6" s="44">
         <f t="shared" si="0"/>
-        <v>45244</v>
+        <v>45237</v>
       </c>
       <c r="AH6" s="44">
         <f t="shared" si="0"/>
-        <v>45245</v>
+        <v>45238</v>
       </c>
       <c r="AI6" s="44">
         <f t="shared" si="0"/>
-        <v>45246</v>
+        <v>45239</v>
       </c>
       <c r="AJ6" s="44">
         <f t="shared" si="0"/>
-        <v>45247</v>
+        <v>45240</v>
       </c>
       <c r="AK6" s="44">
         <f t="shared" si="0"/>
-        <v>45248</v>
+        <v>45241</v>
       </c>
       <c r="AL6" s="54">
         <f t="shared" si="0"/>
-        <v>45249</v>
+        <v>45242</v>
       </c>
       <c r="AM6" s="53">
         <f t="shared" si="0"/>
-        <v>45250</v>
+        <v>45243</v>
       </c>
       <c r="AN6" s="44">
         <f t="shared" si="0"/>
-        <v>45251</v>
+        <v>45244</v>
       </c>
       <c r="AO6" s="44">
         <f t="shared" si="0"/>
-        <v>45252</v>
+        <v>45245</v>
       </c>
       <c r="AP6" s="44">
         <f t="shared" si="0"/>
-        <v>45253</v>
+        <v>45246</v>
       </c>
       <c r="AQ6" s="44">
         <f t="shared" si="0"/>
-        <v>45254</v>
+        <v>45247</v>
       </c>
       <c r="AR6" s="44">
         <f t="shared" ref="AR6:BN6" si="1">AQ6+1</f>
-        <v>45255</v>
+        <v>45248</v>
       </c>
       <c r="AS6" s="54">
         <f t="shared" si="1"/>
-        <v>45256</v>
+        <v>45249</v>
       </c>
       <c r="AT6" s="53">
         <f t="shared" si="1"/>
-        <v>45257</v>
+        <v>45250</v>
       </c>
       <c r="AU6" s="44">
         <f t="shared" si="1"/>
-        <v>45258</v>
+        <v>45251</v>
       </c>
       <c r="AV6" s="44">
         <f t="shared" si="1"/>
-        <v>45259</v>
+        <v>45252</v>
       </c>
       <c r="AW6" s="44">
         <f t="shared" si="1"/>
-        <v>45260</v>
+        <v>45253</v>
       </c>
       <c r="AX6" s="44">
         <f t="shared" si="1"/>
-        <v>45261</v>
+        <v>45254</v>
       </c>
       <c r="AY6" s="44">
         <f t="shared" si="1"/>
-        <v>45262</v>
+        <v>45255</v>
       </c>
       <c r="AZ6" s="54">
         <f t="shared" si="1"/>
-        <v>45263</v>
+        <v>45256</v>
       </c>
       <c r="BA6" s="53">
         <f t="shared" si="1"/>
-        <v>45264</v>
+        <v>45257</v>
       </c>
       <c r="BB6" s="44">
         <f t="shared" si="1"/>
-        <v>45265</v>
+        <v>45258</v>
       </c>
       <c r="BC6" s="44">
         <f t="shared" si="1"/>
-        <v>45266</v>
+        <v>45259</v>
       </c>
       <c r="BD6" s="44">
         <f t="shared" si="1"/>
-        <v>45267</v>
+        <v>45260</v>
       </c>
       <c r="BE6" s="44">
         <f t="shared" si="1"/>
-        <v>45268</v>
+        <v>45261</v>
       </c>
       <c r="BF6" s="44">
         <f t="shared" si="1"/>
-        <v>45269</v>
+        <v>45262</v>
       </c>
       <c r="BG6" s="54">
         <f t="shared" si="1"/>
-        <v>45270</v>
+        <v>45263</v>
       </c>
       <c r="BH6" s="53">
         <f t="shared" si="1"/>
-        <v>45271</v>
+        <v>45264</v>
       </c>
       <c r="BI6" s="44">
         <f t="shared" si="1"/>
-        <v>45272</v>
+        <v>45265</v>
       </c>
       <c r="BJ6" s="44">
         <f t="shared" si="1"/>
-        <v>45273</v>
+        <v>45266</v>
       </c>
       <c r="BK6" s="44">
         <f t="shared" si="1"/>
-        <v>45274</v>
+        <v>45267</v>
       </c>
       <c r="BL6" s="44">
         <f t="shared" si="1"/>
-        <v>45275</v>
+        <v>45268</v>
       </c>
       <c r="BM6" s="44">
         <f t="shared" si="1"/>
-        <v>45276</v>
+        <v>45269</v>
       </c>
       <c r="BN6" s="54">
         <f t="shared" si="1"/>
-        <v>45277</v>
+        <v>45270</v>
       </c>
     </row>
     <row r="7" spans="1:66" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -5785,7 +5785,7 @@
         <v>2</v>
       </c>
       <c r="H21" s="108">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="I21" s="109">
         <f t="shared" si="4"/>
@@ -5873,7 +5873,7 @@
         <v>1</v>
       </c>
       <c r="H22" s="108">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" s="109">
         <f t="shared" ref="I22" si="11">IF(OR(F22=0,E22=0)," - ",NETWORKDAYS(E22,F22))</f>
@@ -6043,7 +6043,7 @@
         <v>2</v>
       </c>
       <c r="H24" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24" s="43">
         <f t="shared" si="4"/>
@@ -7771,7 +7771,7 @@
     </row>
     <row r="44" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" s="39" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A44:A51" si="24">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>5.1</v>
       </c>
       <c r="B44" s="75" t="s">
@@ -7859,7 +7859,7 @@
     </row>
     <row r="45" spans="1:66" s="40" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A45" s="39" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" si="24"/>
         <v>5.2</v>
       </c>
       <c r="B45" s="75" t="s">
@@ -7874,7 +7874,7 @@
         <v>45237</v>
       </c>
       <c r="F45" s="59">
-        <f t="shared" ref="F45" si="24">IF(ISBLANK(E45)," - ",IF(G45=0,E45,E45+G45-1))</f>
+        <f t="shared" ref="F45" si="25">IF(ISBLANK(E45)," - ",IF(G45=0,E45,E45+G45-1))</f>
         <v>45240</v>
       </c>
       <c r="G45" s="41">
@@ -7884,7 +7884,7 @@
         <v>0</v>
       </c>
       <c r="I45" s="43">
-        <f t="shared" ref="I45" si="25">IF(OR(F45=0,E45=0)," - ",NETWORKDAYS(E45,F45))</f>
+        <f t="shared" ref="I45" si="26">IF(OR(F45=0,E45=0)," - ",NETWORKDAYS(E45,F45))</f>
         <v>4</v>
       </c>
       <c r="J45" s="56"/>
@@ -7947,7 +7947,7 @@
     </row>
     <row r="46" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" s="39" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" si="24"/>
         <v>5.3</v>
       </c>
       <c r="B46" s="75" t="s">
@@ -8035,7 +8035,7 @@
     </row>
     <row r="47" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" s="39" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" si="24"/>
         <v>5.4</v>
       </c>
       <c r="B47" s="75" t="s">
@@ -8123,7 +8123,7 @@
     </row>
     <row r="48" spans="1:66" s="40" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A48" s="39" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" si="24"/>
         <v>5.5</v>
       </c>
       <c r="B48" s="75" t="s">
@@ -8211,7 +8211,7 @@
     </row>
     <row r="49" spans="1:66" s="40" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A49" s="39" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" si="24"/>
         <v>5.6</v>
       </c>
       <c r="B49" s="75" t="s">
@@ -8226,7 +8226,7 @@
         <v>45243</v>
       </c>
       <c r="F49" s="59">
-        <f t="shared" ref="F49" si="26">IF(ISBLANK(E49)," - ",IF(G49=0,E49,E49+G49-1))</f>
+        <f t="shared" ref="F49" si="27">IF(ISBLANK(E49)," - ",IF(G49=0,E49,E49+G49-1))</f>
         <v>45245</v>
       </c>
       <c r="G49" s="41">
@@ -8236,7 +8236,7 @@
         <v>0</v>
       </c>
       <c r="I49" s="43">
-        <f t="shared" ref="I49" si="27">IF(OR(F49=0,E49=0)," - ",NETWORKDAYS(E49,F49))</f>
+        <f t="shared" ref="I49" si="28">IF(OR(F49=0,E49=0)," - ",NETWORKDAYS(E49,F49))</f>
         <v>3</v>
       </c>
       <c r="J49" s="56"/>
@@ -8299,7 +8299,7 @@
     </row>
     <row r="50" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A50" s="39" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" si="24"/>
         <v>5.7</v>
       </c>
       <c r="B50" s="75" t="s">
@@ -8387,7 +8387,7 @@
     </row>
     <row r="51" spans="1:66" s="40" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A51" s="39" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" si="24"/>
         <v>5.8</v>
       </c>
       <c r="B51" s="75" t="s">
@@ -8487,7 +8487,7 @@
         <v>45250</v>
       </c>
       <c r="F52" s="60">
-        <f t="shared" ref="F52" si="28">IF(ISBLANK(E52)," - ",IF(G52=0,E52,E52+G52-1))</f>
+        <f t="shared" ref="F52" si="29">IF(ISBLANK(E52)," - ",IF(G52=0,E52,E52+G52-1))</f>
         <v>45254</v>
       </c>
       <c r="G52" s="36">
@@ -8495,7 +8495,7 @@
       </c>
       <c r="H52" s="37"/>
       <c r="I52" s="38">
-        <f t="shared" ref="I52" si="29">IF(OR(F52=0,E52=0)," - ",NETWORKDAYS(E52,F52))</f>
+        <f t="shared" ref="I52" si="30">IF(OR(F52=0,E52=0)," - ",NETWORKDAYS(E52,F52))</f>
         <v>5</v>
       </c>
       <c r="J52" s="57"/>
@@ -8661,7 +8661,7 @@
         <v>45252</v>
       </c>
       <c r="F54" s="59">
-        <f t="shared" ref="F54" si="30">IF(ISBLANK(E54)," - ",IF(G54=0,E54,E54+G54-1))</f>
+        <f t="shared" ref="F54" si="31">IF(ISBLANK(E54)," - ",IF(G54=0,E54,E54+G54-1))</f>
         <v>45252</v>
       </c>
       <c r="G54" s="41">
@@ -8671,7 +8671,7 @@
         <v>0</v>
       </c>
       <c r="I54" s="43">
-        <f t="shared" ref="I54" si="31">IF(OR(F54=0,E54=0)," - ",NETWORKDAYS(E54,F54))</f>
+        <f t="shared" ref="I54" si="32">IF(OR(F54=0,E54=0)," - ",NETWORKDAYS(E54,F54))</f>
         <v>1</v>
       </c>
       <c r="J54" s="56"/>
@@ -8999,6 +8999,15 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -9009,15 +9018,6 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H8:H13 H23:H28 H15:H21 H37:H41 H48:H51">
@@ -9241,7 +9241,7 @@
   <pageSetup scale="63" fitToHeight="0" orientation="landscape" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <ignoredErrors>
-    <ignoredError sqref="H9 H12 G25:H25 H23 H24 G26:H26" unlockedFormula="1"/>
+    <ignoredError sqref="H9 H12 G25:H25 H23 G26:H26" unlockedFormula="1"/>
     <ignoredError sqref="A23 A12" formula="1"/>
   </ignoredErrors>
   <drawing r:id="rId3"/>

</xml_diff>

<commit_message>
docs (gantt): update status workload
</commit_message>
<xml_diff>
--- a/docs/Gantt Chart.xlsx
+++ b/docs/Gantt Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\punch\Documents\GitHub\warawiriweb\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ECF10C8-DCBF-4F39-B07E-5B79D7F254CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901A7179-DF63-4147-9352-737DCDB1F50C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2875,6 +2875,13 @@
     <xf numFmtId="1" fontId="50" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="45" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2884,6 +2891,10 @@
     <xf numFmtId="0" fontId="48" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="45" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="167" fontId="45" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2892,17 +2903,6 @@
     </xf>
     <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="45" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="45" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3201,7 +3201,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$H$4" horiz="1" max="100" min="1" page="0" val="4"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$H$4" horiz="1" max="100" min="1" page="0" val="5"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3860,8 +3860,8 @@
   <dimension ref="A1:BN57"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T30" sqref="T30"/>
+      <pane ySplit="7" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R33" sqref="R33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3888,29 +3888,29 @@
       <c r="E1" s="29"/>
       <c r="F1" s="29"/>
       <c r="I1" s="78"/>
-      <c r="K1" s="117" t="s">
+      <c r="K1" s="111" t="s">
         <v>71</v>
       </c>
-      <c r="L1" s="117"/>
-      <c r="M1" s="117"/>
-      <c r="N1" s="117"/>
-      <c r="O1" s="117"/>
-      <c r="P1" s="117"/>
-      <c r="Q1" s="117"/>
-      <c r="R1" s="117"/>
-      <c r="S1" s="117"/>
-      <c r="T1" s="117"/>
-      <c r="U1" s="117"/>
-      <c r="V1" s="117"/>
-      <c r="W1" s="117"/>
-      <c r="X1" s="117"/>
-      <c r="Y1" s="117"/>
-      <c r="Z1" s="117"/>
-      <c r="AA1" s="117"/>
-      <c r="AB1" s="117"/>
-      <c r="AC1" s="117"/>
-      <c r="AD1" s="117"/>
-      <c r="AE1" s="117"/>
+      <c r="L1" s="111"/>
+      <c r="M1" s="111"/>
+      <c r="N1" s="111"/>
+      <c r="O1" s="111"/>
+      <c r="P1" s="111"/>
+      <c r="Q1" s="111"/>
+      <c r="R1" s="111"/>
+      <c r="S1" s="111"/>
+      <c r="T1" s="111"/>
+      <c r="U1" s="111"/>
+      <c r="V1" s="111"/>
+      <c r="W1" s="111"/>
+      <c r="X1" s="111"/>
+      <c r="Y1" s="111"/>
+      <c r="Z1" s="111"/>
+      <c r="AA1" s="111"/>
+      <c r="AB1" s="111"/>
+      <c r="AC1" s="111"/>
+      <c r="AD1" s="111"/>
+      <c r="AE1" s="111"/>
     </row>
     <row r="2" spans="1:66" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
@@ -3950,196 +3950,196 @@
       <c r="B4" s="65" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="119">
+      <c r="C4" s="116">
         <v>45194</v>
       </c>
-      <c r="D4" s="119"/>
-      <c r="E4" s="119"/>
+      <c r="D4" s="116"/>
+      <c r="E4" s="116"/>
       <c r="F4" s="64"/>
       <c r="G4" s="65" t="s">
         <v>68</v>
       </c>
       <c r="H4" s="77">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="30"/>
-      <c r="K4" s="111" t="str">
+      <c r="K4" s="113" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 4</v>
-      </c>
-      <c r="L4" s="112"/>
-      <c r="M4" s="112"/>
-      <c r="N4" s="112"/>
-      <c r="O4" s="112"/>
-      <c r="P4" s="112"/>
-      <c r="Q4" s="113"/>
-      <c r="R4" s="111" t="str">
+        <v>Week 5</v>
+      </c>
+      <c r="L4" s="114"/>
+      <c r="M4" s="114"/>
+      <c r="N4" s="114"/>
+      <c r="O4" s="114"/>
+      <c r="P4" s="114"/>
+      <c r="Q4" s="115"/>
+      <c r="R4" s="113" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 5</v>
-      </c>
-      <c r="S4" s="112"/>
-      <c r="T4" s="112"/>
-      <c r="U4" s="112"/>
-      <c r="V4" s="112"/>
-      <c r="W4" s="112"/>
-      <c r="X4" s="113"/>
-      <c r="Y4" s="111" t="str">
+        <v>Week 6</v>
+      </c>
+      <c r="S4" s="114"/>
+      <c r="T4" s="114"/>
+      <c r="U4" s="114"/>
+      <c r="V4" s="114"/>
+      <c r="W4" s="114"/>
+      <c r="X4" s="115"/>
+      <c r="Y4" s="113" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 6</v>
-      </c>
-      <c r="Z4" s="112"/>
-      <c r="AA4" s="112"/>
-      <c r="AB4" s="112"/>
-      <c r="AC4" s="112"/>
-      <c r="AD4" s="112"/>
-      <c r="AE4" s="113"/>
-      <c r="AF4" s="111" t="str">
+        <v>Week 7</v>
+      </c>
+      <c r="Z4" s="114"/>
+      <c r="AA4" s="114"/>
+      <c r="AB4" s="114"/>
+      <c r="AC4" s="114"/>
+      <c r="AD4" s="114"/>
+      <c r="AE4" s="115"/>
+      <c r="AF4" s="113" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 7</v>
-      </c>
-      <c r="AG4" s="112"/>
-      <c r="AH4" s="112"/>
-      <c r="AI4" s="112"/>
-      <c r="AJ4" s="112"/>
-      <c r="AK4" s="112"/>
-      <c r="AL4" s="113"/>
-      <c r="AM4" s="111" t="str">
+        <v>Week 8</v>
+      </c>
+      <c r="AG4" s="114"/>
+      <c r="AH4" s="114"/>
+      <c r="AI4" s="114"/>
+      <c r="AJ4" s="114"/>
+      <c r="AK4" s="114"/>
+      <c r="AL4" s="115"/>
+      <c r="AM4" s="113" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 8</v>
-      </c>
-      <c r="AN4" s="112"/>
-      <c r="AO4" s="112"/>
-      <c r="AP4" s="112"/>
-      <c r="AQ4" s="112"/>
-      <c r="AR4" s="112"/>
-      <c r="AS4" s="113"/>
-      <c r="AT4" s="111" t="str">
+        <v>Week 9</v>
+      </c>
+      <c r="AN4" s="114"/>
+      <c r="AO4" s="114"/>
+      <c r="AP4" s="114"/>
+      <c r="AQ4" s="114"/>
+      <c r="AR4" s="114"/>
+      <c r="AS4" s="115"/>
+      <c r="AT4" s="113" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 9</v>
-      </c>
-      <c r="AU4" s="112"/>
-      <c r="AV4" s="112"/>
-      <c r="AW4" s="112"/>
-      <c r="AX4" s="112"/>
-      <c r="AY4" s="112"/>
-      <c r="AZ4" s="113"/>
-      <c r="BA4" s="111" t="str">
+        <v>Week 10</v>
+      </c>
+      <c r="AU4" s="114"/>
+      <c r="AV4" s="114"/>
+      <c r="AW4" s="114"/>
+      <c r="AX4" s="114"/>
+      <c r="AY4" s="114"/>
+      <c r="AZ4" s="115"/>
+      <c r="BA4" s="113" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 10</v>
-      </c>
-      <c r="BB4" s="112"/>
-      <c r="BC4" s="112"/>
-      <c r="BD4" s="112"/>
-      <c r="BE4" s="112"/>
-      <c r="BF4" s="112"/>
-      <c r="BG4" s="113"/>
-      <c r="BH4" s="111" t="str">
+        <v>Week 11</v>
+      </c>
+      <c r="BB4" s="114"/>
+      <c r="BC4" s="114"/>
+      <c r="BD4" s="114"/>
+      <c r="BE4" s="114"/>
+      <c r="BF4" s="114"/>
+      <c r="BG4" s="115"/>
+      <c r="BH4" s="113" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 11</v>
-      </c>
-      <c r="BI4" s="112"/>
-      <c r="BJ4" s="112"/>
-      <c r="BK4" s="112"/>
-      <c r="BL4" s="112"/>
-      <c r="BM4" s="112"/>
-      <c r="BN4" s="113"/>
+        <v>Week 12</v>
+      </c>
+      <c r="BI4" s="114"/>
+      <c r="BJ4" s="114"/>
+      <c r="BK4" s="114"/>
+      <c r="BL4" s="114"/>
+      <c r="BM4" s="114"/>
+      <c r="BN4" s="115"/>
     </row>
     <row r="5" spans="1:66" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="64"/>
       <c r="B5" s="65" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="118" t="s">
+      <c r="C5" s="112" t="s">
         <v>132</v>
       </c>
-      <c r="D5" s="118"/>
-      <c r="E5" s="118"/>
+      <c r="D5" s="112"/>
+      <c r="E5" s="112"/>
       <c r="F5" s="64"/>
       <c r="G5" s="64"/>
       <c r="H5" s="64"/>
       <c r="I5" s="64"/>
       <c r="J5" s="30"/>
-      <c r="K5" s="114">
+      <c r="K5" s="117">
         <f>K6</f>
-        <v>45215</v>
-      </c>
-      <c r="L5" s="115"/>
-      <c r="M5" s="115"/>
-      <c r="N5" s="115"/>
-      <c r="O5" s="115"/>
-      <c r="P5" s="115"/>
-      <c r="Q5" s="116"/>
-      <c r="R5" s="114">
+        <v>45222</v>
+      </c>
+      <c r="L5" s="118"/>
+      <c r="M5" s="118"/>
+      <c r="N5" s="118"/>
+      <c r="O5" s="118"/>
+      <c r="P5" s="118"/>
+      <c r="Q5" s="119"/>
+      <c r="R5" s="117">
         <f>R6</f>
-        <v>45222</v>
-      </c>
-      <c r="S5" s="115"/>
-      <c r="T5" s="115"/>
-      <c r="U5" s="115"/>
-      <c r="V5" s="115"/>
-      <c r="W5" s="115"/>
-      <c r="X5" s="116"/>
-      <c r="Y5" s="114">
+        <v>45229</v>
+      </c>
+      <c r="S5" s="118"/>
+      <c r="T5" s="118"/>
+      <c r="U5" s="118"/>
+      <c r="V5" s="118"/>
+      <c r="W5" s="118"/>
+      <c r="X5" s="119"/>
+      <c r="Y5" s="117">
         <f>Y6</f>
-        <v>45229</v>
-      </c>
-      <c r="Z5" s="115"/>
-      <c r="AA5" s="115"/>
-      <c r="AB5" s="115"/>
-      <c r="AC5" s="115"/>
-      <c r="AD5" s="115"/>
-      <c r="AE5" s="116"/>
-      <c r="AF5" s="114">
+        <v>45236</v>
+      </c>
+      <c r="Z5" s="118"/>
+      <c r="AA5" s="118"/>
+      <c r="AB5" s="118"/>
+      <c r="AC5" s="118"/>
+      <c r="AD5" s="118"/>
+      <c r="AE5" s="119"/>
+      <c r="AF5" s="117">
         <f>AF6</f>
-        <v>45236</v>
-      </c>
-      <c r="AG5" s="115"/>
-      <c r="AH5" s="115"/>
-      <c r="AI5" s="115"/>
-      <c r="AJ5" s="115"/>
-      <c r="AK5" s="115"/>
-      <c r="AL5" s="116"/>
-      <c r="AM5" s="114">
+        <v>45243</v>
+      </c>
+      <c r="AG5" s="118"/>
+      <c r="AH5" s="118"/>
+      <c r="AI5" s="118"/>
+      <c r="AJ5" s="118"/>
+      <c r="AK5" s="118"/>
+      <c r="AL5" s="119"/>
+      <c r="AM5" s="117">
         <f>AM6</f>
-        <v>45243</v>
-      </c>
-      <c r="AN5" s="115"/>
-      <c r="AO5" s="115"/>
-      <c r="AP5" s="115"/>
-      <c r="AQ5" s="115"/>
-      <c r="AR5" s="115"/>
-      <c r="AS5" s="116"/>
-      <c r="AT5" s="114">
+        <v>45250</v>
+      </c>
+      <c r="AN5" s="118"/>
+      <c r="AO5" s="118"/>
+      <c r="AP5" s="118"/>
+      <c r="AQ5" s="118"/>
+      <c r="AR5" s="118"/>
+      <c r="AS5" s="119"/>
+      <c r="AT5" s="117">
         <f>AT6</f>
-        <v>45250</v>
-      </c>
-      <c r="AU5" s="115"/>
-      <c r="AV5" s="115"/>
-      <c r="AW5" s="115"/>
-      <c r="AX5" s="115"/>
-      <c r="AY5" s="115"/>
-      <c r="AZ5" s="116"/>
-      <c r="BA5" s="114">
+        <v>45257</v>
+      </c>
+      <c r="AU5" s="118"/>
+      <c r="AV5" s="118"/>
+      <c r="AW5" s="118"/>
+      <c r="AX5" s="118"/>
+      <c r="AY5" s="118"/>
+      <c r="AZ5" s="119"/>
+      <c r="BA5" s="117">
         <f>BA6</f>
-        <v>45257</v>
-      </c>
-      <c r="BB5" s="115"/>
-      <c r="BC5" s="115"/>
-      <c r="BD5" s="115"/>
-      <c r="BE5" s="115"/>
-      <c r="BF5" s="115"/>
-      <c r="BG5" s="116"/>
-      <c r="BH5" s="114">
+        <v>45264</v>
+      </c>
+      <c r="BB5" s="118"/>
+      <c r="BC5" s="118"/>
+      <c r="BD5" s="118"/>
+      <c r="BE5" s="118"/>
+      <c r="BF5" s="118"/>
+      <c r="BG5" s="119"/>
+      <c r="BH5" s="117">
         <f>BH6</f>
-        <v>45264</v>
-      </c>
-      <c r="BI5" s="115"/>
-      <c r="BJ5" s="115"/>
-      <c r="BK5" s="115"/>
-      <c r="BL5" s="115"/>
-      <c r="BM5" s="115"/>
-      <c r="BN5" s="116"/>
+        <v>45271</v>
+      </c>
+      <c r="BI5" s="118"/>
+      <c r="BJ5" s="118"/>
+      <c r="BK5" s="118"/>
+      <c r="BL5" s="118"/>
+      <c r="BM5" s="118"/>
+      <c r="BN5" s="119"/>
     </row>
     <row r="6" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A6" s="30"/>
@@ -4154,227 +4154,227 @@
       <c r="J6" s="30"/>
       <c r="K6" s="53">
         <f>C4-WEEKDAY(C4,1)+2+7*(H4-1)</f>
-        <v>45215</v>
+        <v>45222</v>
       </c>
       <c r="L6" s="44">
         <f t="shared" ref="L6:AQ6" si="0">K6+1</f>
-        <v>45216</v>
+        <v>45223</v>
       </c>
       <c r="M6" s="44">
         <f t="shared" si="0"/>
-        <v>45217</v>
+        <v>45224</v>
       </c>
       <c r="N6" s="44">
         <f t="shared" si="0"/>
-        <v>45218</v>
+        <v>45225</v>
       </c>
       <c r="O6" s="44">
         <f t="shared" si="0"/>
-        <v>45219</v>
+        <v>45226</v>
       </c>
       <c r="P6" s="44">
         <f t="shared" si="0"/>
-        <v>45220</v>
+        <v>45227</v>
       </c>
       <c r="Q6" s="54">
         <f t="shared" si="0"/>
-        <v>45221</v>
+        <v>45228</v>
       </c>
       <c r="R6" s="53">
         <f t="shared" si="0"/>
-        <v>45222</v>
+        <v>45229</v>
       </c>
       <c r="S6" s="44">
         <f t="shared" si="0"/>
-        <v>45223</v>
+        <v>45230</v>
       </c>
       <c r="T6" s="44">
         <f t="shared" si="0"/>
-        <v>45224</v>
+        <v>45231</v>
       </c>
       <c r="U6" s="44">
         <f t="shared" si="0"/>
-        <v>45225</v>
+        <v>45232</v>
       </c>
       <c r="V6" s="44">
         <f t="shared" si="0"/>
-        <v>45226</v>
+        <v>45233</v>
       </c>
       <c r="W6" s="44">
         <f t="shared" si="0"/>
-        <v>45227</v>
+        <v>45234</v>
       </c>
       <c r="X6" s="54">
         <f t="shared" si="0"/>
-        <v>45228</v>
+        <v>45235</v>
       </c>
       <c r="Y6" s="53">
         <f t="shared" si="0"/>
-        <v>45229</v>
+        <v>45236</v>
       </c>
       <c r="Z6" s="44">
         <f t="shared" si="0"/>
-        <v>45230</v>
+        <v>45237</v>
       </c>
       <c r="AA6" s="44">
         <f t="shared" si="0"/>
-        <v>45231</v>
+        <v>45238</v>
       </c>
       <c r="AB6" s="44">
         <f t="shared" si="0"/>
-        <v>45232</v>
+        <v>45239</v>
       </c>
       <c r="AC6" s="44">
         <f t="shared" si="0"/>
-        <v>45233</v>
+        <v>45240</v>
       </c>
       <c r="AD6" s="44">
         <f t="shared" si="0"/>
-        <v>45234</v>
+        <v>45241</v>
       </c>
       <c r="AE6" s="54">
         <f t="shared" si="0"/>
-        <v>45235</v>
+        <v>45242</v>
       </c>
       <c r="AF6" s="53">
         <f t="shared" si="0"/>
-        <v>45236</v>
+        <v>45243</v>
       </c>
       <c r="AG6" s="44">
         <f t="shared" si="0"/>
-        <v>45237</v>
+        <v>45244</v>
       </c>
       <c r="AH6" s="44">
         <f t="shared" si="0"/>
-        <v>45238</v>
+        <v>45245</v>
       </c>
       <c r="AI6" s="44">
         <f t="shared" si="0"/>
-        <v>45239</v>
+        <v>45246</v>
       </c>
       <c r="AJ6" s="44">
         <f t="shared" si="0"/>
-        <v>45240</v>
+        <v>45247</v>
       </c>
       <c r="AK6" s="44">
         <f t="shared" si="0"/>
-        <v>45241</v>
+        <v>45248</v>
       </c>
       <c r="AL6" s="54">
         <f t="shared" si="0"/>
-        <v>45242</v>
+        <v>45249</v>
       </c>
       <c r="AM6" s="53">
         <f t="shared" si="0"/>
-        <v>45243</v>
+        <v>45250</v>
       </c>
       <c r="AN6" s="44">
         <f t="shared" si="0"/>
-        <v>45244</v>
+        <v>45251</v>
       </c>
       <c r="AO6" s="44">
         <f t="shared" si="0"/>
-        <v>45245</v>
+        <v>45252</v>
       </c>
       <c r="AP6" s="44">
         <f t="shared" si="0"/>
-        <v>45246</v>
+        <v>45253</v>
       </c>
       <c r="AQ6" s="44">
         <f t="shared" si="0"/>
-        <v>45247</v>
+        <v>45254</v>
       </c>
       <c r="AR6" s="44">
         <f t="shared" ref="AR6:BN6" si="1">AQ6+1</f>
-        <v>45248</v>
+        <v>45255</v>
       </c>
       <c r="AS6" s="54">
         <f t="shared" si="1"/>
-        <v>45249</v>
+        <v>45256</v>
       </c>
       <c r="AT6" s="53">
         <f t="shared" si="1"/>
-        <v>45250</v>
+        <v>45257</v>
       </c>
       <c r="AU6" s="44">
         <f t="shared" si="1"/>
-        <v>45251</v>
+        <v>45258</v>
       </c>
       <c r="AV6" s="44">
         <f t="shared" si="1"/>
-        <v>45252</v>
+        <v>45259</v>
       </c>
       <c r="AW6" s="44">
         <f t="shared" si="1"/>
-        <v>45253</v>
+        <v>45260</v>
       </c>
       <c r="AX6" s="44">
         <f t="shared" si="1"/>
-        <v>45254</v>
+        <v>45261</v>
       </c>
       <c r="AY6" s="44">
         <f t="shared" si="1"/>
-        <v>45255</v>
+        <v>45262</v>
       </c>
       <c r="AZ6" s="54">
         <f t="shared" si="1"/>
-        <v>45256</v>
+        <v>45263</v>
       </c>
       <c r="BA6" s="53">
         <f t="shared" si="1"/>
-        <v>45257</v>
+        <v>45264</v>
       </c>
       <c r="BB6" s="44">
         <f t="shared" si="1"/>
-        <v>45258</v>
+        <v>45265</v>
       </c>
       <c r="BC6" s="44">
         <f t="shared" si="1"/>
-        <v>45259</v>
+        <v>45266</v>
       </c>
       <c r="BD6" s="44">
         <f t="shared" si="1"/>
-        <v>45260</v>
+        <v>45267</v>
       </c>
       <c r="BE6" s="44">
         <f t="shared" si="1"/>
-        <v>45261</v>
+        <v>45268</v>
       </c>
       <c r="BF6" s="44">
         <f t="shared" si="1"/>
-        <v>45262</v>
+        <v>45269</v>
       </c>
       <c r="BG6" s="54">
         <f t="shared" si="1"/>
-        <v>45263</v>
+        <v>45270</v>
       </c>
       <c r="BH6" s="53">
         <f t="shared" si="1"/>
-        <v>45264</v>
+        <v>45271</v>
       </c>
       <c r="BI6" s="44">
         <f t="shared" si="1"/>
-        <v>45265</v>
+        <v>45272</v>
       </c>
       <c r="BJ6" s="44">
         <f t="shared" si="1"/>
-        <v>45266</v>
+        <v>45273</v>
       </c>
       <c r="BK6" s="44">
         <f t="shared" si="1"/>
-        <v>45267</v>
+        <v>45274</v>
       </c>
       <c r="BL6" s="44">
         <f t="shared" si="1"/>
-        <v>45268</v>
+        <v>45275</v>
       </c>
       <c r="BM6" s="44">
         <f t="shared" si="1"/>
-        <v>45269</v>
+        <v>45276</v>
       </c>
       <c r="BN6" s="54">
         <f t="shared" si="1"/>
-        <v>45270</v>
+        <v>45277</v>
       </c>
     </row>
     <row r="7" spans="1:66" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -6131,7 +6131,7 @@
         <v>1</v>
       </c>
       <c r="H25" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25" s="43">
         <f t="shared" si="4"/>
@@ -6219,7 +6219,7 @@
         <v>1</v>
       </c>
       <c r="H26" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26" s="43">
         <f t="shared" si="4"/>
@@ -6307,7 +6307,7 @@
         <v>2</v>
       </c>
       <c r="H27" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I27" s="43">
         <f>IF(OR(F27=0,E27=0)," - ",NETWORKDAYS(E27,F27))</f>
@@ -6395,7 +6395,7 @@
         <v>2</v>
       </c>
       <c r="H28" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I28" s="43">
         <f t="shared" si="4"/>
@@ -6483,7 +6483,7 @@
         <v>2</v>
       </c>
       <c r="H29" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I29" s="43">
         <f t="shared" ref="I29" si="14">IF(OR(F29=0,E29=0)," - ",NETWORKDAYS(E29,F29))</f>
@@ -6571,7 +6571,7 @@
         <v>1</v>
       </c>
       <c r="H30" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I30" s="43">
         <f t="shared" ref="I30:I36" si="16">IF(OR(F30=0,E30=0)," - ",NETWORKDAYS(E30,F30))</f>
@@ -8999,15 +8999,6 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -9018,6 +9009,15 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H8:H13 H23:H28 H15:H21 H37:H41 H48:H51">
@@ -9241,7 +9241,7 @@
   <pageSetup scale="63" fitToHeight="0" orientation="landscape" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <ignoredErrors>
-    <ignoredError sqref="H9 H12 G25:H25 H23 G26:H26" unlockedFormula="1"/>
+    <ignoredError sqref="H9 H12 G25 H23 G26" unlockedFormula="1"/>
     <ignoredError sqref="A23 A12" formula="1"/>
   </ignoredErrors>
   <drawing r:id="rId3"/>

</xml_diff>

<commit_message>
docs (gantt): update workload, ubah role
</commit_message>
<xml_diff>
--- a/docs/Gantt Chart.xlsx
+++ b/docs/Gantt Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\punch\Documents\GitHub\warawiriweb\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D46F16D-6A49-4070-885E-EDD70C7FC2DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AD76F61-5DD4-4041-AF92-7600A86C3BD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25080" yWindow="8805" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2875,6 +2875,13 @@
     <xf numFmtId="1" fontId="50" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="45" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2884,6 +2891,10 @@
     <xf numFmtId="0" fontId="48" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="45" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="167" fontId="45" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2892,17 +2903,6 @@
     </xf>
     <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="45" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="45" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3860,8 +3860,8 @@
   <dimension ref="A1:BN57"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O34" sqref="O34"/>
+      <pane ySplit="7" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Y30" sqref="Y30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3888,29 +3888,29 @@
       <c r="E1" s="29"/>
       <c r="F1" s="29"/>
       <c r="I1" s="78"/>
-      <c r="K1" s="117" t="s">
+      <c r="K1" s="111" t="s">
         <v>71</v>
       </c>
-      <c r="L1" s="117"/>
-      <c r="M1" s="117"/>
-      <c r="N1" s="117"/>
-      <c r="O1" s="117"/>
-      <c r="P1" s="117"/>
-      <c r="Q1" s="117"/>
-      <c r="R1" s="117"/>
-      <c r="S1" s="117"/>
-      <c r="T1" s="117"/>
-      <c r="U1" s="117"/>
-      <c r="V1" s="117"/>
-      <c r="W1" s="117"/>
-      <c r="X1" s="117"/>
-      <c r="Y1" s="117"/>
-      <c r="Z1" s="117"/>
-      <c r="AA1" s="117"/>
-      <c r="AB1" s="117"/>
-      <c r="AC1" s="117"/>
-      <c r="AD1" s="117"/>
-      <c r="AE1" s="117"/>
+      <c r="L1" s="111"/>
+      <c r="M1" s="111"/>
+      <c r="N1" s="111"/>
+      <c r="O1" s="111"/>
+      <c r="P1" s="111"/>
+      <c r="Q1" s="111"/>
+      <c r="R1" s="111"/>
+      <c r="S1" s="111"/>
+      <c r="T1" s="111"/>
+      <c r="U1" s="111"/>
+      <c r="V1" s="111"/>
+      <c r="W1" s="111"/>
+      <c r="X1" s="111"/>
+      <c r="Y1" s="111"/>
+      <c r="Z1" s="111"/>
+      <c r="AA1" s="111"/>
+      <c r="AB1" s="111"/>
+      <c r="AC1" s="111"/>
+      <c r="AD1" s="111"/>
+      <c r="AE1" s="111"/>
     </row>
     <row r="2" spans="1:66" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
@@ -3950,11 +3950,11 @@
       <c r="B4" s="65" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="119">
+      <c r="C4" s="116">
         <v>45194</v>
       </c>
-      <c r="D4" s="119"/>
-      <c r="E4" s="119"/>
+      <c r="D4" s="116"/>
+      <c r="E4" s="116"/>
       <c r="F4" s="64"/>
       <c r="G4" s="65" t="s">
         <v>68</v>
@@ -3964,182 +3964,182 @@
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="30"/>
-      <c r="K4" s="111" t="str">
+      <c r="K4" s="113" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="L4" s="112"/>
-      <c r="M4" s="112"/>
-      <c r="N4" s="112"/>
-      <c r="O4" s="112"/>
-      <c r="P4" s="112"/>
-      <c r="Q4" s="113"/>
-      <c r="R4" s="111" t="str">
+      <c r="L4" s="114"/>
+      <c r="M4" s="114"/>
+      <c r="N4" s="114"/>
+      <c r="O4" s="114"/>
+      <c r="P4" s="114"/>
+      <c r="Q4" s="115"/>
+      <c r="R4" s="113" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="S4" s="112"/>
-      <c r="T4" s="112"/>
-      <c r="U4" s="112"/>
-      <c r="V4" s="112"/>
-      <c r="W4" s="112"/>
-      <c r="X4" s="113"/>
-      <c r="Y4" s="111" t="str">
+      <c r="S4" s="114"/>
+      <c r="T4" s="114"/>
+      <c r="U4" s="114"/>
+      <c r="V4" s="114"/>
+      <c r="W4" s="114"/>
+      <c r="X4" s="115"/>
+      <c r="Y4" s="113" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="Z4" s="112"/>
-      <c r="AA4" s="112"/>
-      <c r="AB4" s="112"/>
-      <c r="AC4" s="112"/>
-      <c r="AD4" s="112"/>
-      <c r="AE4" s="113"/>
-      <c r="AF4" s="111" t="str">
+      <c r="Z4" s="114"/>
+      <c r="AA4" s="114"/>
+      <c r="AB4" s="114"/>
+      <c r="AC4" s="114"/>
+      <c r="AD4" s="114"/>
+      <c r="AE4" s="115"/>
+      <c r="AF4" s="113" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="AG4" s="112"/>
-      <c r="AH4" s="112"/>
-      <c r="AI4" s="112"/>
-      <c r="AJ4" s="112"/>
-      <c r="AK4" s="112"/>
-      <c r="AL4" s="113"/>
-      <c r="AM4" s="111" t="str">
+      <c r="AG4" s="114"/>
+      <c r="AH4" s="114"/>
+      <c r="AI4" s="114"/>
+      <c r="AJ4" s="114"/>
+      <c r="AK4" s="114"/>
+      <c r="AL4" s="115"/>
+      <c r="AM4" s="113" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 9</v>
       </c>
-      <c r="AN4" s="112"/>
-      <c r="AO4" s="112"/>
-      <c r="AP4" s="112"/>
-      <c r="AQ4" s="112"/>
-      <c r="AR4" s="112"/>
-      <c r="AS4" s="113"/>
-      <c r="AT4" s="111" t="str">
+      <c r="AN4" s="114"/>
+      <c r="AO4" s="114"/>
+      <c r="AP4" s="114"/>
+      <c r="AQ4" s="114"/>
+      <c r="AR4" s="114"/>
+      <c r="AS4" s="115"/>
+      <c r="AT4" s="113" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 10</v>
       </c>
-      <c r="AU4" s="112"/>
-      <c r="AV4" s="112"/>
-      <c r="AW4" s="112"/>
-      <c r="AX4" s="112"/>
-      <c r="AY4" s="112"/>
-      <c r="AZ4" s="113"/>
-      <c r="BA4" s="111" t="str">
+      <c r="AU4" s="114"/>
+      <c r="AV4" s="114"/>
+      <c r="AW4" s="114"/>
+      <c r="AX4" s="114"/>
+      <c r="AY4" s="114"/>
+      <c r="AZ4" s="115"/>
+      <c r="BA4" s="113" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 11</v>
       </c>
-      <c r="BB4" s="112"/>
-      <c r="BC4" s="112"/>
-      <c r="BD4" s="112"/>
-      <c r="BE4" s="112"/>
-      <c r="BF4" s="112"/>
-      <c r="BG4" s="113"/>
-      <c r="BH4" s="111" t="str">
+      <c r="BB4" s="114"/>
+      <c r="BC4" s="114"/>
+      <c r="BD4" s="114"/>
+      <c r="BE4" s="114"/>
+      <c r="BF4" s="114"/>
+      <c r="BG4" s="115"/>
+      <c r="BH4" s="113" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 12</v>
       </c>
-      <c r="BI4" s="112"/>
-      <c r="BJ4" s="112"/>
-      <c r="BK4" s="112"/>
-      <c r="BL4" s="112"/>
-      <c r="BM4" s="112"/>
-      <c r="BN4" s="113"/>
+      <c r="BI4" s="114"/>
+      <c r="BJ4" s="114"/>
+      <c r="BK4" s="114"/>
+      <c r="BL4" s="114"/>
+      <c r="BM4" s="114"/>
+      <c r="BN4" s="115"/>
     </row>
     <row r="5" spans="1:66" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="64"/>
       <c r="B5" s="65" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="118" t="s">
+      <c r="C5" s="112" t="s">
         <v>132</v>
       </c>
-      <c r="D5" s="118"/>
-      <c r="E5" s="118"/>
+      <c r="D5" s="112"/>
+      <c r="E5" s="112"/>
       <c r="F5" s="64"/>
       <c r="G5" s="64"/>
       <c r="H5" s="64"/>
       <c r="I5" s="64"/>
       <c r="J5" s="30"/>
-      <c r="K5" s="114">
+      <c r="K5" s="117">
         <f>K6</f>
         <v>45222</v>
       </c>
-      <c r="L5" s="115"/>
-      <c r="M5" s="115"/>
-      <c r="N5" s="115"/>
-      <c r="O5" s="115"/>
-      <c r="P5" s="115"/>
-      <c r="Q5" s="116"/>
-      <c r="R5" s="114">
+      <c r="L5" s="118"/>
+      <c r="M5" s="118"/>
+      <c r="N5" s="118"/>
+      <c r="O5" s="118"/>
+      <c r="P5" s="118"/>
+      <c r="Q5" s="119"/>
+      <c r="R5" s="117">
         <f>R6</f>
         <v>45229</v>
       </c>
-      <c r="S5" s="115"/>
-      <c r="T5" s="115"/>
-      <c r="U5" s="115"/>
-      <c r="V5" s="115"/>
-      <c r="W5" s="115"/>
-      <c r="X5" s="116"/>
-      <c r="Y5" s="114">
+      <c r="S5" s="118"/>
+      <c r="T5" s="118"/>
+      <c r="U5" s="118"/>
+      <c r="V5" s="118"/>
+      <c r="W5" s="118"/>
+      <c r="X5" s="119"/>
+      <c r="Y5" s="117">
         <f>Y6</f>
         <v>45236</v>
       </c>
-      <c r="Z5" s="115"/>
-      <c r="AA5" s="115"/>
-      <c r="AB5" s="115"/>
-      <c r="AC5" s="115"/>
-      <c r="AD5" s="115"/>
-      <c r="AE5" s="116"/>
-      <c r="AF5" s="114">
+      <c r="Z5" s="118"/>
+      <c r="AA5" s="118"/>
+      <c r="AB5" s="118"/>
+      <c r="AC5" s="118"/>
+      <c r="AD5" s="118"/>
+      <c r="AE5" s="119"/>
+      <c r="AF5" s="117">
         <f>AF6</f>
         <v>45243</v>
       </c>
-      <c r="AG5" s="115"/>
-      <c r="AH5" s="115"/>
-      <c r="AI5" s="115"/>
-      <c r="AJ5" s="115"/>
-      <c r="AK5" s="115"/>
-      <c r="AL5" s="116"/>
-      <c r="AM5" s="114">
+      <c r="AG5" s="118"/>
+      <c r="AH5" s="118"/>
+      <c r="AI5" s="118"/>
+      <c r="AJ5" s="118"/>
+      <c r="AK5" s="118"/>
+      <c r="AL5" s="119"/>
+      <c r="AM5" s="117">
         <f>AM6</f>
         <v>45250</v>
       </c>
-      <c r="AN5" s="115"/>
-      <c r="AO5" s="115"/>
-      <c r="AP5" s="115"/>
-      <c r="AQ5" s="115"/>
-      <c r="AR5" s="115"/>
-      <c r="AS5" s="116"/>
-      <c r="AT5" s="114">
+      <c r="AN5" s="118"/>
+      <c r="AO5" s="118"/>
+      <c r="AP5" s="118"/>
+      <c r="AQ5" s="118"/>
+      <c r="AR5" s="118"/>
+      <c r="AS5" s="119"/>
+      <c r="AT5" s="117">
         <f>AT6</f>
         <v>45257</v>
       </c>
-      <c r="AU5" s="115"/>
-      <c r="AV5" s="115"/>
-      <c r="AW5" s="115"/>
-      <c r="AX5" s="115"/>
-      <c r="AY5" s="115"/>
-      <c r="AZ5" s="116"/>
-      <c r="BA5" s="114">
+      <c r="AU5" s="118"/>
+      <c r="AV5" s="118"/>
+      <c r="AW5" s="118"/>
+      <c r="AX5" s="118"/>
+      <c r="AY5" s="118"/>
+      <c r="AZ5" s="119"/>
+      <c r="BA5" s="117">
         <f>BA6</f>
         <v>45264</v>
       </c>
-      <c r="BB5" s="115"/>
-      <c r="BC5" s="115"/>
-      <c r="BD5" s="115"/>
-      <c r="BE5" s="115"/>
-      <c r="BF5" s="115"/>
-      <c r="BG5" s="116"/>
-      <c r="BH5" s="114">
+      <c r="BB5" s="118"/>
+      <c r="BC5" s="118"/>
+      <c r="BD5" s="118"/>
+      <c r="BE5" s="118"/>
+      <c r="BF5" s="118"/>
+      <c r="BG5" s="119"/>
+      <c r="BH5" s="117">
         <f>BH6</f>
         <v>45271</v>
       </c>
-      <c r="BI5" s="115"/>
-      <c r="BJ5" s="115"/>
-      <c r="BK5" s="115"/>
-      <c r="BL5" s="115"/>
-      <c r="BM5" s="115"/>
-      <c r="BN5" s="116"/>
+      <c r="BI5" s="118"/>
+      <c r="BJ5" s="118"/>
+      <c r="BK5" s="118"/>
+      <c r="BL5" s="118"/>
+      <c r="BM5" s="118"/>
+      <c r="BN5" s="119"/>
     </row>
     <row r="6" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A6" s="30"/>
@@ -6918,7 +6918,7 @@
         <v>2</v>
       </c>
       <c r="H34" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I34" s="43">
         <f t="shared" si="16"/>
@@ -7006,7 +7006,7 @@
         <v>2</v>
       </c>
       <c r="H35" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I35" s="43">
         <f t="shared" si="16"/>
@@ -7079,7 +7079,7 @@
         <v>165</v>
       </c>
       <c r="C36" s="40" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="D36" s="76"/>
       <c r="E36" s="58">
@@ -8999,15 +8999,6 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -9018,6 +9009,15 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H8:H13 H23:H28 H15:H21 H37:H41 H48:H51">

</xml_diff>

<commit_message>
fix: gantt + faq
</commit_message>
<xml_diff>
--- a/docs/Gantt Chart.xlsx
+++ b/docs/Gantt Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FILE DDE\Kuliah\S7\PTI\warawiriweb\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4434BA06-EFE5-4D2D-9CA8-392901B0D076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263D426E-4908-4BDA-83BF-D22F0201AE29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2870,13 +2870,6 @@
     <xf numFmtId="1" fontId="50" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="45" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2886,10 +2879,6 @@
     <xf numFmtId="0" fontId="48" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="45" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="167" fontId="45" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2898,6 +2887,17 @@
     </xf>
     <xf numFmtId="167" fontId="45" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="45" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="45" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3907,8 +3907,8 @@
   <dimension ref="A1:BN59"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V53" sqref="V53"/>
+      <pane ySplit="7" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3935,29 +3935,29 @@
       <c r="E1" s="29"/>
       <c r="F1" s="29"/>
       <c r="I1" s="78"/>
-      <c r="K1" s="111" t="s">
+      <c r="K1" s="117" t="s">
         <v>71</v>
       </c>
-      <c r="L1" s="111"/>
-      <c r="M1" s="111"/>
-      <c r="N1" s="111"/>
-      <c r="O1" s="111"/>
-      <c r="P1" s="111"/>
-      <c r="Q1" s="111"/>
-      <c r="R1" s="111"/>
-      <c r="S1" s="111"/>
-      <c r="T1" s="111"/>
-      <c r="U1" s="111"/>
-      <c r="V1" s="111"/>
-      <c r="W1" s="111"/>
-      <c r="X1" s="111"/>
-      <c r="Y1" s="111"/>
-      <c r="Z1" s="111"/>
-      <c r="AA1" s="111"/>
-      <c r="AB1" s="111"/>
-      <c r="AC1" s="111"/>
-      <c r="AD1" s="111"/>
-      <c r="AE1" s="111"/>
+      <c r="L1" s="117"/>
+      <c r="M1" s="117"/>
+      <c r="N1" s="117"/>
+      <c r="O1" s="117"/>
+      <c r="P1" s="117"/>
+      <c r="Q1" s="117"/>
+      <c r="R1" s="117"/>
+      <c r="S1" s="117"/>
+      <c r="T1" s="117"/>
+      <c r="U1" s="117"/>
+      <c r="V1" s="117"/>
+      <c r="W1" s="117"/>
+      <c r="X1" s="117"/>
+      <c r="Y1" s="117"/>
+      <c r="Z1" s="117"/>
+      <c r="AA1" s="117"/>
+      <c r="AB1" s="117"/>
+      <c r="AC1" s="117"/>
+      <c r="AD1" s="117"/>
+      <c r="AE1" s="117"/>
     </row>
     <row r="2" spans="1:66" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
@@ -3997,11 +3997,11 @@
       <c r="B4" s="65" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="116">
+      <c r="C4" s="119">
         <v>45194</v>
       </c>
-      <c r="D4" s="116"/>
-      <c r="E4" s="116"/>
+      <c r="D4" s="119"/>
+      <c r="E4" s="119"/>
       <c r="F4" s="64"/>
       <c r="G4" s="65" t="s">
         <v>68</v>
@@ -4011,182 +4011,182 @@
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="30"/>
-      <c r="K4" s="113" t="str">
+      <c r="K4" s="111" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="L4" s="114"/>
-      <c r="M4" s="114"/>
-      <c r="N4" s="114"/>
-      <c r="O4" s="114"/>
-      <c r="P4" s="114"/>
-      <c r="Q4" s="115"/>
-      <c r="R4" s="113" t="str">
+      <c r="L4" s="112"/>
+      <c r="M4" s="112"/>
+      <c r="N4" s="112"/>
+      <c r="O4" s="112"/>
+      <c r="P4" s="112"/>
+      <c r="Q4" s="113"/>
+      <c r="R4" s="111" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="S4" s="114"/>
-      <c r="T4" s="114"/>
-      <c r="U4" s="114"/>
-      <c r="V4" s="114"/>
-      <c r="W4" s="114"/>
-      <c r="X4" s="115"/>
-      <c r="Y4" s="113" t="str">
+      <c r="S4" s="112"/>
+      <c r="T4" s="112"/>
+      <c r="U4" s="112"/>
+      <c r="V4" s="112"/>
+      <c r="W4" s="112"/>
+      <c r="X4" s="113"/>
+      <c r="Y4" s="111" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 9</v>
       </c>
-      <c r="Z4" s="114"/>
-      <c r="AA4" s="114"/>
-      <c r="AB4" s="114"/>
-      <c r="AC4" s="114"/>
-      <c r="AD4" s="114"/>
-      <c r="AE4" s="115"/>
-      <c r="AF4" s="113" t="str">
+      <c r="Z4" s="112"/>
+      <c r="AA4" s="112"/>
+      <c r="AB4" s="112"/>
+      <c r="AC4" s="112"/>
+      <c r="AD4" s="112"/>
+      <c r="AE4" s="113"/>
+      <c r="AF4" s="111" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 10</v>
       </c>
-      <c r="AG4" s="114"/>
-      <c r="AH4" s="114"/>
-      <c r="AI4" s="114"/>
-      <c r="AJ4" s="114"/>
-      <c r="AK4" s="114"/>
-      <c r="AL4" s="115"/>
-      <c r="AM4" s="113" t="str">
+      <c r="AG4" s="112"/>
+      <c r="AH4" s="112"/>
+      <c r="AI4" s="112"/>
+      <c r="AJ4" s="112"/>
+      <c r="AK4" s="112"/>
+      <c r="AL4" s="113"/>
+      <c r="AM4" s="111" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 11</v>
       </c>
-      <c r="AN4" s="114"/>
-      <c r="AO4" s="114"/>
-      <c r="AP4" s="114"/>
-      <c r="AQ4" s="114"/>
-      <c r="AR4" s="114"/>
-      <c r="AS4" s="115"/>
-      <c r="AT4" s="113" t="str">
+      <c r="AN4" s="112"/>
+      <c r="AO4" s="112"/>
+      <c r="AP4" s="112"/>
+      <c r="AQ4" s="112"/>
+      <c r="AR4" s="112"/>
+      <c r="AS4" s="113"/>
+      <c r="AT4" s="111" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 12</v>
       </c>
-      <c r="AU4" s="114"/>
-      <c r="AV4" s="114"/>
-      <c r="AW4" s="114"/>
-      <c r="AX4" s="114"/>
-      <c r="AY4" s="114"/>
-      <c r="AZ4" s="115"/>
-      <c r="BA4" s="113" t="str">
+      <c r="AU4" s="112"/>
+      <c r="AV4" s="112"/>
+      <c r="AW4" s="112"/>
+      <c r="AX4" s="112"/>
+      <c r="AY4" s="112"/>
+      <c r="AZ4" s="113"/>
+      <c r="BA4" s="111" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 13</v>
       </c>
-      <c r="BB4" s="114"/>
-      <c r="BC4" s="114"/>
-      <c r="BD4" s="114"/>
-      <c r="BE4" s="114"/>
-      <c r="BF4" s="114"/>
-      <c r="BG4" s="115"/>
-      <c r="BH4" s="113" t="str">
+      <c r="BB4" s="112"/>
+      <c r="BC4" s="112"/>
+      <c r="BD4" s="112"/>
+      <c r="BE4" s="112"/>
+      <c r="BF4" s="112"/>
+      <c r="BG4" s="113"/>
+      <c r="BH4" s="111" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 14</v>
       </c>
-      <c r="BI4" s="114"/>
-      <c r="BJ4" s="114"/>
-      <c r="BK4" s="114"/>
-      <c r="BL4" s="114"/>
-      <c r="BM4" s="114"/>
-      <c r="BN4" s="115"/>
+      <c r="BI4" s="112"/>
+      <c r="BJ4" s="112"/>
+      <c r="BK4" s="112"/>
+      <c r="BL4" s="112"/>
+      <c r="BM4" s="112"/>
+      <c r="BN4" s="113"/>
     </row>
     <row r="5" spans="1:66" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="64"/>
       <c r="B5" s="65" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="112" t="s">
+      <c r="C5" s="118" t="s">
         <v>132</v>
       </c>
-      <c r="D5" s="112"/>
-      <c r="E5" s="112"/>
+      <c r="D5" s="118"/>
+      <c r="E5" s="118"/>
       <c r="F5" s="64"/>
       <c r="G5" s="64"/>
       <c r="H5" s="64"/>
       <c r="I5" s="64"/>
       <c r="J5" s="30"/>
-      <c r="K5" s="117">
+      <c r="K5" s="114">
         <f>K6</f>
         <v>45236</v>
       </c>
-      <c r="L5" s="118"/>
-      <c r="M5" s="118"/>
-      <c r="N5" s="118"/>
-      <c r="O5" s="118"/>
-      <c r="P5" s="118"/>
-      <c r="Q5" s="119"/>
-      <c r="R5" s="117">
+      <c r="L5" s="115"/>
+      <c r="M5" s="115"/>
+      <c r="N5" s="115"/>
+      <c r="O5" s="115"/>
+      <c r="P5" s="115"/>
+      <c r="Q5" s="116"/>
+      <c r="R5" s="114">
         <f>R6</f>
         <v>45243</v>
       </c>
-      <c r="S5" s="118"/>
-      <c r="T5" s="118"/>
-      <c r="U5" s="118"/>
-      <c r="V5" s="118"/>
-      <c r="W5" s="118"/>
-      <c r="X5" s="119"/>
-      <c r="Y5" s="117">
+      <c r="S5" s="115"/>
+      <c r="T5" s="115"/>
+      <c r="U5" s="115"/>
+      <c r="V5" s="115"/>
+      <c r="W5" s="115"/>
+      <c r="X5" s="116"/>
+      <c r="Y5" s="114">
         <f>Y6</f>
         <v>45250</v>
       </c>
-      <c r="Z5" s="118"/>
-      <c r="AA5" s="118"/>
-      <c r="AB5" s="118"/>
-      <c r="AC5" s="118"/>
-      <c r="AD5" s="118"/>
-      <c r="AE5" s="119"/>
-      <c r="AF5" s="117">
+      <c r="Z5" s="115"/>
+      <c r="AA5" s="115"/>
+      <c r="AB5" s="115"/>
+      <c r="AC5" s="115"/>
+      <c r="AD5" s="115"/>
+      <c r="AE5" s="116"/>
+      <c r="AF5" s="114">
         <f>AF6</f>
         <v>45257</v>
       </c>
-      <c r="AG5" s="118"/>
-      <c r="AH5" s="118"/>
-      <c r="AI5" s="118"/>
-      <c r="AJ5" s="118"/>
-      <c r="AK5" s="118"/>
-      <c r="AL5" s="119"/>
-      <c r="AM5" s="117">
+      <c r="AG5" s="115"/>
+      <c r="AH5" s="115"/>
+      <c r="AI5" s="115"/>
+      <c r="AJ5" s="115"/>
+      <c r="AK5" s="115"/>
+      <c r="AL5" s="116"/>
+      <c r="AM5" s="114">
         <f>AM6</f>
         <v>45264</v>
       </c>
-      <c r="AN5" s="118"/>
-      <c r="AO5" s="118"/>
-      <c r="AP5" s="118"/>
-      <c r="AQ5" s="118"/>
-      <c r="AR5" s="118"/>
-      <c r="AS5" s="119"/>
-      <c r="AT5" s="117">
+      <c r="AN5" s="115"/>
+      <c r="AO5" s="115"/>
+      <c r="AP5" s="115"/>
+      <c r="AQ5" s="115"/>
+      <c r="AR5" s="115"/>
+      <c r="AS5" s="116"/>
+      <c r="AT5" s="114">
         <f>AT6</f>
         <v>45271</v>
       </c>
-      <c r="AU5" s="118"/>
-      <c r="AV5" s="118"/>
-      <c r="AW5" s="118"/>
-      <c r="AX5" s="118"/>
-      <c r="AY5" s="118"/>
-      <c r="AZ5" s="119"/>
-      <c r="BA5" s="117">
+      <c r="AU5" s="115"/>
+      <c r="AV5" s="115"/>
+      <c r="AW5" s="115"/>
+      <c r="AX5" s="115"/>
+      <c r="AY5" s="115"/>
+      <c r="AZ5" s="116"/>
+      <c r="BA5" s="114">
         <f>BA6</f>
         <v>45278</v>
       </c>
-      <c r="BB5" s="118"/>
-      <c r="BC5" s="118"/>
-      <c r="BD5" s="118"/>
-      <c r="BE5" s="118"/>
-      <c r="BF5" s="118"/>
-      <c r="BG5" s="119"/>
-      <c r="BH5" s="117">
+      <c r="BB5" s="115"/>
+      <c r="BC5" s="115"/>
+      <c r="BD5" s="115"/>
+      <c r="BE5" s="115"/>
+      <c r="BF5" s="115"/>
+      <c r="BG5" s="116"/>
+      <c r="BH5" s="114">
         <f>BH6</f>
         <v>45285</v>
       </c>
-      <c r="BI5" s="118"/>
-      <c r="BJ5" s="118"/>
-      <c r="BK5" s="118"/>
-      <c r="BL5" s="118"/>
-      <c r="BM5" s="118"/>
-      <c r="BN5" s="119"/>
+      <c r="BI5" s="115"/>
+      <c r="BJ5" s="115"/>
+      <c r="BK5" s="115"/>
+      <c r="BL5" s="115"/>
+      <c r="BM5" s="115"/>
+      <c r="BN5" s="116"/>
     </row>
     <row r="6" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A6" s="30"/>
@@ -7493,7 +7493,7 @@
         <v>2</v>
       </c>
       <c r="H40" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I40" s="43">
         <f>IF(OR(F40=0,E40=0)," - ",NETWORKDAYS(E40,F40))</f>
@@ -8280,7 +8280,7 @@
         <v>2</v>
       </c>
       <c r="H49" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I49" s="43">
         <f>IF(OR(F49=0,E49=0)," - ",NETWORKDAYS(E49,F49))</f>
@@ -8456,7 +8456,7 @@
         <v>2</v>
       </c>
       <c r="H51" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I51" s="43">
         <f t="shared" ref="I51" si="28">IF(OR(F51=0,E51=0)," - ",NETWORKDAYS(E51,F51))</f>
@@ -9222,6 +9222,15 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -9232,15 +9241,6 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H8:H13 H23:H28 H15:H21 H37:H41 H50:H53">

</xml_diff>